<commit_message>
changed allfields datasets a bit
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -431,55 +431,55 @@
     <t>there</t>
   </si>
   <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>ds1</t>
+  </si>
+  <si>
+    <t>ds2</t>
+  </si>
+  <si>
+    <t>replaces</t>
+  </si>
+  <si>
+    <t>isRequiredBy</t>
+  </si>
+  <si>
+    <t>dummy</t>
+  </si>
+  <si>
+    <t>blabla</t>
+  </si>
+  <si>
+    <t>barbapappa</t>
+  </si>
+  <si>
+    <t>http://x</t>
+  </si>
+  <si>
+    <t>http://y</t>
+  </si>
+  <si>
+    <t>random test data</t>
+  </si>
+  <si>
+    <t>http://scholar.google.com</t>
+  </si>
+  <si>
+    <t>videos/some.txt</t>
+  </si>
+  <si>
+    <t>whatever</t>
+  </si>
+  <si>
+    <t>info:eu-repo/dai/nl/123456789X</t>
+  </si>
+  <si>
+    <t>info:eu-repo/dai/nl/012345678</t>
+  </si>
+  <si>
     <t>degrees</t>
-  </si>
-  <si>
-    <t>RD</t>
-  </si>
-  <si>
-    <t>ds1</t>
-  </si>
-  <si>
-    <t>ds2</t>
-  </si>
-  <si>
-    <t>replaces</t>
-  </si>
-  <si>
-    <t>isRequiredBy</t>
-  </si>
-  <si>
-    <t>dummy</t>
-  </si>
-  <si>
-    <t>blabla</t>
-  </si>
-  <si>
-    <t>barbapappa</t>
-  </si>
-  <si>
-    <t>http://x</t>
-  </si>
-  <si>
-    <t>http://y</t>
-  </si>
-  <si>
-    <t>random test data</t>
-  </si>
-  <si>
-    <t>http://scholar.google.com</t>
-  </si>
-  <si>
-    <t>videos/some.txt</t>
-  </si>
-  <si>
-    <t>whatever</t>
-  </si>
-  <si>
-    <t>info:eu-repo/dai/nl/123456789X</t>
-  </si>
-  <si>
-    <t>info:eu-repo/dai/nl/012345678</t>
   </si>
 </sst>
 </file>
@@ -823,14 +823,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:BA9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AJ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BB2" sqref="BB2"/>
+      <selection pane="bottomRight" activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1082,7 +1081,7 @@
         <v>118</v>
       </c>
       <c r="N2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O2" t="s">
         <v>121</v>
@@ -1112,7 +1111,7 @@
         <v>131</v>
       </c>
       <c r="Y2" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="Z2">
         <v>83575.399999999994</v>
@@ -1121,19 +1120,19 @@
         <v>455271.2</v>
       </c>
       <c r="AF2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AG2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AH2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AI2" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AJ2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AK2" t="s">
         <v>69</v>
@@ -1142,7 +1141,7 @@
         <v>72</v>
       </c>
       <c r="AM2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AN2" t="s">
         <v>61</v>
@@ -1178,7 +1177,7 @@
         <v>96</v>
       </c>
       <c r="AZ2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BA2" t="s">
         <v>97</v>
@@ -1220,7 +1219,7 @@
         <v>132</v>
       </c>
       <c r="Y3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AB3">
         <v>1</v>
@@ -1235,10 +1234,10 @@
         <v>4</v>
       </c>
       <c r="AG3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AH3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK3" t="s">
         <v>70</v>
@@ -1263,10 +1262,10 @@
         <v>68</v>
       </c>
       <c r="AI4" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:53" ht="96" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1299,10 +1298,10 @@
         <v>77</v>
       </c>
       <c r="AF5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AH5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AK5" t="s">
         <v>69</v>
@@ -1311,7 +1310,7 @@
         <v>72</v>
       </c>
       <c r="AM5" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AN5" t="s">
         <v>61</v>
@@ -1350,7 +1349,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:53" ht="96" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1367,7 +1366,7 @@
         <v>114</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I6" t="s">
         <v>115</v>
@@ -1398,7 +1397,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:53" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1425,7 +1424,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:53" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1440,7 +1439,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:53" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1458,13 +1457,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BA9">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="ruimtereis01"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <hyperlinks>
     <hyperlink ref="AI2" r:id="rId1"/>
     <hyperlink ref="AI4" r:id="rId2"/>

</xml_diff>

<commit_message>
bugfix and expected output updated
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="149">
   <si>
     <t>DATASET</t>
   </si>
@@ -456,9 +456,6 @@
   </si>
   <si>
     <t>http://x</t>
-  </si>
-  <si>
-    <t>http://y</t>
   </si>
   <si>
     <t>random test data</t>
@@ -826,10 +823,10 @@
   <dimension ref="A1:BA9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB4" sqref="AB4"/>
+      <selection pane="bottomRight" activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1081,7 +1078,7 @@
         <v>118</v>
       </c>
       <c r="N2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O2" t="s">
         <v>121</v>
@@ -1111,7 +1108,7 @@
         <v>131</v>
       </c>
       <c r="Y2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Z2">
         <v>83575.399999999994</v>
@@ -1128,11 +1125,9 @@
       <c r="AH2" t="s">
         <v>138</v>
       </c>
-      <c r="AI2" s="7" t="s">
-        <v>141</v>
-      </c>
+      <c r="AI2" s="7"/>
       <c r="AJ2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AK2" t="s">
         <v>69</v>
@@ -1141,7 +1136,7 @@
         <v>72</v>
       </c>
       <c r="AM2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AN2" t="s">
         <v>61</v>
@@ -1177,7 +1172,7 @@
         <v>96</v>
       </c>
       <c r="AZ2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="BA2" t="s">
         <v>97</v>
@@ -1262,7 +1257,7 @@
         <v>68</v>
       </c>
       <c r="AI4" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:53" ht="96" x14ac:dyDescent="0.2">
@@ -1310,7 +1305,7 @@
         <v>72</v>
       </c>
       <c r="AM5" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AN5" t="s">
         <v>61</v>
@@ -1366,7 +1361,7 @@
         <v>114</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I6" t="s">
         <v>115</v>
@@ -1458,9 +1453,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AI2" r:id="rId1"/>
-    <hyperlink ref="AI4" r:id="rId2"/>
-    <hyperlink ref="AM5" r:id="rId3"/>
+    <hyperlink ref="AI4" r:id="rId1"/>
+    <hyperlink ref="AM5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
small changes to instructions.csv
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -35,28 +35,6 @@
     <author>Richard van Heest</author>
   </authors>
   <commentList>
-    <comment ref="AV3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Richard van Heest:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-defaults to AV_FILE's filename</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="AW3" authorId="0">
       <text>
         <r>
@@ -107,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="141">
   <si>
     <t>DATASET</t>
   </si>
@@ -521,9 +499,6 @@
   </si>
   <si>
     <t>video about the centaur meteorite</t>
-  </si>
-  <si>
-    <t>ruimtereis01/path/to/a/random/video/hubble.mpg</t>
   </si>
   <si>
     <t>application/vnd.openxmlformats-officedocument.wordprocessingml.document</t>
@@ -617,7 +592,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -634,6 +609,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -917,10 +893,10 @@
   <dimension ref="A1:AX10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AM2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO10" sqref="AO10"/>
+      <selection pane="bottomRight" activeCell="AU3" sqref="AU3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1316,8 +1292,11 @@
       <c r="AL3" t="s">
         <v>73</v>
       </c>
-      <c r="AU3" t="s">
-        <v>138</v>
+      <c r="AU3" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="AV3" s="12" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1368,7 +1347,7 @@
       </c>
       <c r="AJ4" s="6"/>
       <c r="AK4" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AL4" s="6"/>
       <c r="AM4" s="6"/>
@@ -1379,12 +1358,8 @@
       <c r="AR4" s="6"/>
       <c r="AS4" s="6"/>
       <c r="AT4" s="6"/>
-      <c r="AU4" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AV4" s="6" t="s">
-        <v>141</v>
-      </c>
+      <c r="AU4" s="6"/>
+      <c r="AV4" s="6"/>
       <c r="AW4" s="6"/>
       <c r="AX4" s="6"/>
     </row>

</xml_diff>

<commit_message>
add multiple subtitles for video to the example
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -29,63 +29,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Richard van Heest</author>
-  </authors>
-  <commentList>
-    <comment ref="AW3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Richard van Heest:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-optional</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AT5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Richard van Heest:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Only allowed once;
-defaults to DDM_ACCESSRIGHTS</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="145">
   <si>
     <t>DATASET</t>
   </si>
@@ -508,6 +453,18 @@
   </si>
   <si>
     <t>our daily wake up call</t>
+  </si>
+  <si>
+    <t>AV_SUBTITLES_LANGUAGE</t>
+  </si>
+  <si>
+    <t>ruimtereis01/reisverslag/centaur-nederlands.srt</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>nl</t>
   </si>
 </sst>
 </file>
@@ -541,20 +498,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="81"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
-      <color theme="11"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -589,27 +550,26 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -889,14 +849,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AY10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="AM2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AU3" sqref="AU3"/>
+      <selection pane="bottomRight" activeCell="AX3" sqref="AX3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,633 +908,887 @@
     <col min="46" max="46" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="43.1640625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="40.33203125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AC1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AD1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="11" t="s">
+      <c r="AE1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AF1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AG1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AH1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AI1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="11" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="11" t="s">
+      <c r="AK1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AL1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="11" t="s">
+      <c r="AM1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="11" t="s">
+      <c r="AN1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AO1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="11" t="s">
+      <c r="AP1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AR1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AS1" s="6" t="s">
+      <c r="AS1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="AT1" s="6" t="s">
+      <c r="AT1" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AU1" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="AV1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AW1" s="6" t="s">
+      <c r="AW1" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AX1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AY1" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:50" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:51" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="M2" t="s">
+      <c r="L2" s="5"/>
+      <c r="M2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="6">
         <v>42143</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="V2" t="s">
+      <c r="U2" s="5"/>
+      <c r="V2" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="5">
         <v>83575.399999999994</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="5">
         <v>455271.2</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AG2" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AH2" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" t="s">
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AK2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AL2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AM2" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AN2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AO2" s="1">
+      <c r="AO2" s="6">
         <v>33815</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AP2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AQ2" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AR2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AS2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AT2" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AU2" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AV2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AW2" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AX2" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="AY2" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K3" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" t="s">
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="V3" t="s">
+      <c r="U3" s="5"/>
+      <c r="V3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="X3" t="s">
+      <c r="W3" s="5"/>
+      <c r="X3" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Y3" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="AB3">
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5">
         <v>1</v>
       </c>
-      <c r="AC3">
+      <c r="AC3" s="5">
         <v>2</v>
       </c>
-      <c r="AD3">
+      <c r="AD3" s="5">
         <v>3</v>
       </c>
-      <c r="AE3">
+      <c r="AE3" s="5">
         <v>4</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AH3" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AK3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AL3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="AU3" s="12" t="s">
+      <c r="AM3" s="5"/>
+      <c r="AN3" s="5"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="5"/>
+      <c r="AQ3" s="5"/>
+      <c r="AR3" s="5"/>
+      <c r="AS3" s="5"/>
+      <c r="AT3" s="5"/>
+      <c r="AU3" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AV3" s="5"/>
+      <c r="AW3" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="AX3" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="AY3" s="5"/>
+    </row>
+    <row r="4" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="R4" s="4"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="4"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="4"/>
+      <c r="AS4" s="4"/>
+      <c r="AT4" s="4"/>
+      <c r="AU4" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="AV3" s="12" t="s">
+      <c r="AV4" s="4" t="s">
         <v>140</v>
       </c>
+      <c r="AW4" s="4"/>
+      <c r="AX4" s="4"/>
+      <c r="AY4" s="4"/>
     </row>
-    <row r="4" spans="1:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="R4" s="6"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
-      <c r="AF4" s="6"/>
-      <c r="AG4" s="6"/>
-      <c r="AH4" s="6"/>
-      <c r="AI4" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="AJ4" s="6"/>
-      <c r="AK4" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="AL4" s="6"/>
-      <c r="AM4" s="6"/>
-      <c r="AN4" s="6"/>
-      <c r="AO4" s="6"/>
-      <c r="AP4" s="6"/>
-      <c r="AQ4" s="6"/>
-      <c r="AR4" s="6"/>
-      <c r="AS4" s="6"/>
-      <c r="AT4" s="6"/>
-      <c r="AU4" s="6"/>
-      <c r="AV4" s="6"/>
-      <c r="AW4" s="6"/>
-      <c r="AX4" s="6"/>
+    <row r="5" spans="1:51" ht="96" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="R5" s="5"/>
+      <c r="S5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AN5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="5"/>
+      <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="5"/>
+      <c r="AY5" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="5" spans="1:50" ht="96" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:51" ht="96" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" t="s">
-        <v>99</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="T5" t="s">
-        <v>64</v>
-      </c>
-      <c r="V5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>114</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AM5" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP5" t="s">
+      <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="R6" s="5"/>
+      <c r="S6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="5"/>
+      <c r="AQ6" s="5"/>
+      <c r="AR6" s="5"/>
+      <c r="AS6" s="5"/>
+      <c r="AT6" s="5"/>
+      <c r="AU6" s="5"/>
+      <c r="AV6" s="5"/>
+      <c r="AW6" s="5"/>
+      <c r="AX6" s="5"/>
+      <c r="AY6" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="5"/>
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="5"/>
+      <c r="AQ7" s="5"/>
+      <c r="AR7" s="5"/>
+      <c r="AS7" s="5"/>
+      <c r="AT7" s="5"/>
+      <c r="AU7" s="5"/>
+      <c r="AV7" s="5"/>
+      <c r="AW7" s="5"/>
+      <c r="AX7" s="5"/>
+      <c r="AY7" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="5"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="5"/>
+      <c r="AI8" s="5"/>
+      <c r="AJ8" s="5"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="5"/>
+      <c r="AM8" s="5"/>
+      <c r="AN8" s="5"/>
+      <c r="AO8" s="5"/>
+      <c r="AP8" s="5"/>
+      <c r="AQ8" s="5"/>
+      <c r="AR8" s="5"/>
+      <c r="AS8" s="5"/>
+      <c r="AT8" s="5"/>
+      <c r="AU8" s="5"/>
+      <c r="AV8" s="5"/>
+      <c r="AW8" s="5"/>
+      <c r="AX8" s="5"/>
+      <c r="AY8" s="5"/>
+    </row>
+    <row r="9" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="9">
+        <v>42137</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="4"/>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="4"/>
+      <c r="AN9" s="4"/>
+      <c r="AO9" s="4"/>
+      <c r="AP9" s="4"/>
+      <c r="AQ9" s="4"/>
+      <c r="AR9" s="4"/>
+      <c r="AS9" s="4"/>
+      <c r="AT9" s="4"/>
+      <c r="AU9" s="4"/>
+      <c r="AV9" s="4"/>
+      <c r="AW9" s="4"/>
+      <c r="AX9" s="4"/>
+      <c r="AY9" s="4"/>
+    </row>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="6">
+        <v>42581</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="5"/>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="5"/>
+      <c r="AM10" s="5"/>
+      <c r="AN10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AX5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:50" ht="96" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="I6" t="s">
-        <v>89</v>
-      </c>
-      <c r="P6" s="1"/>
-      <c r="Q6" t="s">
-        <v>100</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="T6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>74</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="P7" s="1"/>
-      <c r="Q7" t="s">
-        <v>101</v>
-      </c>
-      <c r="AX7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="P8" s="1"/>
-      <c r="Q8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="7">
-        <v>42137</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="6"/>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="6"/>
-      <c r="AE9" s="6"/>
-      <c r="AF9" s="6"/>
-      <c r="AG9" s="6"/>
-      <c r="AH9" s="6"/>
-      <c r="AI9" s="6"/>
-      <c r="AJ9" s="6"/>
-      <c r="AK9" s="6"/>
-      <c r="AL9" s="6"/>
-      <c r="AM9" s="6"/>
-      <c r="AN9" s="6"/>
-      <c r="AO9" s="6"/>
-      <c r="AP9" s="6"/>
-      <c r="AQ9" s="6"/>
-      <c r="AR9" s="6"/>
-      <c r="AS9" s="6"/>
-      <c r="AT9" s="6"/>
-      <c r="AU9" s="6"/>
-      <c r="AV9" s="6"/>
-      <c r="AW9" s="6"/>
-      <c r="AX9" s="6"/>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E10" t="s">
-        <v>132</v>
-      </c>
-      <c r="G10" t="s">
-        <v>133</v>
-      </c>
-      <c r="I10" t="s">
-        <v>134</v>
-      </c>
-      <c r="P10" s="1">
-        <v>42581</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>129</v>
-      </c>
-      <c r="S10" t="s">
-        <v>130</v>
-      </c>
-      <c r="T10" t="s">
-        <v>131</v>
-      </c>
-      <c r="AN10" t="s">
-        <v>123</v>
-      </c>
-      <c r="AP10" t="s">
-        <v>60</v>
-      </c>
+      <c r="AQ10" s="5"/>
+      <c r="AR10" s="5"/>
+      <c r="AS10" s="5"/>
+      <c r="AT10" s="5"/>
+      <c r="AU10" s="5"/>
+      <c r="AV10" s="5"/>
+      <c r="AW10" s="5"/>
+      <c r="AX10" s="5"/>
+      <c r="AY10" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1583,6 +1797,5 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
another change to the instructions.csv
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="146">
   <si>
     <t>DATASET</t>
   </si>
@@ -465,6 +465,9 @@
   </si>
   <si>
     <t>nl</t>
+  </si>
+  <si>
+    <t>RESTRICTED_GROUP</t>
   </si>
 </sst>
 </file>
@@ -547,9 +550,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -571,9 +575,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -856,7 +861,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="AM2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AX3" sqref="AX3"/>
+      <selection pane="bottomRight" activeCell="AT2" sqref="AT2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -905,7 +910,7 @@
     <col min="43" max="43" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="13.5" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="43.1640625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="40.33203125" bestFit="1" customWidth="1"/>
@@ -1186,7 +1191,7 @@
         <v>84</v>
       </c>
       <c r="AT2" s="5" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="AU2" s="5" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
change examples according to the rest of this PR
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -861,10 +861,10 @@
   <dimension ref="A1:AY10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AM2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AY10" sqref="AY10"/>
+      <selection pane="bottomRight" activeCell="AO11" sqref="AO11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1453,7 +1453,9 @@
       <c r="AN5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AO5" s="5"/>
+      <c r="AO5" s="6">
+        <v>42581</v>
+      </c>
       <c r="AP5" s="5" t="s">
         <v>60</v>
       </c>
@@ -1784,7 +1786,9 @@
       <c r="AN10" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="AO10" s="5"/>
+      <c r="AO10" s="6">
+        <v>42216</v>
+      </c>
       <c r="AP10" s="5" t="s">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
adjust examples according to previous commit
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -864,7 +864,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO11" sqref="AO11"/>
+      <selection pane="bottomRight" activeCell="AO5" sqref="AO5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1453,9 +1453,7 @@
       <c r="AN5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AO5" s="6">
-        <v>42581</v>
-      </c>
+      <c r="AO5" s="6"/>
       <c r="AP5" s="5" t="s">
         <v>60</v>
       </c>
@@ -1786,9 +1784,7 @@
       <c r="AN10" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="AO10" s="6">
-        <v>42216</v>
-      </c>
+      <c r="AO10" s="6"/>
       <c r="AP10" s="5" t="s">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
EASY-1238:  Move ddm:available from Metadata to Profile (#55)
* update ddm xsd version
* change examples according to the rest of this PR
* revert DDM_AVAILABLE as mandatory field
* DDM_AVAILABLE should be in profile, rather than metadata
* let DDM_AVAILABLE default to today's date
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -861,10 +861,10 @@
   <dimension ref="A1:AY10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AM2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AY10" sqref="AY10"/>
+      <selection pane="bottomRight" activeCell="AO5" sqref="AO5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1453,7 +1453,7 @@
       <c r="AN5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AO5" s="5"/>
+      <c r="AO5" s="6"/>
       <c r="AP5" s="5" t="s">
         <v>60</v>
       </c>
@@ -1784,7 +1784,7 @@
       <c r="AN10" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="AO10" s="5"/>
+      <c r="AO10" s="6"/>
       <c r="AP10" s="5" t="s">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
unique value checking and extracting for the values that require at most or exactly one value per dataset
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="147">
   <si>
     <t>DATASET</t>
   </si>
@@ -553,9 +553,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -578,10 +580,12 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -864,7 +868,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO5" sqref="AO5"/>
+      <selection pane="bottomRight" activeCell="AP5" sqref="AP5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1408,7 +1412,9 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="6"/>
+      <c r="P5" s="6">
+        <v>42137</v>
+      </c>
       <c r="Q5" s="5" t="s">
         <v>99</v>
       </c>
@@ -1499,7 +1505,9 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
-      <c r="P6" s="6"/>
+      <c r="P6" s="6">
+        <v>42137</v>
+      </c>
       <c r="Q6" s="5" t="s">
         <v>100</v>
       </c>
@@ -1533,7 +1541,9 @@
         <v>74</v>
       </c>
       <c r="AM6" s="5"/>
-      <c r="AN6" s="5"/>
+      <c r="AN6" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="AO6" s="5"/>
       <c r="AP6" s="5"/>
       <c r="AQ6" s="5"/>
@@ -1566,7 +1576,9 @@
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="6"/>
+      <c r="P7" s="6">
+        <v>42137</v>
+      </c>
       <c r="Q7" s="5" t="s">
         <v>101</v>
       </c>
@@ -1592,7 +1604,9 @@
       <c r="AK7" s="5"/>
       <c r="AL7" s="5"/>
       <c r="AM7" s="5"/>
-      <c r="AN7" s="5"/>
+      <c r="AN7" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="AO7" s="5"/>
       <c r="AP7" s="5"/>
       <c r="AQ7" s="5"/>
@@ -1625,7 +1639,9 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
+      <c r="P8" s="6">
+        <v>42137</v>
+      </c>
       <c r="Q8" s="5" t="s">
         <v>102</v>
       </c>
@@ -1651,7 +1667,9 @@
       <c r="AK8" s="5"/>
       <c r="AL8" s="5"/>
       <c r="AM8" s="5"/>
-      <c r="AN8" s="5"/>
+      <c r="AN8" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="AO8" s="5"/>
       <c r="AP8" s="5"/>
       <c r="AQ8" s="5"/>
@@ -1710,7 +1728,9 @@
       <c r="AK9" s="4"/>
       <c r="AL9" s="4"/>
       <c r="AM9" s="4"/>
-      <c r="AN9" s="4"/>
+      <c r="AN9" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="AO9" s="4"/>
       <c r="AP9" s="4"/>
       <c r="AQ9" s="4"/>

</xml_diff>

<commit_message>
add formats xsi:type to dataset.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -239,9 +239,6 @@
     <t>abr:ABRcomplex</t>
   </si>
   <si>
-    <t>video/mpeg</t>
-  </si>
-  <si>
     <t>text/plain</t>
   </si>
   <si>
@@ -471,6 +468,9 @@
   </si>
   <si>
     <t>D37000</t>
+  </si>
+  <si>
+    <t>video/mpeg1</t>
   </si>
 </sst>
 </file>
@@ -865,10 +865,10 @@
   <dimension ref="A1:AY10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AP5" sqref="AP5"/>
+      <selection pane="bottomRight" activeCell="AK5" sqref="AK5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1052,28 +1052,28 @@
         <v>41</v>
       </c>
       <c r="AQ1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AS1" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="AT1" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AU1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AW1" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="AV1" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW1" s="4" t="s">
-        <v>125</v>
-      </c>
       <c r="AX1" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AY1" s="4" t="s">
         <v>42</v>
@@ -1104,29 +1104,29 @@
         <v>62</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P2" s="6">
         <v>42143</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="S2" s="7" t="s">
         <v>56</v>
@@ -1136,16 +1136,16 @@
       </c>
       <c r="U2" s="5"/>
       <c r="V2" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z2" s="5">
         <v>83575.399999999994</v>
@@ -1158,26 +1158,26 @@
       <c r="AD2" s="5"/>
       <c r="AE2" s="5"/>
       <c r="AF2" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AI2" s="8"/>
       <c r="AJ2" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AN2" s="5" t="s">
         <v>61</v>
@@ -1189,31 +1189,31 @@
         <v>60</v>
       </c>
       <c r="AQ2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR2" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AR2" s="5" t="s">
+      <c r="AS2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="AS2" s="5" t="s">
+      <c r="AT2" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="AU2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="AV2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="AW2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AX2" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="AY2" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="AT2" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="AU2" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="AV2" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="AW2" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="AX2" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="AY2" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.2">
@@ -1232,22 +1232,22 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="S3" s="5" t="s">
         <v>57</v>
@@ -1257,14 +1257,14 @@
       </c>
       <c r="U3" s="5"/>
       <c r="V3" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W3" s="5"/>
       <c r="X3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y3" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
@@ -1282,18 +1282,18 @@
       </c>
       <c r="AF3" s="5"/>
       <c r="AG3" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="5"/>
       <c r="AK3" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AL3" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AM3" s="5"/>
       <c r="AN3" s="5"/>
@@ -1304,14 +1304,14 @@
       <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AV3" s="5"/>
       <c r="AW3" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AX3" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AY3" s="5"/>
     </row>
@@ -1335,7 +1335,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R4" s="4"/>
       <c r="S4" s="10"/>
@@ -1359,11 +1359,11 @@
       <c r="AG4" s="4"/>
       <c r="AH4" s="4"/>
       <c r="AI4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AJ4" s="4"/>
       <c r="AK4" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AL4" s="4"/>
       <c r="AM4" s="4"/>
@@ -1375,10 +1375,10 @@
       <c r="AS4" s="4"/>
       <c r="AT4" s="4"/>
       <c r="AU4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AV4" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="AV4" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="AW4" s="4"/>
       <c r="AX4" s="4"/>
@@ -1416,7 +1416,7 @@
         <v>42137</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R5" s="5"/>
       <c r="S5" s="7" t="s">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="U5" s="5"/>
       <c r="V5" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
@@ -1439,22 +1439,22 @@
       <c r="AD5" s="5"/>
       <c r="AE5" s="5"/>
       <c r="AF5" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AG5" s="5"/>
       <c r="AH5" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AI5" s="5"/>
       <c r="AJ5" s="5"/>
       <c r="AK5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AL5" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="AM5" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AN5" s="5" t="s">
         <v>61</v>
@@ -1472,7 +1472,7 @@
       <c r="AW5" s="5"/>
       <c r="AX5" s="5"/>
       <c r="AY5" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:51" ht="96" x14ac:dyDescent="0.2">
@@ -1485,19 +1485,19 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -1509,7 +1509,7 @@
         <v>42137</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R6" s="5"/>
       <c r="S6" s="7" t="s">
@@ -1535,10 +1535,10 @@
       <c r="AI6" s="5"/>
       <c r="AJ6" s="5"/>
       <c r="AK6" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AM6" s="5"/>
       <c r="AN6" s="5" t="s">
@@ -1555,7 +1555,7 @@
       <c r="AW6" s="5"/>
       <c r="AX6" s="5"/>
       <c r="AY6" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.2">
@@ -1580,7 +1580,7 @@
         <v>42137</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
@@ -1618,7 +1618,7 @@
       <c r="AW7" s="5"/>
       <c r="AX7" s="5"/>
       <c r="AY7" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.2">
@@ -1643,7 +1643,7 @@
         <v>42137</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
@@ -1704,7 +1704,7 @@
         <v>42137</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
@@ -1745,23 +1745,23 @@
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>128</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -1773,14 +1773,14 @@
         <v>42581</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R10" s="5"/>
       <c r="S10" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="T10" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>131</v>
       </c>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
@@ -1802,11 +1802,11 @@
       <c r="AL10" s="5"/>
       <c r="AM10" s="5"/>
       <c r="AN10" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AO10" s="6"/>
       <c r="AP10" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AQ10" s="5"/>
       <c r="AR10" s="5"/>
@@ -1817,7 +1817,7 @@
       <c r="AW10" s="5"/>
       <c r="AX10" s="5"/>
       <c r="AY10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add iso 639-2 check to DC_LANGUAGE
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -865,10 +865,10 @@
   <dimension ref="A1:AY10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AK5" sqref="AK5"/>
+      <selection pane="bottomRight" activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,7 +909,7 @@
     <col min="35" max="35" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="65.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="15.1640625" bestFit="1" customWidth="1"/>
@@ -921,7 +921,7 @@
     <col min="47" max="47" width="43.1640625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding xsi:type as attribute to dc:language; add extra check to lanugage validation; fix and expand tests
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="148">
   <si>
     <t>DATASET</t>
   </si>
@@ -245,15 +245,6 @@
     <t>image/jpeg</t>
   </si>
   <si>
-    <t>NL</t>
-  </si>
-  <si>
-    <t>encoding=UTF-8</t>
-  </si>
-  <si>
-    <t>EN</t>
-  </si>
-  <si>
     <t>PALEOLB</t>
   </si>
   <si>
@@ -471,6 +462,18 @@
   </si>
   <si>
     <t>video/mpeg1</t>
+  </si>
+  <si>
+    <t>nld</t>
+  </si>
+  <si>
+    <t>eng</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>dut</t>
   </si>
 </sst>
 </file>
@@ -868,7 +871,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL3" sqref="AL3"/>
+      <selection pane="bottomRight" activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1052,28 +1055,28 @@
         <v>41</v>
       </c>
       <c r="AQ1" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="AR1" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AS1" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="AT1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AU1" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="AW1" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="AU1" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="AV1" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AW1" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="AX1" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AY1" s="4" t="s">
         <v>42</v>
@@ -1104,29 +1107,29 @@
         <v>62</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="P2" s="6">
         <v>42143</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="S2" s="7" t="s">
         <v>56</v>
@@ -1136,16 +1139,16 @@
       </c>
       <c r="U2" s="5"/>
       <c r="V2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="W2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="W2" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="X2" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Z2" s="5">
         <v>83575.399999999994</v>
@@ -1158,26 +1161,26 @@
       <c r="AD2" s="5"/>
       <c r="AE2" s="5"/>
       <c r="AF2" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AI2" s="8"/>
       <c r="AJ2" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AN2" s="5" t="s">
         <v>61</v>
@@ -1189,31 +1192,31 @@
         <v>60</v>
       </c>
       <c r="AQ2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT2" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="AU2" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AV2" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="AW2" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="AX2" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="AY2" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="AR2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AS2" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="AT2" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="AU2" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="AV2" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="AW2" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="AX2" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="AY2" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.2">
@@ -1232,22 +1235,22 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="S3" s="5" t="s">
         <v>57</v>
@@ -1257,14 +1260,14 @@
       </c>
       <c r="U3" s="5"/>
       <c r="V3" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="W3" s="5"/>
       <c r="X3" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
@@ -1282,10 +1285,10 @@
       </c>
       <c r="AF3" s="5"/>
       <c r="AG3" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="5"/>
@@ -1293,7 +1296,7 @@
         <v>69</v>
       </c>
       <c r="AL3" s="5" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="AM3" s="5"/>
       <c r="AN3" s="5"/>
@@ -1304,14 +1307,14 @@
       <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="AV3" s="5"/>
       <c r="AW3" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AX3" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AY3" s="5"/>
     </row>
@@ -1335,7 +1338,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="R4" s="4"/>
       <c r="S4" s="10"/>
@@ -1359,11 +1362,11 @@
       <c r="AG4" s="4"/>
       <c r="AH4" s="4"/>
       <c r="AI4" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="AJ4" s="4"/>
       <c r="AK4" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="AL4" s="4"/>
       <c r="AM4" s="4"/>
@@ -1375,10 +1378,10 @@
       <c r="AS4" s="4"/>
       <c r="AT4" s="4"/>
       <c r="AU4" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="AV4" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AW4" s="4"/>
       <c r="AX4" s="4"/>
@@ -1416,7 +1419,7 @@
         <v>42137</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="R5" s="5"/>
       <c r="S5" s="7" t="s">
@@ -1427,7 +1430,7 @@
       </c>
       <c r="U5" s="5"/>
       <c r="V5" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
@@ -1439,11 +1442,11 @@
       <c r="AD5" s="5"/>
       <c r="AE5" s="5"/>
       <c r="AF5" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AG5" s="5"/>
       <c r="AH5" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AI5" s="5"/>
       <c r="AJ5" s="5"/>
@@ -1451,10 +1454,10 @@
         <v>70</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>71</v>
+        <v>146</v>
       </c>
       <c r="AM5" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AN5" s="5" t="s">
         <v>61</v>
@@ -1472,7 +1475,7 @@
       <c r="AW5" s="5"/>
       <c r="AX5" s="5"/>
       <c r="AY5" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:51" ht="96" x14ac:dyDescent="0.2">
@@ -1485,19 +1488,19 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -1509,7 +1512,7 @@
         <v>42137</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="R6" s="5"/>
       <c r="S6" s="7" t="s">
@@ -1538,7 +1541,7 @@
         <v>69</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>73</v>
+        <v>147</v>
       </c>
       <c r="AM6" s="5"/>
       <c r="AN6" s="5" t="s">
@@ -1555,7 +1558,7 @@
       <c r="AW6" s="5"/>
       <c r="AX6" s="5"/>
       <c r="AY6" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.2">
@@ -1580,7 +1583,7 @@
         <v>42137</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
@@ -1618,7 +1621,7 @@
       <c r="AW7" s="5"/>
       <c r="AX7" s="5"/>
       <c r="AY7" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.2">
@@ -1643,7 +1646,7 @@
         <v>42137</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
@@ -1704,7 +1707,7 @@
         <v>42137</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
@@ -1745,23 +1748,23 @@
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -1773,14 +1776,14 @@
         <v>42581</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="R10" s="5"/>
       <c r="S10" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="T10" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
@@ -1802,11 +1805,11 @@
       <c r="AL10" s="5"/>
       <c r="AM10" s="5"/>
       <c r="AN10" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="AO10" s="6"/>
       <c r="AP10" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AQ10" s="5"/>
       <c r="AR10" s="5"/>
@@ -1817,7 +1820,7 @@
       <c r="AW10" s="5"/>
       <c r="AX10" s="5"/>
       <c r="AY10" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add DC_TYPE values, parser and xml serializer with correct xsi:type attribute
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -368,9 +368,6 @@
     <t>http://x</t>
   </si>
   <si>
-    <t>random test data</t>
-  </si>
-  <si>
     <t>http://scholar.google.com</t>
   </si>
   <si>
@@ -474,6 +471,9 @@
   </si>
   <si>
     <t>dut</t>
+  </si>
+  <si>
+    <t>Text</t>
   </si>
 </sst>
 </file>
@@ -556,9 +556,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -583,12 +585,14 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -871,7 +875,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL6" sqref="AL6"/>
+      <selection pane="bottomRight" activeCell="AJ3" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1064,19 +1068,19 @@
         <v>77</v>
       </c>
       <c r="AT1" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AU1" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="AW1" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="AV1" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="AW1" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="AX1" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AY1" s="4" t="s">
         <v>42</v>
@@ -1117,7 +1121,7 @@
         <v>88</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>91</v>
@@ -1148,7 +1152,7 @@
         <v>101</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Z2" s="5">
         <v>83575.399999999994</v>
@@ -1171,16 +1175,16 @@
       </c>
       <c r="AI2" s="8"/>
       <c r="AJ2" s="5" t="s">
-        <v>112</v>
+        <v>147</v>
       </c>
       <c r="AK2" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL2" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="AL2" s="5" t="s">
-        <v>144</v>
-      </c>
       <c r="AM2" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AN2" s="5" t="s">
         <v>61</v>
@@ -1201,19 +1205,19 @@
         <v>80</v>
       </c>
       <c r="AT2" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AU2" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="AV2" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="AW2" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="AV2" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AW2" s="5" t="s">
-        <v>132</v>
-      </c>
       <c r="AX2" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AY2" s="5" t="s">
         <v>81</v>
@@ -1296,7 +1300,7 @@
         <v>69</v>
       </c>
       <c r="AL3" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM3" s="5"/>
       <c r="AN3" s="5"/>
@@ -1307,14 +1311,14 @@
       <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AV3" s="5"/>
       <c r="AW3" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AX3" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AY3" s="5"/>
     </row>
@@ -1366,7 +1370,7 @@
       </c>
       <c r="AJ4" s="4"/>
       <c r="AK4" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AL4" s="4"/>
       <c r="AM4" s="4"/>
@@ -1378,10 +1382,10 @@
       <c r="AS4" s="4"/>
       <c r="AT4" s="4"/>
       <c r="AU4" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="AV4" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="AV4" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="AW4" s="4"/>
       <c r="AX4" s="4"/>
@@ -1454,10 +1458,10 @@
         <v>70</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AM5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AN5" s="5" t="s">
         <v>61</v>
@@ -1497,7 +1501,7 @@
         <v>84</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>85</v>
@@ -1541,7 +1545,7 @@
         <v>69</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AM6" s="5"/>
       <c r="AN6" s="5" t="s">
@@ -1748,23 +1752,23 @@
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -1776,14 +1780,14 @@
         <v>42581</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R10" s="5"/>
       <c r="S10" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="T10" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
@@ -1805,11 +1809,11 @@
       <c r="AL10" s="5"/>
       <c r="AM10" s="5"/>
       <c r="AN10" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AO10" s="6"/>
       <c r="AP10" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AQ10" s="5"/>
       <c r="AR10" s="5"/>

</xml_diff>

<commit_message>
EASY-1257: DC_LANGUAGE / DC_FORMAT / DC_TYPE uitbreiden met xsi:type in DDM (#67)
* remove DDM object

* formats configuration and reading into Settings

* add formats property to BlackBoxSpec

* null handling for formats property

* add formats xsi:type to dataset.xml

* add iso 639-2 check to DC_LANGUAGE

* adding xsi:type as attribute to dc:language; add extra check to lanugage validation; fix and expand tests

* random thing: write BagCompleters with anonymous constructor extension

* space

* add DC_TYPE values, parser and xml serializer with correct xsi:type attribute

* add extra check to make sure AV_SUBTITLE_LANGUAGE is a ISO639-1 language tag

* change single quotes to double quotes

* Corrected debug-config logback file. (Production logback was already correct.)

* Ignore temp Excel files

* Removed formats.file setting
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="148">
   <si>
     <t>DATASET</t>
   </si>
@@ -239,24 +239,12 @@
     <t>abr:ABRcomplex</t>
   </si>
   <si>
-    <t>video/mpeg</t>
-  </si>
-  <si>
     <t>text/plain</t>
   </si>
   <si>
     <t>image/jpeg</t>
   </si>
   <si>
-    <t>NL</t>
-  </si>
-  <si>
-    <t>encoding=UTF-8</t>
-  </si>
-  <si>
-    <t>EN</t>
-  </si>
-  <si>
     <t>PALEOLB</t>
   </si>
   <si>
@@ -380,9 +368,6 @@
     <t>http://x</t>
   </si>
   <si>
-    <t>random test data</t>
-  </si>
-  <si>
     <t>http://scholar.google.com</t>
   </si>
   <si>
@@ -471,6 +456,24 @@
   </si>
   <si>
     <t>D37000</t>
+  </si>
+  <si>
+    <t>video/mpeg1</t>
+  </si>
+  <si>
+    <t>nld</t>
+  </si>
+  <si>
+    <t>eng</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>dut</t>
+  </si>
+  <si>
+    <t>Text</t>
   </si>
 </sst>
 </file>
@@ -553,9 +556,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -580,12 +585,14 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -865,10 +872,10 @@
   <dimension ref="A1:AY10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AP5" sqref="AP5"/>
+      <selection pane="bottomRight" activeCell="AJ3" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,7 +916,7 @@
     <col min="35" max="35" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="65.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="15.1640625" bestFit="1" customWidth="1"/>
@@ -921,7 +928,7 @@
     <col min="47" max="47" width="43.1640625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1052,28 +1059,28 @@
         <v>41</v>
       </c>
       <c r="AQ1" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="AR1" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AS1" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="AT1" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="AU1" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="AV1" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="AW1" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="AX1" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="AY1" s="4" t="s">
         <v>42</v>
@@ -1104,29 +1111,29 @@
         <v>62</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="P2" s="6">
         <v>42143</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="S2" s="7" t="s">
         <v>56</v>
@@ -1136,16 +1143,16 @@
       </c>
       <c r="U2" s="5"/>
       <c r="V2" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Z2" s="5">
         <v>83575.399999999994</v>
@@ -1158,26 +1165,26 @@
       <c r="AD2" s="5"/>
       <c r="AE2" s="5"/>
       <c r="AF2" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH2" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="AG2" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH2" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="AI2" s="8"/>
       <c r="AJ2" s="5" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="AN2" s="5" t="s">
         <v>61</v>
@@ -1189,31 +1196,31 @@
         <v>60</v>
       </c>
       <c r="AQ2" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="AR2" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="AS2" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="AT2" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="AU2" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="AV2" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="AW2" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AX2" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AY2" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.2">
@@ -1232,22 +1239,22 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="S3" s="5" t="s">
         <v>57</v>
@@ -1257,14 +1264,14 @@
       </c>
       <c r="U3" s="5"/>
       <c r="V3" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="W3" s="5"/>
       <c r="X3" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
@@ -1282,18 +1289,18 @@
       </c>
       <c r="AF3" s="5"/>
       <c r="AG3" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="5"/>
       <c r="AK3" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AL3" s="5" t="s">
-        <v>73</v>
+        <v>144</v>
       </c>
       <c r="AM3" s="5"/>
       <c r="AN3" s="5"/>
@@ -1304,14 +1311,14 @@
       <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="AV3" s="5"/>
       <c r="AW3" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="AX3" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="AY3" s="5"/>
     </row>
@@ -1335,7 +1342,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="R4" s="4"/>
       <c r="S4" s="10"/>
@@ -1359,11 +1366,11 @@
       <c r="AG4" s="4"/>
       <c r="AH4" s="4"/>
       <c r="AI4" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="AJ4" s="4"/>
       <c r="AK4" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="AL4" s="4"/>
       <c r="AM4" s="4"/>
@@ -1375,10 +1382,10 @@
       <c r="AS4" s="4"/>
       <c r="AT4" s="4"/>
       <c r="AU4" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="AV4" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="AW4" s="4"/>
       <c r="AX4" s="4"/>
@@ -1416,7 +1423,7 @@
         <v>42137</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="R5" s="5"/>
       <c r="S5" s="7" t="s">
@@ -1427,7 +1434,7 @@
       </c>
       <c r="U5" s="5"/>
       <c r="V5" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
@@ -1439,22 +1446,22 @@
       <c r="AD5" s="5"/>
       <c r="AE5" s="5"/>
       <c r="AF5" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="AG5" s="5"/>
       <c r="AH5" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="AI5" s="5"/>
       <c r="AJ5" s="5"/>
       <c r="AK5" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="AM5" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="AN5" s="5" t="s">
         <v>61</v>
@@ -1472,7 +1479,7 @@
       <c r="AW5" s="5"/>
       <c r="AX5" s="5"/>
       <c r="AY5" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:51" ht="96" x14ac:dyDescent="0.2">
@@ -1485,19 +1492,19 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -1509,7 +1516,7 @@
         <v>42137</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="R6" s="5"/>
       <c r="S6" s="7" t="s">
@@ -1535,10 +1542,10 @@
       <c r="AI6" s="5"/>
       <c r="AJ6" s="5"/>
       <c r="AK6" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="AM6" s="5"/>
       <c r="AN6" s="5" t="s">
@@ -1555,7 +1562,7 @@
       <c r="AW6" s="5"/>
       <c r="AX6" s="5"/>
       <c r="AY6" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.2">
@@ -1580,7 +1587,7 @@
         <v>42137</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
@@ -1618,7 +1625,7 @@
       <c r="AW7" s="5"/>
       <c r="AX7" s="5"/>
       <c r="AY7" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.2">
@@ -1643,7 +1650,7 @@
         <v>42137</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
@@ -1704,7 +1711,7 @@
         <v>42137</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
@@ -1745,23 +1752,23 @@
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -1773,14 +1780,14 @@
         <v>42581</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="R10" s="5"/>
       <c r="S10" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="T10" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
@@ -1802,11 +1809,11 @@
       <c r="AL10" s="5"/>
       <c r="AM10" s="5"/>
       <c r="AN10" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AO10" s="6"/>
       <c r="AP10" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="AQ10" s="5"/>
       <c r="AR10" s="5"/>
@@ -1817,7 +1824,7 @@
       <c r="AW10" s="5"/>
       <c r="AX10" s="5"/>
       <c r="AY10" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
proper names for identifier-types
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -485,7 +485,7 @@
     <t>0925-6229</t>
   </si>
   <si>
-    <t>ARCHIS_ZAAK_IDENTIFICATIE</t>
+    <t>ARCHIS-ZAAK-IDENTIFICATIE</t>
   </si>
 </sst>
 </file>
@@ -893,7 +893,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF6" sqref="AF6"/>
+      <selection pane="bottomRight" activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
EASY-1258: Add DC_IDENTIFIER_TYPE (#69)
* add DC_IDENTIFIER_TYPE as a column to the instructions.csv
* parse this new column into an enum type
* use this enum type in the DDM generation
* adjust/add tests accordingly
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AX$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AY$9</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="152">
   <si>
     <t>DATASET</t>
   </si>
@@ -474,6 +474,18 @@
   </si>
   <si>
     <t>Text</t>
+  </si>
+  <si>
+    <t>DC_IDENTIFIER_TYPE</t>
+  </si>
+  <si>
+    <t>ISSN</t>
+  </si>
+  <si>
+    <t>0925-6229</t>
+  </si>
+  <si>
+    <t>ARCHIS-ZAAK-IDENTIFICATIE</t>
   </si>
 </sst>
 </file>
@@ -556,9 +568,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -585,7 +600,7 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -593,6 +608,9 @@
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -869,13 +887,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY10"/>
+  <dimension ref="A1:AZ10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AJ3" sqref="AJ3"/>
+      <selection pane="bottomRight" activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -911,27 +929,28 @@
     <col min="30" max="30" width="17" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="65.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="23" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1029,64 +1048,67 @@
         <v>31</v>
       </c>
       <c r="AG1" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:51" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>43</v>
       </c>
@@ -1167,63 +1189,64 @@
       <c r="AF2" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AI2" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="5" t="s">
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="AK2" s="5" t="s">
+      <c r="AL2" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="AL2" s="5" t="s">
+      <c r="AM2" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="AM2" s="5" t="s">
+      <c r="AN2" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="AN2" s="5" t="s">
+      <c r="AO2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AO2" s="6">
+      <c r="AP2" s="6">
         <v>33815</v>
       </c>
-      <c r="AP2" s="5" t="s">
+      <c r="AQ2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AQ2" s="5" t="s">
+      <c r="AR2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AR2" s="5" t="s">
+      <c r="AS2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AS2" s="5" t="s">
+      <c r="AT2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AT2" s="5" t="s">
+      <c r="AU2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="AU2" s="5" t="s">
+      <c r="AV2" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="AV2" s="5" t="s">
+      <c r="AW2" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="AW2" s="5" t="s">
+      <c r="AX2" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="AX2" s="5" t="s">
+      <c r="AY2" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="AY2" s="5" t="s">
+      <c r="AZ2" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>43</v>
       </c>
@@ -1287,22 +1310,26 @@
       <c r="AE3" s="5">
         <v>4</v>
       </c>
-      <c r="AF3" s="5"/>
+      <c r="AF3" s="5">
+        <v>6663</v>
+      </c>
       <c r="AG3" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH3" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="AH3" s="5" t="s">
+      <c r="AI3" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="AI3" s="5"/>
       <c r="AJ3" s="5"/>
-      <c r="AK3" s="5" t="s">
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AL3" s="5" t="s">
+      <c r="AM3" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="AM3" s="5"/>
       <c r="AN3" s="5"/>
       <c r="AO3" s="5"/>
       <c r="AP3" s="5"/>
@@ -1310,19 +1337,20 @@
       <c r="AR3" s="5"/>
       <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
-      <c r="AU3" s="5" t="s">
+      <c r="AU3" s="5"/>
+      <c r="AV3" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="AV3" s="5"/>
-      <c r="AW3" s="5" t="s">
+      <c r="AW3" s="5"/>
+      <c r="AX3" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="AX3" s="5" t="s">
+      <c r="AY3" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="AY3" s="5"/>
+      <c r="AZ3" s="5"/>
     </row>
-    <row r="4" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
@@ -1365,14 +1393,14 @@
       <c r="AF4" s="4"/>
       <c r="AG4" s="4"/>
       <c r="AH4" s="4"/>
-      <c r="AI4" s="2" t="s">
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="4" t="s">
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="AL4" s="4"/>
       <c r="AM4" s="4"/>
       <c r="AN4" s="4"/>
       <c r="AO4" s="4"/>
@@ -1381,17 +1409,18 @@
       <c r="AR4" s="4"/>
       <c r="AS4" s="4"/>
       <c r="AT4" s="4"/>
-      <c r="AU4" s="4" t="s">
+      <c r="AU4" s="4"/>
+      <c r="AV4" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="AV4" s="4" t="s">
+      <c r="AW4" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="AW4" s="4"/>
       <c r="AX4" s="4"/>
       <c r="AY4" s="4"/>
+      <c r="AZ4" s="4"/>
     </row>
-    <row r="5" spans="1:51" ht="96" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>44</v>
       </c>
@@ -1449,28 +1478,28 @@
         <v>105</v>
       </c>
       <c r="AG5" s="5"/>
-      <c r="AH5" s="5" t="s">
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="AI5" s="5"/>
       <c r="AJ5" s="5"/>
-      <c r="AK5" s="5" t="s">
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AL5" s="5" t="s">
+      <c r="AM5" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="AM5" s="1" t="s">
+      <c r="AN5" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AN5" s="5" t="s">
+      <c r="AO5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AO5" s="6"/>
-      <c r="AP5" s="5" t="s">
+      <c r="AP5" s="6"/>
+      <c r="AQ5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AQ5" s="5"/>
       <c r="AR5" s="5"/>
       <c r="AS5" s="5"/>
       <c r="AT5" s="5"/>
@@ -1478,11 +1507,12 @@
       <c r="AV5" s="5"/>
       <c r="AW5" s="5"/>
       <c r="AX5" s="5"/>
-      <c r="AY5" s="5" t="s">
+      <c r="AY5" s="5"/>
+      <c r="AZ5" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:51" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>44</v>
       </c>
@@ -1536,22 +1566,26 @@
       <c r="AC6" s="5"/>
       <c r="AD6" s="5"/>
       <c r="AE6" s="5"/>
-      <c r="AF6" s="5"/>
-      <c r="AG6" s="5"/>
+      <c r="AF6" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AG6" s="5" t="s">
+        <v>149</v>
+      </c>
       <c r="AH6" s="5"/>
       <c r="AI6" s="5"/>
       <c r="AJ6" s="5"/>
-      <c r="AK6" s="5" t="s">
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AL6" s="5" t="s">
+      <c r="AM6" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="AM6" s="5"/>
-      <c r="AN6" s="5" t="s">
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AO6" s="5"/>
       <c r="AP6" s="5"/>
       <c r="AQ6" s="5"/>
       <c r="AR6" s="5"/>
@@ -1561,11 +1595,12 @@
       <c r="AV6" s="5"/>
       <c r="AW6" s="5"/>
       <c r="AX6" s="5"/>
-      <c r="AY6" s="5" t="s">
+      <c r="AY6" s="5"/>
+      <c r="AZ6" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>44</v>
       </c>
@@ -1611,10 +1646,10 @@
       <c r="AK7" s="5"/>
       <c r="AL7" s="5"/>
       <c r="AM7" s="5"/>
-      <c r="AN7" s="5" t="s">
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AO7" s="5"/>
       <c r="AP7" s="5"/>
       <c r="AQ7" s="5"/>
       <c r="AR7" s="5"/>
@@ -1624,11 +1659,12 @@
       <c r="AV7" s="5"/>
       <c r="AW7" s="5"/>
       <c r="AX7" s="5"/>
-      <c r="AY7" s="5" t="s">
+      <c r="AY7" s="5"/>
+      <c r="AZ7" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
@@ -1674,10 +1710,10 @@
       <c r="AK8" s="5"/>
       <c r="AL8" s="5"/>
       <c r="AM8" s="5"/>
-      <c r="AN8" s="5" t="s">
+      <c r="AN8" s="5"/>
+      <c r="AO8" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AO8" s="5"/>
       <c r="AP8" s="5"/>
       <c r="AQ8" s="5"/>
       <c r="AR8" s="5"/>
@@ -1688,8 +1724,9 @@
       <c r="AW8" s="5"/>
       <c r="AX8" s="5"/>
       <c r="AY8" s="5"/>
+      <c r="AZ8" s="5"/>
     </row>
-    <row r="9" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>44</v>
       </c>
@@ -1735,10 +1772,10 @@
       <c r="AK9" s="4"/>
       <c r="AL9" s="4"/>
       <c r="AM9" s="4"/>
-      <c r="AN9" s="4" t="s">
+      <c r="AN9" s="4"/>
+      <c r="AO9" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AO9" s="4"/>
       <c r="AP9" s="4"/>
       <c r="AQ9" s="4"/>
       <c r="AR9" s="4"/>
@@ -1749,8 +1786,9 @@
       <c r="AW9" s="4"/>
       <c r="AX9" s="4"/>
       <c r="AY9" s="4"/>
+      <c r="AZ9" s="4"/>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>122</v>
       </c>
@@ -1808,14 +1846,14 @@
       <c r="AK10" s="5"/>
       <c r="AL10" s="5"/>
       <c r="AM10" s="5"/>
-      <c r="AN10" s="5" t="s">
+      <c r="AN10" s="5"/>
+      <c r="AO10" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="AO10" s="6"/>
-      <c r="AP10" s="5" t="s">
+      <c r="AP10" s="6"/>
+      <c r="AQ10" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="AQ10" s="5"/>
       <c r="AR10" s="5"/>
       <c r="AS10" s="5"/>
       <c r="AT10" s="5"/>
@@ -1823,14 +1861,15 @@
       <c r="AV10" s="5"/>
       <c r="AW10" s="5"/>
       <c r="AX10" s="5"/>
-      <c r="AY10" s="5" t="s">
+      <c r="AY10" s="5"/>
+      <c r="AZ10" s="5" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AI4" r:id="rId1"/>
-    <hyperlink ref="AM5" r:id="rId2"/>
+    <hyperlink ref="AJ4" r:id="rId1"/>
+    <hyperlink ref="AN5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
AV_FILE and AV_SUBTITLES paths are relative to deposit rather than multi-deposit
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -422,30 +422,18 @@
     <t>Duckstad</t>
   </si>
   <si>
-    <t>ruimtereis01/reisverslag/centaur.mpg</t>
-  </si>
-  <si>
-    <t>ruimtereis01/reisverslag/centaur.srt</t>
-  </si>
-  <si>
     <t>video about the centaur meteorite</t>
   </si>
   <si>
     <t>application/vnd.openxmlformats-officedocument.wordprocessingml.document</t>
   </si>
   <si>
-    <t>ruimtereis01/path/to/a/random/sound/chicken.mp3</t>
-  </si>
-  <si>
     <t>our daily wake up call</t>
   </si>
   <si>
     <t>AV_SUBTITLES_LANGUAGE</t>
   </si>
   <si>
-    <t>ruimtereis01/reisverslag/centaur-nederlands.srt</t>
-  </si>
-  <si>
     <t>en</t>
   </si>
   <si>
@@ -486,6 +474,18 @@
   </si>
   <si>
     <t>ARCHIS-ZAAK-IDENTIFICATIE</t>
+  </si>
+  <si>
+    <t>reisverslag/centaur.mpg</t>
+  </si>
+  <si>
+    <t>path/to/a/random/sound/chicken.mp3</t>
+  </si>
+  <si>
+    <t>reisverslag/centaur-nederlands.srt</t>
+  </si>
+  <si>
+    <t>reisverslag/centaur.srt</t>
   </si>
 </sst>
 </file>
@@ -890,10 +890,10 @@
   <dimension ref="A1:AZ10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG3" sqref="AG3"/>
+      <selection pane="bottomRight" activeCell="AX2" sqref="AX2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1048,7 +1048,7 @@
         <v>31</v>
       </c>
       <c r="AG1" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="AH1" s="4" t="s">
         <v>32</v>
@@ -1102,7 +1102,7 @@
         <v>120</v>
       </c>
       <c r="AY1" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AZ1" s="4" t="s">
         <v>42</v>
@@ -1198,13 +1198,13 @@
       </c>
       <c r="AJ2" s="8"/>
       <c r="AK2" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="AN2" s="5" t="s">
         <v>113</v>
@@ -1228,19 +1228,19 @@
         <v>80</v>
       </c>
       <c r="AU2" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AV2" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AW2" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="AW2" s="5" t="s">
-        <v>132</v>
-      </c>
       <c r="AX2" s="5" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="AY2" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="AZ2" s="5" t="s">
         <v>81</v>
@@ -1314,7 +1314,7 @@
         <v>6663</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="AH3" s="5" t="s">
         <v>107</v>
@@ -1328,7 +1328,7 @@
         <v>69</v>
       </c>
       <c r="AM3" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="AN3" s="5"/>
       <c r="AO3" s="5"/>
@@ -1339,14 +1339,14 @@
       <c r="AT3" s="5"/>
       <c r="AU3" s="5"/>
       <c r="AV3" s="5" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="AW3" s="5"/>
       <c r="AX3" s="5" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="AY3" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="AZ3" s="5"/>
     </row>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="AK4" s="4"/>
       <c r="AL4" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AM4" s="4"/>
       <c r="AN4" s="4"/>
@@ -1411,10 +1411,10 @@
       <c r="AT4" s="4"/>
       <c r="AU4" s="4"/>
       <c r="AV4" s="4" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="AW4" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AX4" s="4"/>
       <c r="AY4" s="4"/>
@@ -1488,7 +1488,7 @@
         <v>70</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="AN5" s="1" t="s">
         <v>112</v>
@@ -1567,10 +1567,10 @@
       <c r="AD6" s="5"/>
       <c r="AE6" s="5"/>
       <c r="AF6" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="AG6" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="AH6" s="5"/>
       <c r="AI6" s="5"/>
@@ -1580,7 +1580,7 @@
         <v>69</v>
       </c>
       <c r="AM6" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="AN6" s="5"/>
       <c r="AO6" s="5" t="s">
@@ -1852,7 +1852,7 @@
       </c>
       <c r="AP10" s="6"/>
       <c r="AQ10" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="AR10" s="5"/>
       <c r="AS10" s="5"/>

</xml_diff>

<commit_message>
it is not allowed to have both audio and video files in one dataset
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -29,8 +29,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Richard van Heest</author>
+  </authors>
+  <commentList>
+    <comment ref="AP1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Richard van Heest:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+if not filled in, today's date is taken as default</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="158">
   <si>
     <t>DATASET</t>
   </si>
@@ -486,6 +520,24 @@
   </si>
   <si>
     <t>reisverslag/centaur.srt</t>
+  </si>
+  <si>
+    <t>ruimtereis04</t>
+  </si>
+  <si>
+    <t>OPEN_ACCESS_FOR_REGISTERED_USERS</t>
+  </si>
+  <si>
+    <t>This is a dataset with audio in it</t>
+  </si>
+  <si>
+    <t>Audio Dataset</t>
+  </si>
+  <si>
+    <t>Guus</t>
+  </si>
+  <si>
+    <t>Geluk</t>
   </si>
 </sst>
 </file>
@@ -496,7 +548,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -541,16 +593,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -565,6 +636,26 @@
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -582,23 +673,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -886,14 +986,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AZ11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AX2" sqref="AX2"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -937,7 +1037,7 @@
     <col min="38" max="38" width="65.6640625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="11.1640625" bestFit="1" customWidth="1"/>
@@ -951,918 +1051,967 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AO1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AQ1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AU1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AV1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AW1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AX1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AY1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:52" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="12"/>
+      <c r="I2" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5" t="s">
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2" s="16">
         <v>42143</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5" t="s">
+      <c r="U2" s="4"/>
+      <c r="V2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="W2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="X2" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Y2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="Z2" s="5">
+      <c r="Z2" s="4">
         <v>83575.399999999994</v>
       </c>
-      <c r="AA2" s="5">
+      <c r="AA2" s="4">
         <v>455271.2</v>
       </c>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5" t="s">
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5" t="s">
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AI2" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AJ2" s="8"/>
-      <c r="AK2" s="5" t="s">
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="AL2" s="5" t="s">
+      <c r="AL2" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="AM2" s="5" t="s">
+      <c r="AM2" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="AN2" s="5" t="s">
+      <c r="AN2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="AO2" s="5" t="s">
+      <c r="AO2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AP2" s="6">
+      <c r="AP2" s="16">
         <v>33815</v>
       </c>
-      <c r="AQ2" s="5" t="s">
+      <c r="AQ2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="AR2" s="5" t="s">
+      <c r="AR2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AS2" s="5" t="s">
+      <c r="AS2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AT2" s="5" t="s">
+      <c r="AT2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AU2" s="5" t="s">
+      <c r="AU2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="AV2" s="5" t="s">
+      <c r="AV2" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="AW2" s="5" t="s">
+      <c r="AW2" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="AX2" s="5" t="s">
+      <c r="AX2" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="AY2" s="5" t="s">
+      <c r="AY2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="AZ2" s="5" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="5" t="s">
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="T3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5" t="s">
+      <c r="U3" s="4"/>
+      <c r="V3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5" t="s">
+      <c r="W3" s="4"/>
+      <c r="X3" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Y3" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5">
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4">
         <v>1</v>
       </c>
-      <c r="AC3" s="5">
+      <c r="AC3" s="4">
         <v>2</v>
       </c>
-      <c r="AD3" s="5">
+      <c r="AD3" s="4">
         <v>3</v>
       </c>
-      <c r="AE3" s="5">
+      <c r="AE3" s="4">
         <v>4</v>
       </c>
-      <c r="AF3" s="5">
+      <c r="AF3" s="4">
         <v>6663</v>
       </c>
-      <c r="AG3" s="5" t="s">
+      <c r="AG3" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="AH3" s="5" t="s">
+      <c r="AH3" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="AI3" s="5" t="s">
+      <c r="AI3" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="AJ3" s="5"/>
-      <c r="AK3" s="5"/>
-      <c r="AL3" s="5" t="s">
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AM3" s="5" t="s">
+      <c r="AM3" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="AN3" s="5"/>
-      <c r="AO3" s="5"/>
-      <c r="AP3" s="5"/>
-      <c r="AQ3" s="5"/>
-      <c r="AR3" s="5"/>
-      <c r="AS3" s="5"/>
-      <c r="AT3" s="5"/>
-      <c r="AU3" s="5"/>
-      <c r="AV3" s="5" t="s">
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="12"/>
+      <c r="AP3" s="12"/>
+      <c r="AQ3" s="12"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="4"/>
+      <c r="AT3" s="4"/>
+      <c r="AU3" s="4"/>
+      <c r="AV3" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="AW3" s="5"/>
-      <c r="AX3" s="5" t="s">
+      <c r="AW3" s="4"/>
+      <c r="AX3" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="AY3" s="5" t="s">
+      <c r="AY3" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="AZ3" s="5"/>
+      <c r="AZ3" s="4"/>
     </row>
     <row r="4" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="4" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="R4" s="4"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="4" t="s">
+      <c r="R4" s="3"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="U4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="4"/>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
       <c r="AJ4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4" t="s">
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="4"/>
-      <c r="AQ4" s="4"/>
-      <c r="AR4" s="4"/>
-      <c r="AS4" s="4"/>
-      <c r="AT4" s="4"/>
-      <c r="AU4" s="4"/>
-      <c r="AV4" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="AW4" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="AX4" s="4"/>
-      <c r="AY4" s="4"/>
-      <c r="AZ4" s="4"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="11"/>
+      <c r="AP4" s="11"/>
+      <c r="AQ4" s="11"/>
+      <c r="AR4" s="3"/>
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="3"/>
+      <c r="AU4" s="3"/>
+      <c r="AV4" s="7"/>
+      <c r="AW4" s="7"/>
+      <c r="AX4" s="3"/>
+      <c r="AY4" s="3"/>
+      <c r="AZ4" s="3"/>
     </row>
     <row r="5" spans="1:52" ht="96" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5" t="s">
+      <c r="H5" s="12"/>
+      <c r="I5" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="6">
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="16">
         <v>42137</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="R5" s="5"/>
-      <c r="S5" s="7" t="s">
+      <c r="R5" s="4"/>
+      <c r="S5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="T5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5" t="s">
+      <c r="U5" s="4"/>
+      <c r="V5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5" t="s">
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AG5" s="5"/>
-      <c r="AH5" s="5"/>
-      <c r="AI5" s="5" t="s">
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="AJ5" s="5"/>
-      <c r="AK5" s="5"/>
-      <c r="AL5" s="5" t="s">
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AM5" s="5" t="s">
+      <c r="AM5" s="4" t="s">
         <v>141</v>
       </c>
       <c r="AN5" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AO5" s="5" t="s">
+      <c r="AO5" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AP5" s="6"/>
-      <c r="AQ5" s="5" t="s">
+      <c r="AP5" s="16"/>
+      <c r="AQ5" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="AR5" s="5"/>
-      <c r="AS5" s="5"/>
-      <c r="AT5" s="5"/>
-      <c r="AU5" s="5"/>
-      <c r="AV5" s="5"/>
-      <c r="AW5" s="5"/>
-      <c r="AX5" s="5"/>
-      <c r="AY5" s="5"/>
-      <c r="AZ5" s="5" t="s">
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="4"/>
+      <c r="AT5" s="4"/>
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="4"/>
+      <c r="AW5" s="4"/>
+      <c r="AX5" s="4"/>
+      <c r="AY5" s="4"/>
+      <c r="AZ5" s="4" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:52" ht="96" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="6">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="16">
         <v>42137</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="Q6" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="R6" s="5"/>
-      <c r="S6" s="7" t="s">
+      <c r="R6" s="4"/>
+      <c r="S6" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="T6" s="5" t="s">
+      <c r="T6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="5"/>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="5"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="5" t="s">
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="AG6" s="5" t="s">
+      <c r="AG6" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="AH6" s="5"/>
-      <c r="AI6" s="5"/>
-      <c r="AJ6" s="5"/>
-      <c r="AK6" s="5"/>
-      <c r="AL6" s="5" t="s">
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AM6" s="5" t="s">
+      <c r="AM6" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="AN6" s="5"/>
-      <c r="AO6" s="5" t="s">
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AP6" s="5"/>
-      <c r="AQ6" s="5"/>
-      <c r="AR6" s="5"/>
-      <c r="AS6" s="5"/>
-      <c r="AT6" s="5"/>
-      <c r="AU6" s="5"/>
-      <c r="AV6" s="5"/>
-      <c r="AW6" s="5"/>
-      <c r="AX6" s="5"/>
-      <c r="AY6" s="5"/>
-      <c r="AZ6" s="5" t="s">
+      <c r="AP6" s="12"/>
+      <c r="AQ6" s="12"/>
+      <c r="AR6" s="4"/>
+      <c r="AS6" s="4"/>
+      <c r="AT6" s="4"/>
+      <c r="AU6" s="4"/>
+      <c r="AV6" s="4"/>
+      <c r="AW6" s="4"/>
+      <c r="AX6" s="4"/>
+      <c r="AY6" s="4"/>
+      <c r="AZ6" s="4" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="6">
+      <c r="B7" s="12"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="16">
         <v>42137</v>
       </c>
-      <c r="Q7" s="5" t="s">
+      <c r="Q7" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="5"/>
-      <c r="AB7" s="5"/>
-      <c r="AC7" s="5"/>
-      <c r="AD7" s="5"/>
-      <c r="AE7" s="5"/>
-      <c r="AF7" s="5"/>
-      <c r="AG7" s="5"/>
-      <c r="AH7" s="5"/>
-      <c r="AI7" s="5"/>
-      <c r="AJ7" s="5"/>
-      <c r="AK7" s="5"/>
-      <c r="AL7" s="5"/>
-      <c r="AM7" s="5"/>
-      <c r="AN7" s="5"/>
-      <c r="AO7" s="5" t="s">
+      <c r="R7" s="4"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="4"/>
+      <c r="AH7" s="4"/>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
+      <c r="AN7" s="4"/>
+      <c r="AO7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AP7" s="5"/>
-      <c r="AQ7" s="5"/>
-      <c r="AR7" s="5"/>
-      <c r="AS7" s="5"/>
-      <c r="AT7" s="5"/>
-      <c r="AU7" s="5"/>
-      <c r="AV7" s="5"/>
-      <c r="AW7" s="5"/>
-      <c r="AX7" s="5"/>
-      <c r="AY7" s="5"/>
-      <c r="AZ7" s="5" t="s">
+      <c r="AP7" s="12"/>
+      <c r="AQ7" s="12"/>
+      <c r="AR7" s="4"/>
+      <c r="AS7" s="4"/>
+      <c r="AT7" s="4"/>
+      <c r="AU7" s="4"/>
+      <c r="AV7" s="4"/>
+      <c r="AW7" s="4"/>
+      <c r="AX7" s="4"/>
+      <c r="AY7" s="4"/>
+      <c r="AZ7" s="4" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6">
+      <c r="B8" s="12"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="16">
         <v>42137</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
-      <c r="AE8" s="5"/>
-      <c r="AF8" s="5"/>
-      <c r="AG8" s="5"/>
-      <c r="AH8" s="5"/>
-      <c r="AI8" s="5"/>
-      <c r="AJ8" s="5"/>
-      <c r="AK8" s="5"/>
-      <c r="AL8" s="5"/>
-      <c r="AM8" s="5"/>
-      <c r="AN8" s="5"/>
-      <c r="AO8" s="5" t="s">
+      <c r="R8" s="4"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="4"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="4"/>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="4"/>
+      <c r="AN8" s="4"/>
+      <c r="AO8" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AP8" s="5"/>
-      <c r="AQ8" s="5"/>
-      <c r="AR8" s="5"/>
-      <c r="AS8" s="5"/>
-      <c r="AT8" s="5"/>
-      <c r="AU8" s="5"/>
-      <c r="AV8" s="5"/>
-      <c r="AW8" s="5"/>
-      <c r="AX8" s="5"/>
-      <c r="AY8" s="5"/>
-      <c r="AZ8" s="5"/>
+      <c r="AP8" s="12"/>
+      <c r="AQ8" s="12"/>
+      <c r="AR8" s="4"/>
+      <c r="AS8" s="4"/>
+      <c r="AT8" s="4"/>
+      <c r="AU8" s="4"/>
+      <c r="AV8" s="4"/>
+      <c r="AW8" s="4"/>
+      <c r="AX8" s="4"/>
+      <c r="AY8" s="4"/>
+      <c r="AZ8" s="4"/>
     </row>
     <row r="9" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="9">
+      <c r="B9" s="11"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="17">
         <v>42137</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="Q9" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
-      <c r="AA9" s="4"/>
-      <c r="AB9" s="4"/>
-      <c r="AC9" s="4"/>
-      <c r="AD9" s="4"/>
-      <c r="AE9" s="4"/>
-      <c r="AF9" s="4"/>
-      <c r="AG9" s="4"/>
-      <c r="AH9" s="4"/>
-      <c r="AI9" s="4"/>
-      <c r="AJ9" s="4"/>
-      <c r="AK9" s="4"/>
-      <c r="AL9" s="4"/>
-      <c r="AM9" s="4"/>
-      <c r="AN9" s="4"/>
-      <c r="AO9" s="4" t="s">
+      <c r="R9" s="3"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="3"/>
+      <c r="AO9" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AP9" s="4"/>
-      <c r="AQ9" s="4"/>
-      <c r="AR9" s="4"/>
-      <c r="AS9" s="4"/>
-      <c r="AT9" s="4"/>
-      <c r="AU9" s="4"/>
-      <c r="AV9" s="4"/>
-      <c r="AW9" s="4"/>
-      <c r="AX9" s="4"/>
-      <c r="AY9" s="4"/>
-      <c r="AZ9" s="4"/>
+      <c r="AP9" s="11"/>
+      <c r="AQ9" s="11"/>
+      <c r="AR9" s="3"/>
+      <c r="AS9" s="3"/>
+      <c r="AT9" s="3"/>
+      <c r="AU9" s="3"/>
+      <c r="AV9" s="3"/>
+      <c r="AW9" s="3"/>
+      <c r="AX9" s="3"/>
+      <c r="AY9" s="3"/>
+      <c r="AZ9" s="3"/>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="6">
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="18">
         <v>42581</v>
       </c>
-      <c r="Q10" s="5" t="s">
+      <c r="Q10" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5" t="s">
+      <c r="R10" s="6"/>
+      <c r="S10" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="T10" s="5" t="s">
+      <c r="T10" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
-      <c r="AG10" s="5"/>
-      <c r="AH10" s="5"/>
-      <c r="AI10" s="5"/>
-      <c r="AJ10" s="5"/>
-      <c r="AK10" s="5"/>
-      <c r="AL10" s="5"/>
-      <c r="AM10" s="5"/>
-      <c r="AN10" s="5"/>
-      <c r="AO10" s="5" t="s">
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="6"/>
+      <c r="AI10" s="6"/>
+      <c r="AJ10" s="6"/>
+      <c r="AK10" s="6"/>
+      <c r="AL10" s="6"/>
+      <c r="AM10" s="6"/>
+      <c r="AN10" s="6"/>
+      <c r="AO10" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="AP10" s="6"/>
-      <c r="AQ10" s="5" t="s">
+      <c r="AP10" s="18"/>
+      <c r="AQ10" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="AR10" s="5"/>
-      <c r="AS10" s="5"/>
-      <c r="AT10" s="5"/>
-      <c r="AU10" s="5"/>
-      <c r="AV10" s="5"/>
-      <c r="AW10" s="5"/>
-      <c r="AX10" s="5"/>
-      <c r="AY10" s="5"/>
-      <c r="AZ10" s="5" t="s">
+      <c r="AR10" s="6"/>
+      <c r="AS10" s="6"/>
+      <c r="AT10" s="6"/>
+      <c r="AU10" s="6"/>
+      <c r="AV10" s="6"/>
+      <c r="AW10" s="6"/>
+      <c r="AX10" s="6"/>
+      <c r="AY10" s="6"/>
+      <c r="AZ10" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="P11" s="16">
+        <v>42582</v>
+      </c>
+      <c r="S11" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="AO11" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP11" s="16">
+        <v>42581</v>
+      </c>
+      <c r="AQ11" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV11" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="AW11" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AZ11" s="9" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1873,5 +2022,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add SF_PLAY_MODE to test data
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,27 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38640" windowHeight="21840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AY$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AZ$9</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -64,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="161">
   <si>
     <t>DATASET</t>
   </si>
@@ -538,6 +530,15 @@
   </si>
   <si>
     <t>Geluk</t>
+  </si>
+  <si>
+    <t>SF_PLAY_MODE</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>continuous</t>
   </si>
 </sst>
 </file>
@@ -701,18 +702,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="12">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -979,7 +980,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -987,70 +988,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ11"/>
+  <dimension ref="A1:BA11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AQ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="AV11" sqref="AV11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="50.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="50.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.875" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="14" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="17" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="65.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="65.625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="34.375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="23" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="17.875" customWidth="1"/>
+    <col min="49" max="49" width="43.125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="29.375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="40.375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1193,22 +1195,25 @@
         <v>117</v>
       </c>
       <c r="AV1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AW1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:52" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>43</v>
       </c>
@@ -1331,22 +1336,25 @@
         <v>136</v>
       </c>
       <c r="AV2" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AW2" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BA2" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>43</v>
       </c>
@@ -1438,19 +1446,20 @@
       <c r="AS3" s="4"/>
       <c r="AT3" s="4"/>
       <c r="AU3" s="4"/>
-      <c r="AV3" s="4" t="s">
+      <c r="AV3" s="4"/>
+      <c r="AW3" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="AW3" s="4"/>
-      <c r="AX3" s="4" t="s">
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="AY3" s="4" t="s">
+      <c r="AZ3" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="AZ3" s="4"/>
+      <c r="BA3" s="4"/>
     </row>
-    <row r="4" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>43</v>
       </c>
@@ -1510,13 +1519,14 @@
       <c r="AS4" s="3"/>
       <c r="AT4" s="3"/>
       <c r="AU4" s="3"/>
-      <c r="AV4" s="7"/>
+      <c r="AV4" s="3"/>
       <c r="AW4" s="7"/>
-      <c r="AX4" s="3"/>
+      <c r="AX4" s="7"/>
       <c r="AY4" s="3"/>
       <c r="AZ4" s="3"/>
+      <c r="BA4" s="3"/>
     </row>
-    <row r="5" spans="1:52" ht="96" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>44</v>
       </c>
@@ -1604,11 +1614,12 @@
       <c r="AW5" s="4"/>
       <c r="AX5" s="4"/>
       <c r="AY5" s="4"/>
-      <c r="AZ5" s="4" t="s">
+      <c r="AZ5" s="4"/>
+      <c r="BA5" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>44</v>
       </c>
@@ -1692,11 +1703,12 @@
       <c r="AW6" s="4"/>
       <c r="AX6" s="4"/>
       <c r="AY6" s="4"/>
-      <c r="AZ6" s="4" t="s">
+      <c r="AZ6" s="4"/>
+      <c r="BA6" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>44</v>
       </c>
@@ -1756,11 +1768,12 @@
       <c r="AW7" s="4"/>
       <c r="AX7" s="4"/>
       <c r="AY7" s="4"/>
-      <c r="AZ7" s="4" t="s">
+      <c r="AZ7" s="4"/>
+      <c r="BA7" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>44</v>
       </c>
@@ -1821,8 +1834,9 @@
       <c r="AX8" s="4"/>
       <c r="AY8" s="4"/>
       <c r="AZ8" s="4"/>
+      <c r="BA8" s="4"/>
     </row>
-    <row r="9" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>44</v>
       </c>
@@ -1883,8 +1897,9 @@
       <c r="AX9" s="3"/>
       <c r="AY9" s="3"/>
       <c r="AZ9" s="3"/>
+      <c r="BA9" s="3"/>
     </row>
-    <row r="10" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>122</v>
       </c>
@@ -1958,11 +1973,12 @@
       <c r="AW10" s="6"/>
       <c r="AX10" s="6"/>
       <c r="AY10" s="6"/>
-      <c r="AZ10" s="6" t="s">
+      <c r="AZ10" s="6"/>
+      <c r="BA10" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>152</v>
       </c>
@@ -2005,13 +2021,16 @@
       <c r="AT11" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AV11" s="8" t="s">
+      <c r="AV11" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AW11" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="AW11" s="8" t="s">
+      <c r="AX11" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="AZ11" s="9" t="s">
+      <c r="BA11" s="9" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2021,7 +2040,7 @@
     <hyperlink ref="AN5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EASY-1314 SF_PLAY_MODE in deposit.properties (#80)
* parse the PlayMode from the csv
* add the PlayMode to deposit.properties
* add tests accordingly
* remove an old forgotten version file
* separate the tests in BlackBoxSpec
* fix a bug in xml formatting
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,27 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38640" windowHeight="21840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AY$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AZ$9</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -64,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="161">
   <si>
     <t>DATASET</t>
   </si>
@@ -538,6 +530,15 @@
   </si>
   <si>
     <t>Geluk</t>
+  </si>
+  <si>
+    <t>SF_PLAY_MODE</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>continuous</t>
   </si>
 </sst>
 </file>
@@ -701,18 +702,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="12">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -979,7 +980,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -987,70 +988,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ11"/>
+  <dimension ref="A1:BA11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AQ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="AV11" sqref="AV11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="50.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="50.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.875" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="14" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="17" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="65.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="65.625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="34.375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="23" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="17.875" customWidth="1"/>
+    <col min="49" max="49" width="43.125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="29.375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="40.375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1193,22 +1195,25 @@
         <v>117</v>
       </c>
       <c r="AV1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AW1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:52" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>43</v>
       </c>
@@ -1331,22 +1336,25 @@
         <v>136</v>
       </c>
       <c r="AV2" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AW2" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BA2" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>43</v>
       </c>
@@ -1438,19 +1446,20 @@
       <c r="AS3" s="4"/>
       <c r="AT3" s="4"/>
       <c r="AU3" s="4"/>
-      <c r="AV3" s="4" t="s">
+      <c r="AV3" s="4"/>
+      <c r="AW3" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="AW3" s="4"/>
-      <c r="AX3" s="4" t="s">
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="AY3" s="4" t="s">
+      <c r="AZ3" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="AZ3" s="4"/>
+      <c r="BA3" s="4"/>
     </row>
-    <row r="4" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>43</v>
       </c>
@@ -1510,13 +1519,14 @@
       <c r="AS4" s="3"/>
       <c r="AT4" s="3"/>
       <c r="AU4" s="3"/>
-      <c r="AV4" s="7"/>
+      <c r="AV4" s="3"/>
       <c r="AW4" s="7"/>
-      <c r="AX4" s="3"/>
+      <c r="AX4" s="7"/>
       <c r="AY4" s="3"/>
       <c r="AZ4" s="3"/>
+      <c r="BA4" s="3"/>
     </row>
-    <row r="5" spans="1:52" ht="96" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>44</v>
       </c>
@@ -1604,11 +1614,12 @@
       <c r="AW5" s="4"/>
       <c r="AX5" s="4"/>
       <c r="AY5" s="4"/>
-      <c r="AZ5" s="4" t="s">
+      <c r="AZ5" s="4"/>
+      <c r="BA5" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>44</v>
       </c>
@@ -1692,11 +1703,12 @@
       <c r="AW6" s="4"/>
       <c r="AX6" s="4"/>
       <c r="AY6" s="4"/>
-      <c r="AZ6" s="4" t="s">
+      <c r="AZ6" s="4"/>
+      <c r="BA6" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>44</v>
       </c>
@@ -1756,11 +1768,12 @@
       <c r="AW7" s="4"/>
       <c r="AX7" s="4"/>
       <c r="AY7" s="4"/>
-      <c r="AZ7" s="4" t="s">
+      <c r="AZ7" s="4"/>
+      <c r="BA7" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>44</v>
       </c>
@@ -1821,8 +1834,9 @@
       <c r="AX8" s="4"/>
       <c r="AY8" s="4"/>
       <c r="AZ8" s="4"/>
+      <c r="BA8" s="4"/>
     </row>
-    <row r="9" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>44</v>
       </c>
@@ -1883,8 +1897,9 @@
       <c r="AX9" s="3"/>
       <c r="AY9" s="3"/>
       <c r="AZ9" s="3"/>
+      <c r="BA9" s="3"/>
     </row>
-    <row r="10" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>122</v>
       </c>
@@ -1958,11 +1973,12 @@
       <c r="AW10" s="6"/>
       <c r="AX10" s="6"/>
       <c r="AY10" s="6"/>
-      <c r="AZ10" s="6" t="s">
+      <c r="AZ10" s="6"/>
+      <c r="BA10" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>152</v>
       </c>
@@ -2005,13 +2021,16 @@
       <c r="AT11" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AV11" s="8" t="s">
+      <c r="AV11" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AW11" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="AW11" s="8" t="s">
+      <c r="AX11" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="AZ11" s="9" t="s">
+      <c r="BA11" s="9" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2021,7 +2040,7 @@
     <hyperlink ref="AN5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EASY-1319: Qualifiers on dates (#87)
* date with qualifier
* license headers
* new invalid CSV lines
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38640" windowHeight="21840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AZ$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BB$9</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +35,7 @@
     <author>Richard van Heest</author>
   </authors>
   <commentList>
-    <comment ref="AP1" authorId="0">
+    <comment ref="AR1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="167">
   <si>
     <t>DATASET</t>
   </si>
@@ -539,6 +547,24 @@
   </si>
   <si>
     <t>continuous</t>
+  </si>
+  <si>
+    <t>DCT_DATE</t>
+  </si>
+  <si>
+    <t>DCT_DATE_QUALIFIER</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>Issued</t>
+  </si>
+  <si>
+    <t>Date Accepted</t>
+  </si>
+  <si>
+    <t>Date Copyrighted</t>
   </si>
 </sst>
 </file>
@@ -660,7 +686,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -673,8 +699,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -700,20 +741,41 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="12">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="11" builtinId="9" hidden="1"/>
+  <cellStyles count="27">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -980,7 +1042,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -988,71 +1050,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA11"/>
+  <dimension ref="A1:BC11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AQ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AV11" sqref="AV11"/>
+      <selection pane="bottomRight" activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="50.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="14" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="17" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="24.125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="65.625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="22.375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="34.375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="17.875" customWidth="1"/>
-    <col min="49" max="49" width="43.125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="29.375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="40.375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="17.83203125" customWidth="1"/>
+    <col min="51" max="51" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1162,58 +1226,64 @@
         <v>34</v>
       </c>
       <c r="AK1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AM1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AQ1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="11" t="s">
+      <c r="AR1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="11" t="s">
+      <c r="AS1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:53" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>43</v>
       </c>
@@ -1302,59 +1372,65 @@
         <v>108</v>
       </c>
       <c r="AJ2" s="5"/>
-      <c r="AK2" s="4" t="s">
+      <c r="AK2" s="25">
+        <v>42946</v>
+      </c>
+      <c r="AL2" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="AM2" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AN2" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="AO2" s="12" t="s">
+      <c r="AQ2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AP2" s="16">
+      <c r="AR2" s="16">
         <v>33815</v>
       </c>
-      <c r="AQ2" s="12" t="s">
+      <c r="AS2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AU2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="BA2" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BB2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="BA2" s="4" t="s">
+      <c r="BC2" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>43</v>
       </c>
@@ -1431,35 +1507,41 @@
         <v>109</v>
       </c>
       <c r="AJ3" s="4"/>
-      <c r="AK3" s="4"/>
+      <c r="AK3" s="25">
+        <v>42947</v>
+      </c>
       <c r="AL3" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AM3" s="4" t="s">
+      <c r="AO3" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="AN3" s="4"/>
-      <c r="AO3" s="12"/>
-      <c r="AP3" s="12"/>
+      <c r="AP3" s="4"/>
       <c r="AQ3" s="12"/>
-      <c r="AR3" s="4"/>
-      <c r="AS3" s="4"/>
+      <c r="AR3" s="12"/>
+      <c r="AS3" s="12"/>
       <c r="AT3" s="4"/>
       <c r="AU3" s="4"/>
       <c r="AV3" s="4"/>
-      <c r="AW3" s="4" t="s">
-        <v>148</v>
-      </c>
+      <c r="AW3" s="4"/>
       <c r="AX3" s="4"/>
       <c r="AY3" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ3" s="4"/>
+      <c r="BA3" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="AZ3" s="4" t="s">
+      <c r="BB3" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="BA3" s="4"/>
+      <c r="BC3" s="4"/>
     </row>
-    <row r="4" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>43</v>
       </c>
@@ -1506,27 +1588,29 @@
       <c r="AJ4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AK4" s="3"/>
-      <c r="AL4" s="3" t="s">
+      <c r="AK4" s="22"/>
+      <c r="AL4" s="22"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="AM4" s="3"/>
-      <c r="AN4" s="3"/>
-      <c r="AO4" s="11"/>
-      <c r="AP4" s="11"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="3"/>
       <c r="AQ4" s="11"/>
-      <c r="AR4" s="3"/>
-      <c r="AS4" s="3"/>
+      <c r="AR4" s="11"/>
+      <c r="AS4" s="11"/>
       <c r="AT4" s="3"/>
       <c r="AU4" s="3"/>
       <c r="AV4" s="3"/>
-      <c r="AW4" s="7"/>
-      <c r="AX4" s="7"/>
-      <c r="AY4" s="3"/>
-      <c r="AZ4" s="3"/>
+      <c r="AW4" s="3"/>
+      <c r="AX4" s="3"/>
+      <c r="AY4" s="7"/>
+      <c r="AZ4" s="7"/>
       <c r="BA4" s="3"/>
+      <c r="BB4" s="3"/>
+      <c r="BC4" s="3"/>
     </row>
-    <row r="5" spans="1:53" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>44</v>
       </c>
@@ -1589,25 +1673,30 @@
         <v>110</v>
       </c>
       <c r="AJ5" s="4"/>
-      <c r="AK5" s="4"/>
-      <c r="AL5" s="4" t="s">
+      <c r="AK5" s="26">
+        <f>AK3+DAY(1)</f>
+        <v>42948</v>
+      </c>
+      <c r="AL5" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AM5" s="4" t="s">
+      <c r="AO5" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="AN5" s="1" t="s">
+      <c r="AP5" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AO5" s="12" t="s">
+      <c r="AQ5" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AP5" s="16"/>
-      <c r="AQ5" s="12" t="s">
+      <c r="AR5" s="16"/>
+      <c r="AS5" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="AR5" s="4"/>
-      <c r="AS5" s="4"/>
       <c r="AT5" s="4"/>
       <c r="AU5" s="4"/>
       <c r="AV5" s="4"/>
@@ -1615,11 +1704,13 @@
       <c r="AX5" s="4"/>
       <c r="AY5" s="4"/>
       <c r="AZ5" s="4"/>
-      <c r="BA5" s="4" t="s">
+      <c r="BA5" s="4"/>
+      <c r="BB5" s="4"/>
+      <c r="BC5" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:53" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>44</v>
       </c>
@@ -1682,21 +1773,23 @@
       <c r="AH6" s="4"/>
       <c r="AI6" s="4"/>
       <c r="AJ6" s="4"/>
-      <c r="AK6" s="4"/>
-      <c r="AL6" s="4" t="s">
+      <c r="AK6" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL6" s="21"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AM6" s="4" t="s">
+      <c r="AO6" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="AN6" s="4"/>
-      <c r="AO6" s="12" t="s">
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AP6" s="12"/>
-      <c r="AQ6" s="12"/>
-      <c r="AR6" s="4"/>
-      <c r="AS6" s="4"/>
+      <c r="AR6" s="12"/>
+      <c r="AS6" s="12"/>
       <c r="AT6" s="4"/>
       <c r="AU6" s="4"/>
       <c r="AV6" s="4"/>
@@ -1704,11 +1797,13 @@
       <c r="AX6" s="4"/>
       <c r="AY6" s="4"/>
       <c r="AZ6" s="4"/>
-      <c r="BA6" s="4" t="s">
+      <c r="BA6" s="4"/>
+      <c r="BB6" s="4"/>
+      <c r="BC6" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>44</v>
       </c>
@@ -1751,17 +1846,17 @@
       <c r="AH7" s="4"/>
       <c r="AI7" s="4"/>
       <c r="AJ7" s="4"/>
-      <c r="AK7" s="4"/>
-      <c r="AL7" s="4"/>
+      <c r="AK7" s="21"/>
+      <c r="AL7" s="21"/>
       <c r="AM7" s="4"/>
       <c r="AN7" s="4"/>
-      <c r="AO7" s="12" t="s">
+      <c r="AO7" s="4"/>
+      <c r="AP7" s="4"/>
+      <c r="AQ7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AP7" s="12"/>
-      <c r="AQ7" s="12"/>
-      <c r="AR7" s="4"/>
-      <c r="AS7" s="4"/>
+      <c r="AR7" s="12"/>
+      <c r="AS7" s="12"/>
       <c r="AT7" s="4"/>
       <c r="AU7" s="4"/>
       <c r="AV7" s="4"/>
@@ -1769,11 +1864,13 @@
       <c r="AX7" s="4"/>
       <c r="AY7" s="4"/>
       <c r="AZ7" s="4"/>
-      <c r="BA7" s="4" t="s">
+      <c r="BA7" s="4"/>
+      <c r="BB7" s="4"/>
+      <c r="BC7" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>44</v>
       </c>
@@ -1816,17 +1913,22 @@
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
       <c r="AJ8" s="4"/>
-      <c r="AK8" s="4"/>
-      <c r="AL8" s="4"/>
+      <c r="AK8" s="26">
+        <f>AK5+DAY(1)</f>
+        <v>42949</v>
+      </c>
+      <c r="AL8" s="21" t="s">
+        <v>166</v>
+      </c>
       <c r="AM8" s="4"/>
       <c r="AN8" s="4"/>
-      <c r="AO8" s="12" t="s">
+      <c r="AO8" s="4"/>
+      <c r="AP8" s="4"/>
+      <c r="AQ8" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AP8" s="12"/>
-      <c r="AQ8" s="12"/>
-      <c r="AR8" s="4"/>
-      <c r="AS8" s="4"/>
+      <c r="AR8" s="12"/>
+      <c r="AS8" s="12"/>
       <c r="AT8" s="4"/>
       <c r="AU8" s="4"/>
       <c r="AV8" s="4"/>
@@ -1835,8 +1937,10 @@
       <c r="AY8" s="4"/>
       <c r="AZ8" s="4"/>
       <c r="BA8" s="4"/>
+      <c r="BB8" s="4"/>
+      <c r="BC8" s="4"/>
     </row>
-    <row r="9" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>44</v>
       </c>
@@ -1879,17 +1983,17 @@
       <c r="AH9" s="3"/>
       <c r="AI9" s="3"/>
       <c r="AJ9" s="3"/>
-      <c r="AK9" s="3"/>
-      <c r="AL9" s="3"/>
+      <c r="AK9" s="23"/>
+      <c r="AL9" s="23"/>
       <c r="AM9" s="3"/>
       <c r="AN9" s="3"/>
-      <c r="AO9" s="11" t="s">
+      <c r="AO9" s="3"/>
+      <c r="AP9" s="3"/>
+      <c r="AQ9" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AP9" s="11"/>
-      <c r="AQ9" s="11"/>
-      <c r="AR9" s="3"/>
-      <c r="AS9" s="3"/>
+      <c r="AR9" s="11"/>
+      <c r="AS9" s="11"/>
       <c r="AT9" s="3"/>
       <c r="AU9" s="3"/>
       <c r="AV9" s="3"/>
@@ -1898,8 +2002,10 @@
       <c r="AY9" s="3"/>
       <c r="AZ9" s="3"/>
       <c r="BA9" s="3"/>
+      <c r="BB9" s="3"/>
+      <c r="BC9" s="3"/>
     </row>
-    <row r="10" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>122</v>
       </c>
@@ -1954,19 +2060,19 @@
       <c r="AH10" s="6"/>
       <c r="AI10" s="6"/>
       <c r="AJ10" s="6"/>
-      <c r="AK10" s="6"/>
-      <c r="AL10" s="6"/>
+      <c r="AK10" s="24"/>
+      <c r="AL10" s="24"/>
       <c r="AM10" s="6"/>
       <c r="AN10" s="6"/>
-      <c r="AO10" s="13" t="s">
+      <c r="AO10" s="6"/>
+      <c r="AP10" s="6"/>
+      <c r="AQ10" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="AP10" s="18"/>
-      <c r="AQ10" s="13" t="s">
+      <c r="AR10" s="18"/>
+      <c r="AS10" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="AR10" s="6"/>
-      <c r="AS10" s="6"/>
       <c r="AT10" s="6"/>
       <c r="AU10" s="6"/>
       <c r="AV10" s="6"/>
@@ -1974,11 +2080,13 @@
       <c r="AX10" s="6"/>
       <c r="AY10" s="6"/>
       <c r="AZ10" s="6"/>
-      <c r="BA10" s="6" t="s">
+      <c r="BA10" s="6"/>
+      <c r="BB10" s="6"/>
+      <c r="BC10" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>152</v>
       </c>
@@ -2003,41 +2111,43 @@
       <c r="S11" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="AO11" s="14" t="s">
+      <c r="AK11" s="21"/>
+      <c r="AL11" s="21"/>
+      <c r="AQ11" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="AP11" s="16">
+      <c r="AR11" s="16">
         <v>42581</v>
       </c>
-      <c r="AQ11" s="14" t="s">
+      <c r="AS11" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="AR11" s="4" t="s">
+      <c r="AT11" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AS11" s="4" t="s">
+      <c r="AU11" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AT11" s="4" t="s">
+      <c r="AV11" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AV11" s="4" t="s">
+      <c r="AX11" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="AW11" s="8" t="s">
+      <c r="AY11" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="AX11" s="8" t="s">
+      <c r="AZ11" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="BA11" s="9" t="s">
+      <c r="BC11" s="9" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AJ4" r:id="rId1"/>
-    <hyperlink ref="AN5" r:id="rId2"/>
+    <hyperlink ref="AP5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
rename AV_FILE to AV_FILE_PATH
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -420,9 +420,6 @@
     <t>GROUP_ACCESS</t>
   </si>
   <si>
-    <t>AV_FILE</t>
-  </si>
-  <si>
     <t>AV_SUBTITLES</t>
   </si>
   <si>
@@ -580,6 +577,9 @@
   </si>
   <si>
     <t>RESTRICTED_REQUEST</t>
+  </si>
+  <si>
+    <t>AV_FILE_PATH</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1117,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="AP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BA2" sqref="BA2:BC2"/>
+      <selection pane="bottomRight" activeCell="BA2" sqref="BA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1276,7 +1276,7 @@
         <v>31</v>
       </c>
       <c r="AG1" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AH1" s="3" t="s">
         <v>32</v>
@@ -1288,10 +1288,10 @@
         <v>34</v>
       </c>
       <c r="AK1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AL1" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="AM1" s="3" t="s">
         <v>35</v>
@@ -1315,13 +1315,13 @@
         <v>41</v>
       </c>
       <c r="AT1" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="AU1" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="AU1" s="27" t="s">
+      <c r="AV1" s="27" t="s">
         <v>166</v>
-      </c>
-      <c r="AV1" s="27" t="s">
-        <v>167</v>
       </c>
       <c r="AW1" s="3" t="s">
         <v>75</v>
@@ -1333,16 +1333,16 @@
         <v>77</v>
       </c>
       <c r="AZ1" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BA1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="BB1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="BB1" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="BC1" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="BD1" s="3" t="s">
         <v>42</v>
@@ -1441,16 +1441,16 @@
         <v>42946</v>
       </c>
       <c r="AL2" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AM2" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AN2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="AO2" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="AO2" s="4" t="s">
-        <v>137</v>
       </c>
       <c r="AP2" s="4" t="s">
         <v>113</v>
@@ -1465,13 +1465,13 @@
         <v>60</v>
       </c>
       <c r="AT2" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AU2" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AV2" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AW2" s="4" t="s">
         <v>78</v>
@@ -1483,16 +1483,16 @@
         <v>80</v>
       </c>
       <c r="AZ2" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BA2" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BB2" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BC2" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BD2" s="4" t="s">
         <v>81</v>
@@ -1566,7 +1566,7 @@
         <v>6663</v>
       </c>
       <c r="AG3" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AH3" s="4" t="s">
         <v>107</v>
@@ -1579,38 +1579,38 @@
         <v>42947</v>
       </c>
       <c r="AL3" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AM3" s="4"/>
       <c r="AN3" s="4" t="s">
         <v>69</v>
       </c>
       <c r="AO3" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AP3" s="4"/>
       <c r="AQ3" s="12"/>
       <c r="AR3" s="12"/>
       <c r="AS3" s="12"/>
       <c r="AT3" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AU3" s="28"/>
       <c r="AV3" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AW3" s="4"/>
       <c r="AX3" s="4"/>
       <c r="AY3" s="4"/>
       <c r="AZ3" s="4"/>
       <c r="BA3" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BB3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="BC3" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="BD3" s="4"/>
     </row>
@@ -1665,7 +1665,7 @@
       <c r="AL4" s="22"/>
       <c r="AM4" s="3"/>
       <c r="AN4" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3"/>
@@ -1752,14 +1752,14 @@
         <v>42948</v>
       </c>
       <c r="AL5" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AM5" s="4"/>
       <c r="AN5" s="4" t="s">
         <v>70</v>
       </c>
       <c r="AO5" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AP5" s="1" t="s">
         <v>112</v>
@@ -1772,13 +1772,13 @@
         <v>60</v>
       </c>
       <c r="AT5" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="AU5" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="AU5" s="28" t="s">
+      <c r="AV5" s="28" t="s">
         <v>170</v>
-      </c>
-      <c r="AV5" s="28" t="s">
-        <v>171</v>
       </c>
       <c r="AW5" s="4"/>
       <c r="AX5" s="4"/>
@@ -1846,10 +1846,10 @@
       <c r="AD6" s="4"/>
       <c r="AE6" s="4"/>
       <c r="AF6" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AG6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AH6" s="4"/>
       <c r="AI6" s="4"/>
@@ -1863,7 +1863,7 @@
         <v>69</v>
       </c>
       <c r="AO6" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AP6" s="4"/>
       <c r="AQ6" s="12" t="s">
@@ -2001,7 +2001,7 @@
         <v>42949</v>
       </c>
       <c r="AL8" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AM8" s="4"/>
       <c r="AN8" s="4"/>
@@ -2092,23 +2092,23 @@
     </row>
     <row r="10" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>120</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>121</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -2120,14 +2120,14 @@
         <v>42581</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R10" s="6"/>
       <c r="S10" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="T10" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="T10" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
@@ -2156,7 +2156,7 @@
       </c>
       <c r="AR10" s="18"/>
       <c r="AS10" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AT10" s="29"/>
       <c r="AU10" s="29"/>
@@ -2174,33 +2174,33 @@
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P11" s="16">
         <v>42582</v>
       </c>
       <c r="S11" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AK11" s="21"/>
       <c r="AL11" s="21"/>
       <c r="AQ11" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AR11" s="16">
         <v>42581</v>
@@ -2209,10 +2209,10 @@
         <v>60</v>
       </c>
       <c r="AT11" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AU11" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AV11" s="30"/>
       <c r="AW11" s="4" t="s">
@@ -2225,7 +2225,7 @@
         <v>80</v>
       </c>
       <c r="AZ11" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BA11" s="8"/>
       <c r="BD11" s="9" t="s">

</xml_diff>

<commit_message>
EASY-1318 - relation with link
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="174">
   <si>
     <t>DATASET</t>
   </si>
@@ -580,6 +580,12 @@
   </si>
   <si>
     <t>AV_FILE_PATH</t>
+  </si>
+  <si>
+    <t>foobar</t>
+  </si>
+  <si>
+    <t>isVersionOf</t>
   </si>
 </sst>
 </file>
@@ -590,7 +596,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="00000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -623,14 +629,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -701,9 +699,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -757,7 +764,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -787,8 +793,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -835,6 +842,15 @@
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1114,10 +1130,10 @@
   <dimension ref="A1:BD11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AP2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BA2" sqref="BA2"/>
+      <selection pane="bottomRight" activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1179,31 +1195,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -1224,7 +1240,7 @@
       <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
@@ -1233,7 +1249,7 @@
       <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="S1" s="10" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="3" t="s">
@@ -1305,22 +1321,22 @@
       <c r="AP1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="11" t="s">
+      <c r="AQ1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AR1" s="11" t="s">
+      <c r="AR1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AS1" s="11" t="s">
+      <c r="AS1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="AT1" s="27" t="s">
+      <c r="AT1" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="AU1" s="27" t="s">
+      <c r="AU1" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="AV1" s="27" t="s">
+      <c r="AV1" s="26" t="s">
         <v>166</v>
       </c>
       <c r="AW1" s="3" t="s">
@@ -1349,27 +1365,27 @@
       </c>
     </row>
     <row r="2" spans="1:56" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12" t="s">
+      <c r="H2" s="11"/>
+      <c r="I2" s="11" t="s">
         <v>62</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -1388,7 +1404,7 @@
       <c r="O2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="P2" s="16">
+      <c r="P2" s="15">
         <v>42143</v>
       </c>
       <c r="Q2" s="4" t="s">
@@ -1397,7 +1413,7 @@
       <c r="R2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="S2" s="19" t="s">
+      <c r="S2" s="18" t="s">
         <v>56</v>
       </c>
       <c r="T2" s="4" t="s">
@@ -1436,11 +1452,13 @@
       <c r="AI2" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="25">
+      <c r="AJ2" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="AK2" s="24">
         <v>42946</v>
       </c>
-      <c r="AL2" s="21" t="s">
+      <c r="AL2" s="20" t="s">
         <v>160</v>
       </c>
       <c r="AM2" s="4" t="s">
@@ -1455,13 +1473,13 @@
       <c r="AP2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="AQ2" s="12" t="s">
+      <c r="AQ2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR2" s="16">
+      <c r="AR2" s="15">
         <v>33815</v>
       </c>
-      <c r="AS2" s="12" t="s">
+      <c r="AS2" s="11" t="s">
         <v>60</v>
       </c>
       <c r="AT2" s="4" t="s">
@@ -1499,19 +1517,19 @@
       </c>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
         <v>89</v>
@@ -1524,14 +1542,14 @@
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="16"/>
+      <c r="P3" s="15"/>
       <c r="Q3" s="4" t="s">
         <v>93</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="11" t="s">
         <v>57</v>
       </c>
       <c r="T3" s="4" t="s">
@@ -1575,7 +1593,7 @@
         <v>109</v>
       </c>
       <c r="AJ3" s="4"/>
-      <c r="AK3" s="25">
+      <c r="AK3" s="24">
         <v>42947</v>
       </c>
       <c r="AL3" s="4" t="s">
@@ -1589,14 +1607,14 @@
         <v>137</v>
       </c>
       <c r="AP3" s="4"/>
-      <c r="AQ3" s="12"/>
-      <c r="AR3" s="12"/>
-      <c r="AS3" s="12"/>
-      <c r="AT3" s="28" t="s">
+      <c r="AQ3" s="11"/>
+      <c r="AR3" s="11"/>
+      <c r="AS3" s="11"/>
+      <c r="AT3" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="AU3" s="28"/>
-      <c r="AV3" s="28" t="s">
+      <c r="AU3" s="27"/>
+      <c r="AV3" s="27" t="s">
         <v>133</v>
       </c>
       <c r="AW3" s="4"/>
@@ -1615,29 +1633,29 @@
       <c r="BD3" s="4"/>
     </row>
     <row r="4" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="17"/>
+      <c r="P4" s="16"/>
       <c r="Q4" s="3" t="s">
         <v>94</v>
       </c>
       <c r="R4" s="3"/>
-      <c r="S4" s="20"/>
+      <c r="S4" s="19"/>
       <c r="T4" s="3" t="s">
         <v>66</v>
       </c>
@@ -1661,49 +1679,49 @@
       <c r="AJ4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AK4" s="22"/>
-      <c r="AL4" s="22"/>
+      <c r="AK4" s="21"/>
+      <c r="AL4" s="21"/>
       <c r="AM4" s="3"/>
       <c r="AN4" s="3" t="s">
         <v>128</v>
       </c>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3"/>
-      <c r="AQ4" s="11"/>
-      <c r="AR4" s="11"/>
-      <c r="AS4" s="11"/>
-      <c r="AT4" s="27"/>
-      <c r="AU4" s="27"/>
-      <c r="AV4" s="27"/>
+      <c r="AQ4" s="10"/>
+      <c r="AR4" s="10"/>
+      <c r="AS4" s="10"/>
+      <c r="AT4" s="26"/>
+      <c r="AU4" s="26"/>
+      <c r="AV4" s="26"/>
       <c r="AW4" s="3"/>
       <c r="AX4" s="3"/>
       <c r="AY4" s="3"/>
       <c r="AZ4" s="3"/>
-      <c r="BA4" s="7"/>
+      <c r="BA4" s="6"/>
       <c r="BB4" s="3"/>
       <c r="BC4" s="3"/>
       <c r="BD4" s="3"/>
     </row>
     <row r="5" spans="1:56" ht="96" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12" t="s">
+      <c r="H5" s="11"/>
+      <c r="I5" s="11" t="s">
         <v>63</v>
       </c>
       <c r="J5" s="4"/>
@@ -1712,14 +1730,14 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="16">
+      <c r="P5" s="15">
         <v>42137</v>
       </c>
       <c r="Q5" s="4" t="s">
         <v>95</v>
       </c>
       <c r="R5" s="4"/>
-      <c r="S5" s="19" t="s">
+      <c r="S5" s="18" t="s">
         <v>58</v>
       </c>
       <c r="T5" s="4" t="s">
@@ -1742,16 +1760,17 @@
         <v>105</v>
       </c>
       <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
-      <c r="AI5" s="4" t="s">
+      <c r="AH5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="AJ5" s="4"/>
-      <c r="AK5" s="26">
+      <c r="AK5" s="25">
         <f>AK3+DAY(1)</f>
         <v>42948</v>
       </c>
-      <c r="AL5" s="21" t="s">
+      <c r="AL5" s="20" t="s">
         <v>162</v>
       </c>
       <c r="AM5" s="4"/>
@@ -1764,20 +1783,20 @@
       <c r="AP5" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AQ5" s="12" t="s">
+      <c r="AQ5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR5" s="16"/>
-      <c r="AS5" s="12" t="s">
+      <c r="AR5" s="15"/>
+      <c r="AS5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AT5" s="28" t="s">
+      <c r="AT5" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="AU5" s="28" t="s">
+      <c r="AU5" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="AV5" s="28" t="s">
+      <c r="AV5" s="27" t="s">
         <v>170</v>
       </c>
       <c r="AW5" s="4"/>
@@ -1792,27 +1811,27 @@
       </c>
     </row>
     <row r="6" spans="1:56" ht="96" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>85</v>
       </c>
       <c r="J6" s="4"/>
@@ -1821,14 +1840,14 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="16">
+      <c r="P6" s="15">
         <v>42137</v>
       </c>
       <c r="Q6" s="4" t="s">
         <v>96</v>
       </c>
       <c r="R6" s="4"/>
-      <c r="S6" s="19" t="s">
+      <c r="S6" s="18" t="s">
         <v>59</v>
       </c>
       <c r="T6" s="4" t="s">
@@ -1854,10 +1873,10 @@
       <c r="AH6" s="4"/>
       <c r="AI6" s="4"/>
       <c r="AJ6" s="4"/>
-      <c r="AK6" s="26" t="s">
+      <c r="AK6" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="AL6" s="21"/>
+      <c r="AL6" s="20"/>
       <c r="AM6" s="4"/>
       <c r="AN6" s="4" t="s">
         <v>69</v>
@@ -1866,14 +1885,14 @@
         <v>139</v>
       </c>
       <c r="AP6" s="4"/>
-      <c r="AQ6" s="12" t="s">
+      <c r="AQ6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR6" s="12"/>
-      <c r="AS6" s="12"/>
-      <c r="AT6" s="28"/>
-      <c r="AU6" s="28"/>
-      <c r="AV6" s="28"/>
+      <c r="AR6" s="11"/>
+      <c r="AS6" s="11"/>
+      <c r="AT6" s="27"/>
+      <c r="AU6" s="27"/>
+      <c r="AV6" s="27"/>
       <c r="AW6" s="4"/>
       <c r="AX6" s="4"/>
       <c r="AY6" s="4"/>
@@ -1886,31 +1905,31 @@
       </c>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="16">
+      <c r="P7" s="15">
         <v>42137</v>
       </c>
       <c r="Q7" s="4" t="s">
         <v>97</v>
       </c>
       <c r="R7" s="4"/>
-      <c r="S7" s="12"/>
+      <c r="S7" s="11"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
@@ -1928,20 +1947,20 @@
       <c r="AH7" s="4"/>
       <c r="AI7" s="4"/>
       <c r="AJ7" s="4"/>
-      <c r="AK7" s="21"/>
-      <c r="AL7" s="21"/>
+      <c r="AK7" s="20"/>
+      <c r="AL7" s="20"/>
       <c r="AM7" s="4"/>
       <c r="AN7" s="4"/>
       <c r="AO7" s="4"/>
       <c r="AP7" s="4"/>
-      <c r="AQ7" s="12" t="s">
+      <c r="AQ7" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR7" s="12"/>
-      <c r="AS7" s="12"/>
-      <c r="AT7" s="28"/>
-      <c r="AU7" s="28"/>
-      <c r="AV7" s="28"/>
+      <c r="AR7" s="11"/>
+      <c r="AS7" s="11"/>
+      <c r="AT7" s="27"/>
+      <c r="AU7" s="27"/>
+      <c r="AV7" s="27"/>
       <c r="AW7" s="4"/>
       <c r="AX7" s="4"/>
       <c r="AY7" s="4"/>
@@ -1954,31 +1973,31 @@
       </c>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="16">
+      <c r="P8" s="15">
         <v>42137</v>
       </c>
       <c r="Q8" s="4" t="s">
         <v>98</v>
       </c>
       <c r="R8" s="4"/>
-      <c r="S8" s="12"/>
+      <c r="S8" s="11"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
@@ -1996,25 +2015,25 @@
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
       <c r="AJ8" s="4"/>
-      <c r="AK8" s="26">
+      <c r="AK8" s="25">
         <f>AK5+DAY(1)</f>
         <v>42949</v>
       </c>
-      <c r="AL8" s="21" t="s">
+      <c r="AL8" s="20" t="s">
         <v>163</v>
       </c>
       <c r="AM8" s="4"/>
       <c r="AN8" s="4"/>
       <c r="AO8" s="4"/>
       <c r="AP8" s="4"/>
-      <c r="AQ8" s="12" t="s">
+      <c r="AQ8" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR8" s="12"/>
-      <c r="AS8" s="12"/>
-      <c r="AT8" s="28"/>
-      <c r="AU8" s="28"/>
-      <c r="AV8" s="28"/>
+      <c r="AR8" s="11"/>
+      <c r="AS8" s="11"/>
+      <c r="AT8" s="27"/>
+      <c r="AU8" s="27"/>
+      <c r="AV8" s="27"/>
       <c r="AW8" s="4"/>
       <c r="AX8" s="4"/>
       <c r="AY8" s="4"/>
@@ -2025,31 +2044,31 @@
       <c r="BD8" s="4"/>
     </row>
     <row r="9" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="17">
+      <c r="P9" s="16">
         <v>42137</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>99</v>
       </c>
       <c r="R9" s="3"/>
-      <c r="S9" s="11"/>
+      <c r="S9" s="10"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
@@ -2067,20 +2086,20 @@
       <c r="AH9" s="3"/>
       <c r="AI9" s="3"/>
       <c r="AJ9" s="3"/>
-      <c r="AK9" s="23"/>
-      <c r="AL9" s="23"/>
+      <c r="AK9" s="22"/>
+      <c r="AL9" s="22"/>
       <c r="AM9" s="3"/>
       <c r="AN9" s="3"/>
       <c r="AO9" s="3"/>
       <c r="AP9" s="3"/>
-      <c r="AQ9" s="11" t="s">
+      <c r="AQ9" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AR9" s="11"/>
-      <c r="AS9" s="11"/>
-      <c r="AT9" s="27"/>
-      <c r="AU9" s="27"/>
-      <c r="AV9" s="27"/>
+      <c r="AR9" s="10"/>
+      <c r="AS9" s="10"/>
+      <c r="AT9" s="26"/>
+      <c r="AU9" s="26"/>
+      <c r="AV9" s="26"/>
       <c r="AW9" s="3"/>
       <c r="AX9" s="3"/>
       <c r="AY9" s="3"/>
@@ -2091,130 +2110,130 @@
       <c r="BD9" s="3"/>
     </row>
     <row r="10" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13" t="s">
+      <c r="F10" s="12"/>
+      <c r="G10" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13" t="s">
+      <c r="H10" s="12"/>
+      <c r="I10" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="18">
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="17">
         <v>42581</v>
       </c>
-      <c r="Q10" s="6" t="s">
+      <c r="Q10" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="R10" s="6"/>
-      <c r="S10" s="13" t="s">
+      <c r="R10" s="5"/>
+      <c r="S10" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="T10" s="6" t="s">
+      <c r="T10" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="6"/>
-      <c r="AD10" s="6"/>
-      <c r="AE10" s="6"/>
-      <c r="AF10" s="6"/>
-      <c r="AG10" s="6"/>
-      <c r="AH10" s="6"/>
-      <c r="AI10" s="6"/>
-      <c r="AJ10" s="6"/>
-      <c r="AK10" s="24"/>
-      <c r="AL10" s="24"/>
-      <c r="AM10" s="6"/>
-      <c r="AN10" s="6"/>
-      <c r="AO10" s="6"/>
-      <c r="AP10" s="6"/>
-      <c r="AQ10" s="13" t="s">
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="5"/>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="23"/>
+      <c r="AL10" s="23"/>
+      <c r="AM10" s="5"/>
+      <c r="AN10" s="5"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="5"/>
+      <c r="AQ10" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="AR10" s="18"/>
-      <c r="AS10" s="13" t="s">
+      <c r="AR10" s="17"/>
+      <c r="AS10" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="AT10" s="29"/>
-      <c r="AU10" s="29"/>
-      <c r="AV10" s="29"/>
-      <c r="AW10" s="6"/>
-      <c r="AX10" s="6"/>
-      <c r="AY10" s="6"/>
-      <c r="AZ10" s="6"/>
-      <c r="BA10" s="6"/>
-      <c r="BB10" s="6"/>
-      <c r="BC10" s="6"/>
-      <c r="BD10" s="6" t="s">
+      <c r="AT10" s="28"/>
+      <c r="AU10" s="28"/>
+      <c r="AV10" s="28"/>
+      <c r="AW10" s="5"/>
+      <c r="AX10" s="5"/>
+      <c r="AY10" s="5"/>
+      <c r="AZ10" s="5"/>
+      <c r="BA10" s="5"/>
+      <c r="BB10" s="5"/>
+      <c r="BC10" s="5"/>
+      <c r="BD10" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14" t="s">
+      <c r="F11" s="13"/>
+      <c r="G11" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14" t="s">
+      <c r="H11" s="13"/>
+      <c r="I11" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="P11" s="16">
+      <c r="P11" s="15">
         <v>42582</v>
       </c>
-      <c r="S11" s="14" t="s">
+      <c r="S11" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="AK11" s="21"/>
-      <c r="AL11" s="21"/>
-      <c r="AQ11" s="14" t="s">
+      <c r="AK11" s="20"/>
+      <c r="AL11" s="20"/>
+      <c r="AQ11" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="AR11" s="16">
+      <c r="AR11" s="15">
         <v>42581</v>
       </c>
-      <c r="AS11" s="14" t="s">
+      <c r="AS11" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AT11" s="8" t="s">
+      <c r="AT11" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="AU11" s="8" t="s">
+      <c r="AU11" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="AV11" s="30"/>
+      <c r="AV11" s="29"/>
       <c r="AW11" s="4" t="s">
         <v>78</v>
       </c>
@@ -2227,8 +2246,8 @@
       <c r="AZ11" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="BA11" s="8"/>
-      <c r="BD11" s="9" t="s">
+      <c r="BA11" s="7"/>
+      <c r="BD11" s="8" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EASY-1329 and EASY-1318 (#88)
* EASY-1329: Refine accessRights of files within a dataset for easy-split-multi-deposit	
* rename AV_FILE to AV_FILE_PATH
* documentation
* EASY-1318: relation with href link
* relation qualifier
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BB$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BC$9</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="174">
   <si>
     <t>DATASET</t>
   </si>
@@ -417,21 +417,12 @@
     <t>degrees</t>
   </si>
   <si>
-    <t>SF_ACCESSIBILITY</t>
-  </si>
-  <si>
     <t>GROUP_ACCESS</t>
   </si>
   <si>
-    <t>AV_FILE</t>
-  </si>
-  <si>
     <t>AV_SUBTITLES</t>
   </si>
   <si>
-    <t>AV_FILE_TITLE</t>
-  </si>
-  <si>
     <t>ruimtereis03</t>
   </si>
   <si>
@@ -565,6 +556,36 @@
   </si>
   <si>
     <t>Date Copyrighted</t>
+  </si>
+  <si>
+    <t>FILE_PATH</t>
+  </si>
+  <si>
+    <t>FILE_TITLE</t>
+  </si>
+  <si>
+    <t>FILE_ACCESSIBILITY</t>
+  </si>
+  <si>
+    <t>path/to/a/random/video/hubble.mpg</t>
+  </si>
+  <si>
+    <t>path/to/images/Hubble_01.jpg</t>
+  </si>
+  <si>
+    <t>Hubble</t>
+  </si>
+  <si>
+    <t>RESTRICTED_REQUEST</t>
+  </si>
+  <si>
+    <t>AV_FILE_PATH</t>
+  </si>
+  <si>
+    <t>foobar</t>
+  </si>
+  <si>
+    <t>isVersionOf</t>
   </si>
 </sst>
 </file>
@@ -575,7 +596,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="00000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -608,14 +629,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -686,7 +699,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -714,14 +727,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -747,8 +789,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -774,6 +821,36 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1050,13 +1127,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC11"/>
+  <dimension ref="A1:BD11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL1" sqref="AL1"/>
+      <selection pane="bottomRight" activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,43 +1182,44 @@
     <col min="43" max="43" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="17.83203125" customWidth="1"/>
-    <col min="51" max="51" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="23" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="33" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -1162,7 +1240,7 @@
       <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
@@ -1171,7 +1249,7 @@
       <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="S1" s="10" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="3" t="s">
@@ -1214,7 +1292,7 @@
         <v>31</v>
       </c>
       <c r="AG1" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AH1" s="3" t="s">
         <v>32</v>
@@ -1226,10 +1304,10 @@
         <v>34</v>
       </c>
       <c r="AK1" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="AL1" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AM1" s="3" t="s">
         <v>35</v>
@@ -1243,68 +1321,71 @@
       <c r="AP1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="11" t="s">
+      <c r="AQ1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AR1" s="11" t="s">
+      <c r="AR1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AS1" s="11" t="s">
+      <c r="AS1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AT1" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="AU1" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="AV1" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="AW1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AW1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AX1" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="AY1" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="AZ1" s="3" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="BA1" s="3" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="BB1" s="3" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="BC1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="BD1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:56" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12" t="s">
+      <c r="H2" s="11"/>
+      <c r="I2" s="11" t="s">
         <v>62</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -1323,7 +1404,7 @@
       <c r="O2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="P2" s="16">
+      <c r="P2" s="15">
         <v>42143</v>
       </c>
       <c r="Q2" s="4" t="s">
@@ -1332,7 +1413,7 @@
       <c r="R2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="S2" s="19" t="s">
+      <c r="S2" s="18" t="s">
         <v>56</v>
       </c>
       <c r="T2" s="4" t="s">
@@ -1371,79 +1452,84 @@
       <c r="AI2" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="25">
+      <c r="AJ2" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="AK2" s="24">
         <v>42946</v>
       </c>
-      <c r="AL2" s="21" t="s">
-        <v>163</v>
+      <c r="AL2" s="20" t="s">
+        <v>160</v>
       </c>
       <c r="AM2" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AN2" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="AO2" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AP2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="AQ2" s="12" t="s">
+      <c r="AQ2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR2" s="16">
+      <c r="AR2" s="15">
         <v>33815</v>
       </c>
-      <c r="AS2" s="12" t="s">
+      <c r="AS2" s="11" t="s">
         <v>60</v>
       </c>
       <c r="AT2" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="AU2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="AW2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AW2" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="AX2" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="BA2" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="BB2" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="AZ2" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="BA2" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="BB2" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="BC2" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="BD2" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
         <v>89</v>
@@ -1456,14 +1542,14 @@
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="16"/>
+      <c r="P3" s="15"/>
       <c r="Q3" s="4" t="s">
         <v>93</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="11" t="s">
         <v>57</v>
       </c>
       <c r="T3" s="4" t="s">
@@ -1498,7 +1584,7 @@
         <v>6663</v>
       </c>
       <c r="AG3" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AH3" s="4" t="s">
         <v>107</v>
@@ -1507,64 +1593,69 @@
         <v>109</v>
       </c>
       <c r="AJ3" s="4"/>
-      <c r="AK3" s="25">
+      <c r="AK3" s="24">
         <v>42947</v>
       </c>
       <c r="AL3" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="AM3" s="4"/>
       <c r="AN3" s="4" t="s">
         <v>69</v>
       </c>
       <c r="AO3" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AP3" s="4"/>
-      <c r="AQ3" s="12"/>
-      <c r="AR3" s="12"/>
-      <c r="AS3" s="12"/>
-      <c r="AT3" s="4"/>
-      <c r="AU3" s="4"/>
-      <c r="AV3" s="4"/>
+      <c r="AQ3" s="11"/>
+      <c r="AR3" s="11"/>
+      <c r="AS3" s="11"/>
+      <c r="AT3" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="AU3" s="27"/>
+      <c r="AV3" s="27" t="s">
+        <v>133</v>
+      </c>
       <c r="AW3" s="4"/>
       <c r="AX3" s="4"/>
-      <c r="AY3" s="4" t="s">
-        <v>148</v>
-      </c>
+      <c r="AY3" s="4"/>
       <c r="AZ3" s="4"/>
       <c r="BA3" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="BB3" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="BC3" s="4"/>
+        <v>147</v>
+      </c>
+      <c r="BC3" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="BD3" s="4"/>
     </row>
-    <row r="4" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="17"/>
+      <c r="P4" s="16"/>
       <c r="Q4" s="3" t="s">
         <v>94</v>
       </c>
       <c r="R4" s="3"/>
-      <c r="S4" s="20"/>
+      <c r="S4" s="19"/>
       <c r="T4" s="3" t="s">
         <v>66</v>
       </c>
@@ -1588,48 +1679,49 @@
       <c r="AJ4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AK4" s="22"/>
-      <c r="AL4" s="22"/>
+      <c r="AK4" s="21"/>
+      <c r="AL4" s="21"/>
       <c r="AM4" s="3"/>
       <c r="AN4" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3"/>
-      <c r="AQ4" s="11"/>
-      <c r="AR4" s="11"/>
-      <c r="AS4" s="11"/>
-      <c r="AT4" s="3"/>
-      <c r="AU4" s="3"/>
-      <c r="AV4" s="3"/>
+      <c r="AQ4" s="10"/>
+      <c r="AR4" s="10"/>
+      <c r="AS4" s="10"/>
+      <c r="AT4" s="26"/>
+      <c r="AU4" s="26"/>
+      <c r="AV4" s="26"/>
       <c r="AW4" s="3"/>
       <c r="AX4" s="3"/>
-      <c r="AY4" s="7"/>
-      <c r="AZ4" s="7"/>
-      <c r="BA4" s="3"/>
+      <c r="AY4" s="3"/>
+      <c r="AZ4" s="3"/>
+      <c r="BA4" s="6"/>
       <c r="BB4" s="3"/>
       <c r="BC4" s="3"/>
+      <c r="BD4" s="3"/>
     </row>
-    <row r="5" spans="1:55" ht="96" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:56" ht="96" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12" t="s">
+      <c r="H5" s="11"/>
+      <c r="I5" s="11" t="s">
         <v>63</v>
       </c>
       <c r="J5" s="4"/>
@@ -1638,14 +1730,14 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="16">
+      <c r="P5" s="15">
         <v>42137</v>
       </c>
       <c r="Q5" s="4" t="s">
         <v>95</v>
       </c>
       <c r="R5" s="4"/>
-      <c r="S5" s="19" t="s">
+      <c r="S5" s="18" t="s">
         <v>58</v>
       </c>
       <c r="T5" s="4" t="s">
@@ -1668,70 +1760,78 @@
         <v>105</v>
       </c>
       <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
-      <c r="AI5" s="4" t="s">
+      <c r="AH5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="AJ5" s="4"/>
-      <c r="AK5" s="26">
+      <c r="AK5" s="25">
         <f>AK3+DAY(1)</f>
         <v>42948</v>
       </c>
-      <c r="AL5" s="21" t="s">
-        <v>165</v>
+      <c r="AL5" s="20" t="s">
+        <v>162</v>
       </c>
       <c r="AM5" s="4"/>
       <c r="AN5" s="4" t="s">
         <v>70</v>
       </c>
       <c r="AO5" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AP5" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AQ5" s="12" t="s">
+      <c r="AQ5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR5" s="16"/>
-      <c r="AS5" s="12" t="s">
+      <c r="AR5" s="15"/>
+      <c r="AS5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AT5" s="4"/>
-      <c r="AU5" s="4"/>
-      <c r="AV5" s="4"/>
+      <c r="AT5" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="AU5" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="AV5" s="27" t="s">
+        <v>170</v>
+      </c>
       <c r="AW5" s="4"/>
       <c r="AX5" s="4"/>
       <c r="AY5" s="4"/>
       <c r="AZ5" s="4"/>
       <c r="BA5" s="4"/>
       <c r="BB5" s="4"/>
-      <c r="BC5" s="4" t="s">
+      <c r="BC5" s="4"/>
+      <c r="BD5" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:55" ht="96" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:56" ht="96" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>85</v>
       </c>
       <c r="J6" s="4"/>
@@ -1740,14 +1840,14 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="16">
+      <c r="P6" s="15">
         <v>42137</v>
       </c>
       <c r="Q6" s="4" t="s">
         <v>96</v>
       </c>
       <c r="R6" s="4"/>
-      <c r="S6" s="19" t="s">
+      <c r="S6" s="18" t="s">
         <v>59</v>
       </c>
       <c r="T6" s="4" t="s">
@@ -1765,70 +1865,71 @@
       <c r="AD6" s="4"/>
       <c r="AE6" s="4"/>
       <c r="AF6" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AG6" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AH6" s="4"/>
       <c r="AI6" s="4"/>
       <c r="AJ6" s="4"/>
-      <c r="AK6" s="26" t="s">
+      <c r="AK6" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="AL6" s="21"/>
+      <c r="AL6" s="20"/>
       <c r="AM6" s="4"/>
       <c r="AN6" s="4" t="s">
         <v>69</v>
       </c>
       <c r="AO6" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="AP6" s="4"/>
-      <c r="AQ6" s="12" t="s">
+      <c r="AQ6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR6" s="12"/>
-      <c r="AS6" s="12"/>
-      <c r="AT6" s="4"/>
-      <c r="AU6" s="4"/>
-      <c r="AV6" s="4"/>
+      <c r="AR6" s="11"/>
+      <c r="AS6" s="11"/>
+      <c r="AT6" s="27"/>
+      <c r="AU6" s="27"/>
+      <c r="AV6" s="27"/>
       <c r="AW6" s="4"/>
       <c r="AX6" s="4"/>
       <c r="AY6" s="4"/>
       <c r="AZ6" s="4"/>
       <c r="BA6" s="4"/>
       <c r="BB6" s="4"/>
-      <c r="BC6" s="4" t="s">
+      <c r="BC6" s="4"/>
+      <c r="BD6" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="16">
+      <c r="P7" s="15">
         <v>42137</v>
       </c>
       <c r="Q7" s="4" t="s">
         <v>97</v>
       </c>
       <c r="R7" s="4"/>
-      <c r="S7" s="12"/>
+      <c r="S7" s="11"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
@@ -1846,56 +1947,57 @@
       <c r="AH7" s="4"/>
       <c r="AI7" s="4"/>
       <c r="AJ7" s="4"/>
-      <c r="AK7" s="21"/>
-      <c r="AL7" s="21"/>
+      <c r="AK7" s="20"/>
+      <c r="AL7" s="20"/>
       <c r="AM7" s="4"/>
       <c r="AN7" s="4"/>
       <c r="AO7" s="4"/>
       <c r="AP7" s="4"/>
-      <c r="AQ7" s="12" t="s">
+      <c r="AQ7" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR7" s="12"/>
-      <c r="AS7" s="12"/>
-      <c r="AT7" s="4"/>
-      <c r="AU7" s="4"/>
-      <c r="AV7" s="4"/>
+      <c r="AR7" s="11"/>
+      <c r="AS7" s="11"/>
+      <c r="AT7" s="27"/>
+      <c r="AU7" s="27"/>
+      <c r="AV7" s="27"/>
       <c r="AW7" s="4"/>
       <c r="AX7" s="4"/>
       <c r="AY7" s="4"/>
       <c r="AZ7" s="4"/>
       <c r="BA7" s="4"/>
       <c r="BB7" s="4"/>
-      <c r="BC7" s="4" t="s">
+      <c r="BC7" s="4"/>
+      <c r="BD7" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="16">
+      <c r="P8" s="15">
         <v>42137</v>
       </c>
       <c r="Q8" s="4" t="s">
         <v>98</v>
       </c>
       <c r="R8" s="4"/>
-      <c r="S8" s="12"/>
+      <c r="S8" s="11"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
@@ -1913,25 +2015,25 @@
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
       <c r="AJ8" s="4"/>
-      <c r="AK8" s="26">
+      <c r="AK8" s="25">
         <f>AK5+DAY(1)</f>
         <v>42949</v>
       </c>
-      <c r="AL8" s="21" t="s">
-        <v>166</v>
+      <c r="AL8" s="20" t="s">
+        <v>163</v>
       </c>
       <c r="AM8" s="4"/>
       <c r="AN8" s="4"/>
       <c r="AO8" s="4"/>
       <c r="AP8" s="4"/>
-      <c r="AQ8" s="12" t="s">
+      <c r="AQ8" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR8" s="12"/>
-      <c r="AS8" s="12"/>
-      <c r="AT8" s="4"/>
-      <c r="AU8" s="4"/>
-      <c r="AV8" s="4"/>
+      <c r="AR8" s="11"/>
+      <c r="AS8" s="11"/>
+      <c r="AT8" s="27"/>
+      <c r="AU8" s="27"/>
+      <c r="AV8" s="27"/>
       <c r="AW8" s="4"/>
       <c r="AX8" s="4"/>
       <c r="AY8" s="4"/>
@@ -1939,33 +2041,34 @@
       <c r="BA8" s="4"/>
       <c r="BB8" s="4"/>
       <c r="BC8" s="4"/>
+      <c r="BD8" s="4"/>
     </row>
-    <row r="9" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="17">
+      <c r="P9" s="16">
         <v>42137</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>99</v>
       </c>
       <c r="R9" s="3"/>
-      <c r="S9" s="11"/>
+      <c r="S9" s="10"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
@@ -1983,20 +2086,20 @@
       <c r="AH9" s="3"/>
       <c r="AI9" s="3"/>
       <c r="AJ9" s="3"/>
-      <c r="AK9" s="23"/>
-      <c r="AL9" s="23"/>
+      <c r="AK9" s="22"/>
+      <c r="AL9" s="22"/>
       <c r="AM9" s="3"/>
       <c r="AN9" s="3"/>
       <c r="AO9" s="3"/>
       <c r="AP9" s="3"/>
-      <c r="AQ9" s="11" t="s">
+      <c r="AQ9" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AR9" s="11"/>
-      <c r="AS9" s="11"/>
-      <c r="AT9" s="3"/>
-      <c r="AU9" s="3"/>
-      <c r="AV9" s="3"/>
+      <c r="AR9" s="10"/>
+      <c r="AS9" s="10"/>
+      <c r="AT9" s="26"/>
+      <c r="AU9" s="26"/>
+      <c r="AV9" s="26"/>
       <c r="AW9" s="3"/>
       <c r="AX9" s="3"/>
       <c r="AY9" s="3"/>
@@ -2004,143 +2107,147 @@
       <c r="BA9" s="3"/>
       <c r="BB9" s="3"/>
       <c r="BC9" s="3"/>
+      <c r="BD9" s="3"/>
     </row>
-    <row r="10" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="17">
+        <v>42581</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="R10" s="5"/>
+      <c r="S10" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="T10" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13" t="s">
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="5"/>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="23"/>
+      <c r="AL10" s="23"/>
+      <c r="AM10" s="5"/>
+      <c r="AN10" s="5"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="5"/>
+      <c r="AQ10" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR10" s="17"/>
+      <c r="AS10" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="AT10" s="28"/>
+      <c r="AU10" s="28"/>
+      <c r="AV10" s="28"/>
+      <c r="AW10" s="5"/>
+      <c r="AX10" s="5"/>
+      <c r="AY10" s="5"/>
+      <c r="AZ10" s="5"/>
+      <c r="BA10" s="5"/>
+      <c r="BB10" s="5"/>
+      <c r="BC10" s="5"/>
+      <c r="BD10" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="P11" s="15">
+        <v>42582</v>
+      </c>
+      <c r="S11" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK11" s="20"/>
+      <c r="AL11" s="20"/>
+      <c r="AQ11" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="AR11" s="15">
+        <v>42581</v>
+      </c>
+      <c r="AS11" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT11" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU11" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="18">
-        <v>42581</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="R10" s="6"/>
-      <c r="S10" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="T10" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="6"/>
-      <c r="AD10" s="6"/>
-      <c r="AE10" s="6"/>
-      <c r="AF10" s="6"/>
-      <c r="AG10" s="6"/>
-      <c r="AH10" s="6"/>
-      <c r="AI10" s="6"/>
-      <c r="AJ10" s="6"/>
-      <c r="AK10" s="24"/>
-      <c r="AL10" s="24"/>
-      <c r="AM10" s="6"/>
-      <c r="AN10" s="6"/>
-      <c r="AO10" s="6"/>
-      <c r="AP10" s="6"/>
-      <c r="AQ10" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="AR10" s="18"/>
-      <c r="AS10" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="AT10" s="6"/>
-      <c r="AU10" s="6"/>
-      <c r="AV10" s="6"/>
-      <c r="AW10" s="6"/>
-      <c r="AX10" s="6"/>
-      <c r="AY10" s="6"/>
-      <c r="AZ10" s="6"/>
-      <c r="BA10" s="6"/>
-      <c r="BB10" s="6"/>
-      <c r="BC10" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14" t="s">
+      <c r="AV11" s="29"/>
+      <c r="AW11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ11" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="P11" s="16">
-        <v>42582</v>
-      </c>
-      <c r="S11" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="AK11" s="21"/>
-      <c r="AL11" s="21"/>
-      <c r="AQ11" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="AR11" s="16">
-        <v>42581</v>
-      </c>
-      <c r="AS11" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="AT11" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AU11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AV11" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AX11" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="AY11" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AZ11" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="BC11" s="9" t="s">
+      <c r="BA11" s="7"/>
+      <c r="BD11" s="8" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make instructions.xslx in sync with instructions.csv
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linda/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="175">
   <si>
     <t>DATASET</t>
   </si>
@@ -586,6 +586,9 @@
   </si>
   <si>
     <t>isVersionOf</t>
+  </si>
+  <si>
+    <t>audio/mpeg3</t>
   </si>
 </sst>
 </file>
@@ -1130,10 +1133,10 @@
   <dimension ref="A1:BD11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH5" sqref="AH5"/>
+      <selection pane="bottomRight" activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2167,7 +2170,9 @@
       <c r="AK10" s="23"/>
       <c r="AL10" s="23"/>
       <c r="AM10" s="5"/>
-      <c r="AN10" s="5"/>
+      <c r="AN10" s="5" t="s">
+        <v>174</v>
+      </c>
       <c r="AO10" s="5"/>
       <c r="AP10" s="5"/>
       <c r="AQ10" s="12" t="s">

</xml_diff>

<commit_message>
Throw an error if a Link is provided, but no Title is given
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linda/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="177">
   <si>
     <t>DATASET</t>
   </si>
@@ -586,6 +586,15 @@
   </si>
   <si>
     <t>isVersionOf</t>
+  </si>
+  <si>
+    <t>audio/mpeg3</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>context</t>
   </si>
 </sst>
 </file>
@@ -1130,10 +1139,10 @@
   <dimension ref="A1:BD11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH5" sqref="AH5"/>
+      <selection pane="bottomRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1675,7 +1684,9 @@
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
       <c r="AH4" s="3"/>
-      <c r="AI4" s="3"/>
+      <c r="AI4" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="AJ4" s="2" t="s">
         <v>111</v>
       </c>
@@ -1762,6 +1773,9 @@
       <c r="AG5" s="4"/>
       <c r="AH5" s="4" t="s">
         <v>173</v>
+      </c>
+      <c r="AI5" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="AJ5" s="4" t="s">
         <v>110</v>
@@ -2218,6 +2232,9 @@
       </c>
       <c r="AK11" s="20"/>
       <c r="AL11" s="20"/>
+      <c r="AN11" t="s">
+        <v>174</v>
+      </c>
       <c r="AQ11" s="13" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
EASY-1324:  Throw an error if SF columns are available, but no AV format is specified (#92)
* Add new video/ and audio/ media types
* Rename formats.txt to acceptedMediaTypes.txt
* Throw an error if SF columns are available, but no AV format is specified
* Remove copied values of acceptedMediaTypes in BlackBox and debug-config
* Add unittests
* Document this DC_FORMAT requirement for AV deposits
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linda/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="175">
   <si>
     <t>DATASET</t>
   </si>
@@ -586,6 +586,9 @@
   </si>
   <si>
     <t>isVersionOf</t>
+  </si>
+  <si>
+    <t>audio/mpeg3</t>
   </si>
 </sst>
 </file>
@@ -1130,10 +1133,10 @@
   <dimension ref="A1:BD11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH5" sqref="AH5"/>
+      <selection pane="bottomRight" activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2167,7 +2170,9 @@
       <c r="AK10" s="23"/>
       <c r="AL10" s="23"/>
       <c r="AM10" s="5"/>
-      <c r="AN10" s="5"/>
+      <c r="AN10" s="5" t="s">
+        <v>174</v>
+      </c>
       <c r="AO10" s="5"/>
       <c r="AP10" s="5"/>
       <c r="AQ10" s="12" t="s">

</xml_diff>

<commit_message>
EASY-1356: Throw an error if a Link is provided, but no Title is given (#93)
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="177">
   <si>
     <t>DATASET</t>
   </si>
@@ -589,6 +589,12 @@
   </si>
   <si>
     <t>audio/mpeg3</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>context</t>
   </si>
 </sst>
 </file>
@@ -1133,10 +1139,10 @@
   <dimension ref="A1:BD11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AN12" sqref="AN12"/>
+      <selection pane="bottomRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1678,7 +1684,9 @@
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
       <c r="AH4" s="3"/>
-      <c r="AI4" s="3"/>
+      <c r="AI4" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="AJ4" s="2" t="s">
         <v>111</v>
       </c>
@@ -1765,6 +1773,9 @@
       <c r="AG5" s="4"/>
       <c r="AH5" s="4" t="s">
         <v>173</v>
+      </c>
+      <c r="AI5" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="AJ5" s="4" t="s">
         <v>110</v>
@@ -2170,9 +2181,7 @@
       <c r="AK10" s="23"/>
       <c r="AL10" s="23"/>
       <c r="AM10" s="5"/>
-      <c r="AN10" s="5" t="s">
-        <v>174</v>
-      </c>
+      <c r="AN10" s="5"/>
       <c r="AO10" s="5"/>
       <c r="AP10" s="5"/>
       <c r="AQ10" s="12" t="s">
@@ -2223,6 +2232,9 @@
       </c>
       <c r="AK11" s="20"/>
       <c r="AL11" s="20"/>
+      <c r="AN11" t="s">
+        <v>174</v>
+      </c>
       <c r="AQ11" s="13" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
add DCX_CREATOR_ROLE and DCX_CONTRIBUTOR_ROLE
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linda/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BC$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BE$9</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +35,7 @@
     <author>Richard van Heest</author>
   </authors>
   <commentList>
-    <comment ref="AR1" authorId="0">
+    <comment ref="AT1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="183">
   <si>
     <t>DATASET</t>
   </si>
@@ -595,6 +595,24 @@
   </si>
   <si>
     <t>context</t>
+  </si>
+  <si>
+    <t>DCX_CREATOR_ROLE</t>
+  </si>
+  <si>
+    <t>RegistrationAuthority</t>
+  </si>
+  <si>
+    <t>RightsHolder</t>
+  </si>
+  <si>
+    <t>ProjectManager</t>
+  </si>
+  <si>
+    <t>DCX_CONTRIBUTOR_ROLE</t>
+  </si>
+  <si>
+    <t>WorkPackageLeader</t>
   </si>
 </sst>
 </file>
@@ -708,9 +726,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -804,7 +852,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -860,6 +908,36 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1136,13 +1214,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD11"/>
+  <dimension ref="A1:BF11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI6" sqref="AI6"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1156,54 +1234,56 @@
     <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="50.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="65.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="33" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="14" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="33" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="23" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1231,149 +1311,155 @@
       <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="10" t="s">
+      <c r="AS1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AR1" s="10" t="s">
+      <c r="AT1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AS1" s="10" t="s">
+      <c r="AU1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="AT1" s="26" t="s">
+      <c r="AV1" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="AU1" s="26" t="s">
+      <c r="AW1" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="AV1" s="26" t="s">
+      <c r="AX1" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:56" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:58" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>43</v>
       </c>
@@ -1397,135 +1483,139 @@
       <c r="I2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="4"/>
+      <c r="N2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="P2" s="15">
+      <c r="Q2" s="4"/>
+      <c r="R2" s="15">
         <v>42143</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="S2" s="18" t="s">
+      <c r="U2" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4" t="s">
+      <c r="W2" s="4"/>
+      <c r="X2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="AB2" s="4">
         <v>83575.399999999994</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AC2" s="4">
         <v>455271.2</v>
       </c>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
       <c r="AD2" s="4"/>
       <c r="AE2" s="4"/>
-      <c r="AF2" s="4" t="s">
-        <v>104</v>
-      </c>
+      <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
       <c r="AH2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AJ2" s="30" t="s">
+      <c r="AL2" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="AK2" s="24">
+      <c r="AM2" s="24">
         <v>42946</v>
       </c>
-      <c r="AL2" s="20" t="s">
+      <c r="AN2" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="AQ2" s="11" t="s">
+      <c r="AS2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR2" s="15">
+      <c r="AT2" s="15">
         <v>33815</v>
       </c>
-      <c r="AS2" s="11" t="s">
+      <c r="AU2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="BA2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BB2" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="BA2" s="4" t="s">
+      <c r="BC2" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BD2" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BE2" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BF2" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>43</v>
       </c>
@@ -1539,109 +1629,113 @@
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4" t="s">
+      <c r="J3" s="11"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="15"/>
+      <c r="P3" s="4"/>
       <c r="Q3" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R3" s="15"/>
+      <c r="S3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="U3" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="V3" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="W3" s="4"/>
       <c r="X3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="AA3" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4">
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4">
         <v>1</v>
       </c>
-      <c r="AC3" s="4">
+      <c r="AE3" s="4">
         <v>2</v>
       </c>
-      <c r="AD3" s="4">
+      <c r="AF3" s="4">
         <v>3</v>
       </c>
-      <c r="AE3" s="4">
+      <c r="AG3" s="4">
         <v>4</v>
       </c>
-      <c r="AF3" s="4">
+      <c r="AH3" s="4">
         <v>6663</v>
       </c>
-      <c r="AG3" s="4" t="s">
+      <c r="AI3" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="AH3" s="4" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="AI3" s="4" t="s">
+      <c r="AK3" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="AJ3" s="4"/>
-      <c r="AK3" s="24">
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="24">
         <v>42947</v>
       </c>
-      <c r="AL3" s="4" t="s">
+      <c r="AN3" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="AM3" s="4"/>
-      <c r="AN3" s="4" t="s">
+      <c r="AO3" s="4"/>
+      <c r="AP3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AO3" s="4" t="s">
+      <c r="AQ3" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="AP3" s="4"/>
-      <c r="AQ3" s="11"/>
-      <c r="AR3" s="11"/>
+      <c r="AR3" s="4"/>
       <c r="AS3" s="11"/>
-      <c r="AT3" s="27" t="s">
+      <c r="AT3" s="11"/>
+      <c r="AU3" s="11"/>
+      <c r="AV3" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="AU3" s="27"/>
-      <c r="AV3" s="27" t="s">
+      <c r="AW3" s="27"/>
+      <c r="AX3" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="AW3" s="4"/>
-      <c r="AX3" s="4"/>
       <c r="AY3" s="4"/>
       <c r="AZ3" s="4"/>
-      <c r="BA3" s="4" t="s">
+      <c r="BA3" s="4"/>
+      <c r="BB3" s="4"/>
+      <c r="BC3" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="BB3" s="4" t="s">
+      <c r="BD3" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="BC3" s="4" t="s">
+      <c r="BE3" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="BD3" s="4"/>
+      <c r="BF3" s="4"/>
     </row>
-    <row r="4" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
@@ -1653,26 +1747,26 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="3"/>
+      <c r="J4" s="10"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="3" t="s">
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="R4" s="3"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="3" t="s">
+      <c r="T4" s="3"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
@@ -1684,36 +1778,38 @@
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
       <c r="AH4" s="3"/>
-      <c r="AI4" s="3" t="s">
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="AJ4" s="2" t="s">
+      <c r="AL4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AK4" s="21"/>
-      <c r="AL4" s="21"/>
-      <c r="AM4" s="3"/>
-      <c r="AN4" s="3" t="s">
+      <c r="AM4" s="21"/>
+      <c r="AN4" s="21"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="AO4" s="3"/>
-      <c r="AP4" s="3"/>
-      <c r="AQ4" s="10"/>
-      <c r="AR4" s="10"/>
+      <c r="AQ4" s="3"/>
+      <c r="AR4" s="3"/>
       <c r="AS4" s="10"/>
-      <c r="AT4" s="26"/>
-      <c r="AU4" s="26"/>
+      <c r="AT4" s="10"/>
+      <c r="AU4" s="10"/>
       <c r="AV4" s="26"/>
-      <c r="AW4" s="3"/>
-      <c r="AX4" s="3"/>
+      <c r="AW4" s="26"/>
+      <c r="AX4" s="26"/>
       <c r="AY4" s="3"/>
       <c r="AZ4" s="3"/>
-      <c r="BA4" s="6"/>
+      <c r="BA4" s="3"/>
       <c r="BB4" s="3"/>
-      <c r="BC4" s="3"/>
+      <c r="BC4" s="6"/>
       <c r="BD4" s="3"/>
+      <c r="BE4" s="3"/>
+      <c r="BF4" s="3"/>
     </row>
-    <row r="5" spans="1:56" ht="96" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:58" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>44</v>
       </c>
@@ -1735,31 +1831,33 @@
       <c r="I5" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="J5" s="4"/>
+      <c r="J5" s="11" t="s">
+        <v>179</v>
+      </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="15">
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="15">
         <v>42137</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="R5" s="4"/>
-      <c r="S5" s="18" t="s">
+      <c r="T5" s="4"/>
+      <c r="U5" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="V5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4" t="s">
+      <c r="W5" s="4"/>
+      <c r="X5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
@@ -1767,64 +1865,66 @@
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
-      <c r="AF5" s="4" t="s">
-        <v>105</v>
-      </c>
+      <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="AI5" s="8" t="s">
+      <c r="AK5" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="AJ5" s="4" t="s">
+      <c r="AL5" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="AK5" s="25">
-        <f>AK3+DAY(1)</f>
+      <c r="AM5" s="25">
+        <f>AM3+DAY(1)</f>
         <v>42948</v>
       </c>
-      <c r="AL5" s="20" t="s">
+      <c r="AN5" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="AM5" s="4"/>
-      <c r="AN5" s="4" t="s">
+      <c r="AO5" s="4"/>
+      <c r="AP5" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AO5" s="4" t="s">
+      <c r="AQ5" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="AP5" s="1" t="s">
+      <c r="AR5" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AQ5" s="11" t="s">
+      <c r="AS5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR5" s="15"/>
-      <c r="AS5" s="11" t="s">
+      <c r="AT5" s="15"/>
+      <c r="AU5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AT5" s="27" t="s">
+      <c r="AV5" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="AU5" s="27" t="s">
+      <c r="AW5" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="AV5" s="27" t="s">
+      <c r="AX5" s="27" t="s">
         <v>170</v>
       </c>
-      <c r="AW5" s="4"/>
-      <c r="AX5" s="4"/>
       <c r="AY5" s="4"/>
       <c r="AZ5" s="4"/>
       <c r="BA5" s="4"/>
       <c r="BB5" s="4"/>
       <c r="BC5" s="4"/>
-      <c r="BD5" s="4" t="s">
+      <c r="BD5" s="4"/>
+      <c r="BE5" s="4"/>
+      <c r="BF5" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:56" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:58" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>44</v>
       </c>
@@ -1848,27 +1948,29 @@
       <c r="I6" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="11" t="s">
+        <v>180</v>
+      </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="15">
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="15">
         <v>42137</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="S6" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="R6" s="4"/>
-      <c r="S6" s="18" t="s">
+      <c r="T6" s="4"/>
+      <c r="U6" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="T6" s="4" t="s">
+      <c r="V6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
@@ -1878,47 +1980,49 @@
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
       <c r="AE6" s="4"/>
-      <c r="AF6" s="4" t="s">
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="AG6" s="4" t="s">
+      <c r="AI6" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="AH6" s="4"/>
-      <c r="AI6" s="4"/>
       <c r="AJ6" s="4"/>
-      <c r="AK6" s="25" t="s">
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="AL6" s="20"/>
-      <c r="AM6" s="4"/>
-      <c r="AN6" s="4" t="s">
+      <c r="AN6" s="20"/>
+      <c r="AO6" s="4"/>
+      <c r="AP6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AO6" s="4" t="s">
+      <c r="AQ6" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="AP6" s="4"/>
-      <c r="AQ6" s="11" t="s">
+      <c r="AR6" s="4"/>
+      <c r="AS6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR6" s="11"/>
-      <c r="AS6" s="11"/>
-      <c r="AT6" s="27"/>
-      <c r="AU6" s="27"/>
+      <c r="AT6" s="11"/>
+      <c r="AU6" s="11"/>
       <c r="AV6" s="27"/>
-      <c r="AW6" s="4"/>
-      <c r="AX6" s="4"/>
+      <c r="AW6" s="27"/>
+      <c r="AX6" s="27"/>
       <c r="AY6" s="4"/>
       <c r="AZ6" s="4"/>
       <c r="BA6" s="4"/>
       <c r="BB6" s="4"/>
       <c r="BC6" s="4"/>
-      <c r="BD6" s="4" t="s">
+      <c r="BD6" s="4"/>
+      <c r="BE6" s="4"/>
+      <c r="BF6" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>44</v>
       </c>
@@ -1930,22 +2034,22 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="4"/>
+      <c r="J7" s="11"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="15">
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="15">
         <v>42137</v>
       </c>
-      <c r="Q7" s="4" t="s">
+      <c r="S7" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="R7" s="4"/>
-      <c r="S7" s="11"/>
       <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
+      <c r="U7" s="11"/>
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
@@ -1961,32 +2065,34 @@
       <c r="AH7" s="4"/>
       <c r="AI7" s="4"/>
       <c r="AJ7" s="4"/>
-      <c r="AK7" s="20"/>
-      <c r="AL7" s="20"/>
-      <c r="AM7" s="4"/>
-      <c r="AN7" s="4"/>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="20"/>
+      <c r="AN7" s="20"/>
       <c r="AO7" s="4"/>
       <c r="AP7" s="4"/>
-      <c r="AQ7" s="11" t="s">
+      <c r="AQ7" s="4"/>
+      <c r="AR7" s="4"/>
+      <c r="AS7" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR7" s="11"/>
-      <c r="AS7" s="11"/>
-      <c r="AT7" s="27"/>
-      <c r="AU7" s="27"/>
+      <c r="AT7" s="11"/>
+      <c r="AU7" s="11"/>
       <c r="AV7" s="27"/>
-      <c r="AW7" s="4"/>
-      <c r="AX7" s="4"/>
+      <c r="AW7" s="27"/>
+      <c r="AX7" s="27"/>
       <c r="AY7" s="4"/>
       <c r="AZ7" s="4"/>
       <c r="BA7" s="4"/>
       <c r="BB7" s="4"/>
       <c r="BC7" s="4"/>
-      <c r="BD7" s="4" t="s">
+      <c r="BD7" s="4"/>
+      <c r="BE7" s="4"/>
+      <c r="BF7" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>44</v>
       </c>
@@ -1998,22 +2104,22 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="4"/>
+      <c r="J8" s="11"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="15">
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="15">
         <v>42137</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="S8" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="R8" s="4"/>
-      <c r="S8" s="11"/>
       <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
+      <c r="U8" s="11"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
@@ -2029,35 +2135,37 @@
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
       <c r="AJ8" s="4"/>
-      <c r="AK8" s="25">
-        <f>AK5+DAY(1)</f>
+      <c r="AK8" s="4"/>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="25">
+        <f>AM5+DAY(1)</f>
         <v>42949</v>
       </c>
-      <c r="AL8" s="20" t="s">
+      <c r="AN8" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="AM8" s="4"/>
-      <c r="AN8" s="4"/>
       <c r="AO8" s="4"/>
       <c r="AP8" s="4"/>
-      <c r="AQ8" s="11" t="s">
+      <c r="AQ8" s="4"/>
+      <c r="AR8" s="4"/>
+      <c r="AS8" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AR8" s="11"/>
-      <c r="AS8" s="11"/>
-      <c r="AT8" s="27"/>
-      <c r="AU8" s="27"/>
+      <c r="AT8" s="11"/>
+      <c r="AU8" s="11"/>
       <c r="AV8" s="27"/>
-      <c r="AW8" s="4"/>
-      <c r="AX8" s="4"/>
+      <c r="AW8" s="27"/>
+      <c r="AX8" s="27"/>
       <c r="AY8" s="4"/>
       <c r="AZ8" s="4"/>
       <c r="BA8" s="4"/>
       <c r="BB8" s="4"/>
       <c r="BC8" s="4"/>
       <c r="BD8" s="4"/>
+      <c r="BE8" s="4"/>
+      <c r="BF8" s="4"/>
     </row>
-    <row r="9" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>44</v>
       </c>
@@ -2069,22 +2177,22 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="10"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="16">
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="16">
         <v>42137</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="S9" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="R9" s="3"/>
-      <c r="S9" s="10"/>
       <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
+      <c r="U9" s="10"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
@@ -2100,30 +2208,32 @@
       <c r="AH9" s="3"/>
       <c r="AI9" s="3"/>
       <c r="AJ9" s="3"/>
-      <c r="AK9" s="22"/>
-      <c r="AL9" s="22"/>
-      <c r="AM9" s="3"/>
-      <c r="AN9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="22"/>
+      <c r="AN9" s="22"/>
       <c r="AO9" s="3"/>
       <c r="AP9" s="3"/>
-      <c r="AQ9" s="10" t="s">
+      <c r="AQ9" s="3"/>
+      <c r="AR9" s="3"/>
+      <c r="AS9" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AR9" s="10"/>
-      <c r="AS9" s="10"/>
-      <c r="AT9" s="26"/>
-      <c r="AU9" s="26"/>
+      <c r="AT9" s="10"/>
+      <c r="AU9" s="10"/>
       <c r="AV9" s="26"/>
-      <c r="AW9" s="3"/>
-      <c r="AX9" s="3"/>
+      <c r="AW9" s="26"/>
+      <c r="AX9" s="26"/>
       <c r="AY9" s="3"/>
       <c r="AZ9" s="3"/>
       <c r="BA9" s="3"/>
       <c r="BB9" s="3"/>
       <c r="BC9" s="3"/>
       <c r="BD9" s="3"/>
+      <c r="BE9" s="3"/>
+      <c r="BF9" s="3"/>
     </row>
-    <row r="10" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>119</v>
       </c>
@@ -2143,27 +2253,27 @@
       <c r="I10" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="J10" s="5"/>
+      <c r="J10" s="12"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="17">
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="17">
         <v>42581</v>
       </c>
-      <c r="Q10" s="5" t="s">
+      <c r="S10" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="R10" s="5"/>
-      <c r="S10" s="12" t="s">
+      <c r="T10" s="5"/>
+      <c r="U10" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="T10" s="5" t="s">
+      <c r="V10" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
@@ -2178,34 +2288,36 @@
       <c r="AH10" s="5"/>
       <c r="AI10" s="5"/>
       <c r="AJ10" s="5"/>
-      <c r="AK10" s="23"/>
-      <c r="AL10" s="23"/>
-      <c r="AM10" s="5"/>
-      <c r="AN10" s="5"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="5"/>
+      <c r="AM10" s="23"/>
+      <c r="AN10" s="23"/>
       <c r="AO10" s="5"/>
       <c r="AP10" s="5"/>
-      <c r="AQ10" s="12" t="s">
+      <c r="AQ10" s="5"/>
+      <c r="AR10" s="5"/>
+      <c r="AS10" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="AR10" s="17"/>
-      <c r="AS10" s="12" t="s">
+      <c r="AT10" s="17"/>
+      <c r="AU10" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="AT10" s="28"/>
-      <c r="AU10" s="28"/>
       <c r="AV10" s="28"/>
-      <c r="AW10" s="5"/>
-      <c r="AX10" s="5"/>
+      <c r="AW10" s="28"/>
+      <c r="AX10" s="28"/>
       <c r="AY10" s="5"/>
       <c r="AZ10" s="5"/>
       <c r="BA10" s="5"/>
       <c r="BB10" s="5"/>
       <c r="BC10" s="5"/>
-      <c r="BD10" s="5" t="s">
+      <c r="BD10" s="5"/>
+      <c r="BE10" s="5"/>
+      <c r="BF10" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>149</v>
       </c>
@@ -2224,54 +2336,55 @@
       <c r="I11" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="P11" s="15">
+      <c r="J11" s="13"/>
+      <c r="R11" s="15">
         <v>42582</v>
       </c>
-      <c r="S11" s="13" t="s">
+      <c r="U11" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="AK11" s="20"/>
-      <c r="AL11" s="20"/>
-      <c r="AN11" t="s">
+      <c r="AM11" s="20"/>
+      <c r="AN11" s="20"/>
+      <c r="AP11" t="s">
         <v>174</v>
       </c>
-      <c r="AQ11" s="13" t="s">
+      <c r="AS11" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="AR11" s="15">
+      <c r="AT11" s="15">
         <v>42581</v>
       </c>
-      <c r="AS11" s="13" t="s">
+      <c r="AU11" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AT11" s="7" t="s">
+      <c r="AV11" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="AU11" s="7" t="s">
+      <c r="AW11" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="AV11" s="29"/>
-      <c r="AW11" s="4" t="s">
+      <c r="AX11" s="29"/>
+      <c r="AY11" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AX11" s="4" t="s">
+      <c r="AZ11" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AY11" s="4" t="s">
+      <c r="BA11" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AZ11" s="4" t="s">
+      <c r="BB11" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="BA11" s="7"/>
-      <c r="BD11" s="8" t="s">
+      <c r="BC11" s="7"/>
+      <c r="BF11" s="8" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AJ4" r:id="rId1"/>
-    <hyperlink ref="AP5" r:id="rId2"/>
+    <hyperlink ref="AL4" r:id="rId1"/>
+    <hyperlink ref="AR5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
unit test updates in SplitMultiDepositAppSpec
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gulcinermis/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1A3D58E3-0AD4-614E-A73F-1B90E600C981}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BE$9</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Richard van Heest</author>
   </authors>
   <commentList>
-    <comment ref="AT1" authorId="0">
+    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="187">
   <si>
     <t>DATASET</t>
   </si>
@@ -613,17 +614,29 @@
   </si>
   <si>
     <t>WorkPackageLeader</t>
+  </si>
+  <si>
+    <t>d5e8f0fb-c374-86eb-918c-b06dd5ae5e71</t>
+  </si>
+  <si>
+    <t>1de3f841-0f0d-48bc-b3db-4b03ad4834d7</t>
+  </si>
+  <si>
+    <t>9ad0a3e4-39d4-47a0-b1a1-b6377ed516af</t>
+  </si>
+  <si>
+    <t>773dc53a-1cdb-47c4-992a-254a59b98376</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="00000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -670,6 +683,18 @@
       <b/>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -815,7 +840,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -851,6 +876,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -946,6 +974,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1213,14 +1244,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BG11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BC2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="BD14" sqref="BD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1281,9 +1312,10 @@
     <col min="56" max="56" width="29.1640625" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="23" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="35.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1458,8 +1490,9 @@
       <c r="BF1" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="BG1" s="6"/>
     </row>
-    <row r="2" spans="1:58" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>43</v>
       </c>
@@ -1614,8 +1647,11 @@
       <c r="BF2" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="BG2" s="32" t="s">
+        <v>183</v>
+      </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>43</v>
       </c>
@@ -1735,7 +1771,7 @@
       </c>
       <c r="BF3" s="4"/>
     </row>
-    <row r="4" spans="1:58" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
@@ -1808,8 +1844,9 @@
       <c r="BD4" s="3"/>
       <c r="BE4" s="3"/>
       <c r="BF4" s="3"/>
+      <c r="BG4" s="6"/>
     </row>
-    <row r="5" spans="1:58" ht="96" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>44</v>
       </c>
@@ -1923,8 +1960,11 @@
       <c r="BF5" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="BG5" s="31" t="s">
+        <v>184</v>
+      </c>
     </row>
-    <row r="6" spans="1:58" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>44</v>
       </c>
@@ -2022,7 +2062,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>44</v>
       </c>
@@ -2092,7 +2132,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>44</v>
       </c>
@@ -2165,7 +2205,7 @@
       <c r="BE8" s="4"/>
       <c r="BF8" s="4"/>
     </row>
-    <row r="9" spans="1:58" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>44</v>
       </c>
@@ -2232,8 +2272,9 @@
       <c r="BD9" s="3"/>
       <c r="BE9" s="3"/>
       <c r="BF9" s="3"/>
+      <c r="BG9" s="6"/>
     </row>
-    <row r="10" spans="1:58" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>119</v>
       </c>
@@ -2316,8 +2357,11 @@
       <c r="BF10" s="5" t="s">
         <v>81</v>
       </c>
+      <c r="BG10" s="33" t="s">
+        <v>185</v>
+      </c>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>149</v>
       </c>
@@ -2380,11 +2424,14 @@
       <c r="BF11" s="8" t="s">
         <v>81</v>
       </c>
+      <c r="BG11" s="31" t="s">
+        <v>186</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AL4" r:id="rId1"/>
-    <hyperlink ref="AR5" r:id="rId2"/>
+    <hyperlink ref="AL4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="AR5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
test data and related tagmanifests updated
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gulcinermis/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1A3D58E3-0AD4-614E-A73F-1B90E600C981}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2F94C451-A73A-B249-A6E3-7D3F7941453B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="185">
   <si>
     <t>DATASET</t>
   </si>
@@ -617,12 +617,6 @@
   </si>
   <si>
     <t>d5e8f0fb-c374-86eb-918c-b06dd5ae5e71</t>
-  </si>
-  <si>
-    <t>1de3f841-0f0d-48bc-b3db-4b03ad4834d7</t>
-  </si>
-  <si>
-    <t>9ad0a3e4-39d4-47a0-b1a1-b6377ed516af</t>
   </si>
   <si>
     <t>773dc53a-1cdb-47c4-992a-254a59b98376</t>
@@ -1248,10 +1242,10 @@
   <dimension ref="A1:BG11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BC2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BD14" sqref="BD14"/>
+      <selection pane="bottomRight" activeCell="BG10" sqref="BG10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1844,7 +1838,9 @@
       <c r="BD4" s="3"/>
       <c r="BE4" s="3"/>
       <c r="BF4" s="3"/>
-      <c r="BG4" s="6"/>
+      <c r="BG4" s="32" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="5" spans="1:59" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
@@ -1960,9 +1956,7 @@
       <c r="BF5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BG5" s="31" t="s">
-        <v>184</v>
-      </c>
+      <c r="BG5" s="31"/>
     </row>
     <row r="6" spans="1:59" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
@@ -2357,9 +2351,7 @@
       <c r="BF10" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="BG10" s="33" t="s">
-        <v>185</v>
-      </c>
+      <c r="BG10" s="33"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
@@ -2425,7 +2417,7 @@
         <v>81</v>
       </c>
       <c r="BG11" s="31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EASY-1507: Add Base-Revision column to instructions.csv (#106)
* validate base revision conforms to UUID
* another unit test for validation and reformatting
* unit tests 
* instructions info
* excessive maps removed
* excessive lines removed
* check bag-info.txt cleaned
* base=None removed
* real value instead of base.get
* codacy review: field name conforms to regular expressions
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gulcinermis/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2F94C451-A73A-B249-A6E3-7D3F7941453B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BE$9</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Richard van Heest</author>
   </authors>
   <commentList>
-    <comment ref="AT1" authorId="0">
+    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="185">
   <si>
     <t>DATASET</t>
   </si>
@@ -613,17 +614,23 @@
   </si>
   <si>
     <t>WorkPackageLeader</t>
+  </si>
+  <si>
+    <t>d5e8f0fb-c374-86eb-918c-b06dd5ae5e71</t>
+  </si>
+  <si>
+    <t>773dc53a-1cdb-47c4-992a-254a59b98376</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="00000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -670,6 +677,18 @@
       <b/>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -815,7 +834,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -851,6 +870,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -946,6 +968,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1213,14 +1238,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BG11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="BG10" sqref="BG10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1281,9 +1306,10 @@
     <col min="56" max="56" width="29.1640625" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="23" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="35.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1458,8 +1484,9 @@
       <c r="BF1" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="BG1" s="6"/>
     </row>
-    <row r="2" spans="1:58" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>43</v>
       </c>
@@ -1614,8 +1641,11 @@
       <c r="BF2" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="BG2" s="32" t="s">
+        <v>183</v>
+      </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>43</v>
       </c>
@@ -1735,7 +1765,7 @@
       </c>
       <c r="BF3" s="4"/>
     </row>
-    <row r="4" spans="1:58" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
@@ -1808,8 +1838,11 @@
       <c r="BD4" s="3"/>
       <c r="BE4" s="3"/>
       <c r="BF4" s="3"/>
+      <c r="BG4" s="32" t="s">
+        <v>183</v>
+      </c>
     </row>
-    <row r="5" spans="1:58" ht="96" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>44</v>
       </c>
@@ -1923,8 +1956,9 @@
       <c r="BF5" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="BG5" s="31"/>
     </row>
-    <row r="6" spans="1:58" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>44</v>
       </c>
@@ -2022,7 +2056,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>44</v>
       </c>
@@ -2092,7 +2126,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>44</v>
       </c>
@@ -2165,7 +2199,7 @@
       <c r="BE8" s="4"/>
       <c r="BF8" s="4"/>
     </row>
-    <row r="9" spans="1:58" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>44</v>
       </c>
@@ -2232,8 +2266,9 @@
       <c r="BD9" s="3"/>
       <c r="BE9" s="3"/>
       <c r="BF9" s="3"/>
+      <c r="BG9" s="6"/>
     </row>
-    <row r="10" spans="1:58" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>119</v>
       </c>
@@ -2316,8 +2351,9 @@
       <c r="BF10" s="5" t="s">
         <v>81</v>
       </c>
+      <c r="BG10" s="33"/>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>149</v>
       </c>
@@ -2380,11 +2416,14 @@
       <c r="BF11" s="8" t="s">
         <v>81</v>
       </c>
+      <c r="BG11" s="31" t="s">
+        <v>184</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AL4" r:id="rId1"/>
-    <hyperlink ref="AR5" r:id="rId2"/>
+    <hyperlink ref="AL4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="AR5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Check that visibility is always at least as open as accessibility. Also, restored the ability to report more file attribute errors at once for some cases.
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -5,24 +5,25 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Notes" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Instructions" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$BF$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Instructions!$A$1:$BF$9</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author> </author>
@@ -59,7 +60,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="190">
+  <si>
+    <t xml:space="preserve">Use this XLS as the source, do not directly edit the resulting CSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Export with US Locale settings</t>
+  </si>
   <si>
     <t xml:space="preserve">DATASET</t>
   </si>
@@ -631,7 +638,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY/MM/DD"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="00000"/>
   </numFmts>
   <fonts count="9">
@@ -953,14 +960,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:BH11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BF2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AQ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="BF1" activeCellId="0" sqref="BF1"/>
+      <selection pane="topRight" activeCell="AQ1" activeCellId="0" sqref="AQ1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BH2" activeCellId="0" sqref="BH2"/>
+      <selection pane="bottomRight" activeCell="AY5" activeCellId="0" sqref="AY5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1014,7 +1058,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="29.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="17.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="0" width="11.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="17.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="11.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="54" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="20.83"/>
@@ -1027,257 +1072,257 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="AF1" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="AG1" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AH1" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AI1" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AK1" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AL1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AM1" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AN1" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AO1" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AP1" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AQ1" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AR1" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AS1" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AV1" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AW1" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AX1" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AY1" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AZ1" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="BA1" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="BB1" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="BC1" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="BD1" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="BE1" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="BF1" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="BG1" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="BH1" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="Q2" s="6"/>
       <c r="R2" s="7" t="n">
         <v>42143</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="W2" s="6"/>
       <c r="X2" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="AB2" s="6" t="n">
         <v>83575.4</v>
@@ -1290,89 +1335,89 @@
       <c r="AF2" s="6"/>
       <c r="AG2" s="6"/>
       <c r="AH2" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="AI2" s="6"/>
       <c r="AJ2" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AK2" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="AL2" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AM2" s="10" t="n">
         <v>42946</v>
       </c>
       <c r="AN2" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="AO2" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="AP2" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="AQ2" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AR2" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="AS2" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AT2" s="7" t="n">
         <v>33815</v>
       </c>
       <c r="AU2" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AV2" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="AW2" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AX2" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AY2" s="6"/>
       <c r="AZ2" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="BA2" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BB2" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="BC2" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="BD2" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="BE2" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="BF2" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="BG2" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="BH2" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
@@ -1384,42 +1429,42 @@
       <c r="J3" s="5"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="R3" s="7"/>
       <c r="S3" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="W3" s="6"/>
       <c r="X3" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="Y3" s="6"/>
       <c r="Z3" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
@@ -1439,38 +1484,38 @@
         <v>6663</v>
       </c>
       <c r="AI3" s="6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AJ3" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AK3" s="6" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AL3" s="6"/>
       <c r="AM3" s="10" t="n">
         <v>42947</v>
       </c>
       <c r="AN3" s="6" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="AO3" s="6"/>
       <c r="AP3" s="6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AQ3" s="6" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AR3" s="6"/>
       <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5"/>
       <c r="AV3" s="11" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AW3" s="11"/>
       <c r="AX3" s="11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AY3" s="11"/>
       <c r="AZ3" s="6"/>
@@ -1478,19 +1523,19 @@
       <c r="BB3" s="6"/>
       <c r="BC3" s="6"/>
       <c r="BD3" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="BE3" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="BF3" s="6" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="BG3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -1510,15 +1555,15 @@
       <c r="Q4" s="3"/>
       <c r="R4" s="12"/>
       <c r="S4" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="T4" s="3"/>
       <c r="U4" s="13"/>
       <c r="V4" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
@@ -1534,16 +1579,16 @@
       <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
       <c r="AK4" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="AL4" s="14" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AM4" s="15"/>
       <c r="AN4" s="15"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AQ4" s="3"/>
       <c r="AR4" s="3"/>
@@ -1563,33 +1608,33 @@
       <c r="BF4" s="3"/>
       <c r="BG4" s="3"/>
       <c r="BH4" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="74" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
@@ -1602,18 +1647,18 @@
         <v>42137</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="T5" s="6"/>
       <c r="U5" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="W5" s="6"/>
       <c r="X5" s="6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
@@ -1625,53 +1670,53 @@
       <c r="AF5" s="6"/>
       <c r="AG5" s="6"/>
       <c r="AH5" s="6" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AI5" s="6"/>
       <c r="AJ5" s="6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AK5" s="16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AL5" s="6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AM5" s="10" t="n">
         <f aca="false">AM3+DAY(1)</f>
-        <v>42948</v>
+        <v>42978</v>
       </c>
       <c r="AN5" s="6" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AO5" s="6"/>
       <c r="AP5" s="6" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AQ5" s="6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AR5" s="17" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AS5" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AT5" s="7"/>
       <c r="AU5" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AV5" s="11" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AW5" s="11" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AX5" s="11" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AY5" s="11" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AZ5" s="6"/>
       <c r="BA5" s="6"/>
@@ -1681,36 +1726,36 @@
       <c r="BE5" s="6"/>
       <c r="BF5" s="6"/>
       <c r="BG5" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="BH5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="74" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
@@ -1723,14 +1768,14 @@
         <v>42137</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="T6" s="6"/>
       <c r="U6" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
@@ -1744,28 +1789,28 @@
       <c r="AF6" s="6"/>
       <c r="AG6" s="6"/>
       <c r="AH6" s="6" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AI6" s="6" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="AJ6" s="6"/>
       <c r="AK6" s="6"/>
       <c r="AL6" s="6"/>
       <c r="AM6" s="10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="AN6" s="6"/>
       <c r="AO6" s="6"/>
       <c r="AP6" s="6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AQ6" s="6" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="AR6" s="6"/>
       <c r="AS6" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AT6" s="5"/>
       <c r="AU6" s="5"/>
@@ -1781,12 +1826,12 @@
       <c r="BE6" s="6"/>
       <c r="BF6" s="6"/>
       <c r="BG6" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
@@ -1808,7 +1853,7 @@
         <v>42137</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="T7" s="6"/>
       <c r="U7" s="5"/>
@@ -1836,7 +1881,7 @@
       <c r="AQ7" s="6"/>
       <c r="AR7" s="6"/>
       <c r="AS7" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AT7" s="5"/>
       <c r="AU7" s="5"/>
@@ -1852,12 +1897,12 @@
       <c r="BE7" s="6"/>
       <c r="BF7" s="6"/>
       <c r="BG7" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
@@ -1879,7 +1924,7 @@
         <v>42137</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="T8" s="6"/>
       <c r="U8" s="5"/>
@@ -1902,17 +1947,17 @@
       <c r="AL8" s="6"/>
       <c r="AM8" s="10" t="n">
         <f aca="false">AM5+DAY(1)</f>
-        <v>42949</v>
+        <v>43009</v>
       </c>
       <c r="AN8" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="AO8" s="6"/>
       <c r="AP8" s="6"/>
       <c r="AQ8" s="6"/>
       <c r="AR8" s="6"/>
       <c r="AS8" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AT8" s="5"/>
       <c r="AU8" s="5"/>
@@ -1931,7 +1976,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
@@ -1953,7 +1998,7 @@
         <v>42137</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="T9" s="3"/>
       <c r="U9" s="2"/>
@@ -1981,7 +2026,7 @@
       <c r="AQ9" s="3"/>
       <c r="AR9" s="3"/>
       <c r="AS9" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
@@ -2001,23 +2046,23 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="20" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="J10" s="20"/>
       <c r="K10" s="21"/>
@@ -2031,14 +2076,14 @@
         <v>42581</v>
       </c>
       <c r="S10" s="21" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="T10" s="21"/>
       <c r="U10" s="20" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="V10" s="21" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
@@ -2063,11 +2108,11 @@
       <c r="AQ10" s="21"/>
       <c r="AR10" s="21"/>
       <c r="AS10" s="20" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="AT10" s="22"/>
       <c r="AU10" s="20" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="AV10" s="23"/>
       <c r="AW10" s="23"/>
@@ -2081,76 +2126,76 @@
       <c r="BE10" s="21"/>
       <c r="BF10" s="21"/>
       <c r="BG10" s="21" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="BH10" s="24"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="J11" s="5"/>
       <c r="R11" s="7" t="n">
         <v>42582</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="AM11" s="6"/>
       <c r="AN11" s="6"/>
       <c r="AP11" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="AS11" s="5" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="AT11" s="7" t="n">
         <v>42581</v>
       </c>
       <c r="AU11" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AV11" s="25" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="AW11" s="25" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="AX11" s="26"/>
       <c r="AY11" s="26"/>
       <c r="AZ11" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="BA11" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BB11" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="BC11" s="6" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="BD11" s="25"/>
       <c r="BG11" s="16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="BH11" s="18" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
user license field in instructions + parsing + xml generation
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA0213F-6E14-D84B-8A0E-BC4F0727BBAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59921E1D-9487-9847-93A5-E1D4FEB8C616}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
     <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">Instructions!$A$1:$BF$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">Instructions!$A$1:$BG$9</definedName>
   </definedNames>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -34,7 +34,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="194">
   <si>
     <t>Use this XLS as the source, do not directly edit the resulting CSV</t>
   </si>
@@ -638,6 +638,15 @@
   </si>
   <si>
     <t>video about the hubble space telescope</t>
+  </si>
+  <si>
+    <t>http://creativecommons.org/licenses/by-nc-sa/4.0/</t>
+  </si>
+  <si>
+    <t>http://opensource.org/licenses/MIT</t>
+  </si>
+  <si>
+    <t>DCT_LICENSE</t>
   </si>
 </sst>
 </file>
@@ -1142,6 +1151,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB0F08FF-302C-6D4F-83FA-398A55808377}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12712700"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A384839C-0F16-274A-8A92-4E10DAD5AD70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12725400"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1475,13 +1592,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BH11"/>
+  <dimension ref="A1:BI11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AR2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AQ1" sqref="AQ1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AW3" sqref="AW3"/>
+      <selection pane="bottomRight" activeCell="AT1" sqref="AT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1530,24 +1647,25 @@
     <col min="43" max="43" width="14.33203125" customWidth="1"/>
     <col min="44" max="44" width="22.33203125" customWidth="1"/>
     <col min="45" max="45" width="34.33203125" customWidth="1"/>
-    <col min="46" max="46" width="15.1640625" customWidth="1"/>
-    <col min="47" max="47" width="14.6640625" customWidth="1"/>
-    <col min="48" max="48" width="33" customWidth="1"/>
-    <col min="49" max="49" width="34" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="17.1640625" customWidth="1"/>
-    <col min="52" max="52" width="11.1640625" customWidth="1"/>
-    <col min="53" max="53" width="13.5" customWidth="1"/>
-    <col min="54" max="55" width="14.1640625" customWidth="1"/>
-    <col min="56" max="56" width="20.83203125" customWidth="1"/>
-    <col min="57" max="57" width="29.1640625" customWidth="1"/>
-    <col min="58" max="58" width="23" customWidth="1"/>
-    <col min="59" max="59" width="13.1640625" customWidth="1"/>
-    <col min="60" max="60" width="35.5" customWidth="1"/>
-    <col min="61" max="1025" width="11" customWidth="1"/>
+    <col min="46" max="46" width="34.33203125" style="26" customWidth="1"/>
+    <col min="47" max="47" width="15.1640625" customWidth="1"/>
+    <col min="48" max="48" width="14.6640625" customWidth="1"/>
+    <col min="49" max="49" width="33" customWidth="1"/>
+    <col min="50" max="50" width="34" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="17.1640625" customWidth="1"/>
+    <col min="53" max="53" width="11.1640625" customWidth="1"/>
+    <col min="54" max="54" width="13.5" customWidth="1"/>
+    <col min="55" max="56" width="14.1640625" customWidth="1"/>
+    <col min="57" max="57" width="20.83203125" customWidth="1"/>
+    <col min="58" max="58" width="29.1640625" customWidth="1"/>
+    <col min="59" max="59" width="23" customWidth="1"/>
+    <col min="60" max="60" width="13.1640625" customWidth="1"/>
+    <col min="61" max="61" width="35.5" customWidth="1"/>
+    <col min="62" max="1026" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1684,52 +1802,55 @@
         <v>46</v>
       </c>
       <c r="AT1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AU1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="BF1" s="3" t="s">
+      <c r="BG1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="BG1" s="3" t="s">
+      <c r="BH1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:60" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>62</v>
       </c>
@@ -1845,51 +1966,54 @@
       <c r="AS2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="AT2" s="7">
+      <c r="AT2" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="AU2" s="7">
         <v>33815</v>
       </c>
-      <c r="AU2" s="5" t="s">
+      <c r="AV2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="AV2" s="6" t="s">
+      <c r="AW2" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="AY2" s="6"/>
-      <c r="AZ2" s="6" t="s">
+      <c r="AZ2" s="6"/>
+      <c r="BA2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="BA2" s="6" t="s">
+      <c r="BB2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="BB2" s="6" t="s">
+      <c r="BC2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="BC2" s="6" t="s">
+      <c r="BD2" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="BD2" s="6" t="s">
+      <c r="BE2" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="BE2" s="6" t="s">
+      <c r="BF2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="BF2" s="6" t="s">
+      <c r="BG2" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="BG2" s="6" t="s">
+      <c r="BH2" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="BH2" s="6" t="s">
+      <c r="BI2" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>62</v>
       </c>
@@ -1987,32 +2111,33 @@
       <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5"/>
-      <c r="AV3" s="11" t="s">
+      <c r="AV3" s="5"/>
+      <c r="AW3" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="AW3" s="11" t="s">
+      <c r="AX3" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="AX3" s="11" t="s">
+      <c r="AY3" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="AY3" s="11"/>
-      <c r="AZ3" s="6"/>
+      <c r="AZ3" s="11"/>
       <c r="BA3" s="6"/>
       <c r="BB3" s="6"/>
       <c r="BC3" s="6"/>
-      <c r="BD3" s="6" t="s">
+      <c r="BD3" s="6"/>
+      <c r="BE3" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="BE3" s="6" t="s">
+      <c r="BF3" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="BF3" s="6" t="s">
+      <c r="BG3" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="BG3" s="6"/>
+      <c r="BH3" s="6"/>
     </row>
-    <row r="4" spans="1:60" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>62</v>
       </c>
@@ -2074,11 +2199,11 @@
       <c r="AS4" s="2"/>
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
-      <c r="AV4" s="4"/>
+      <c r="AV4" s="2"/>
       <c r="AW4" s="4"/>
       <c r="AX4" s="4"/>
       <c r="AY4" s="4"/>
-      <c r="AZ4" s="3"/>
+      <c r="AZ4" s="4"/>
       <c r="BA4" s="3"/>
       <c r="BB4" s="3"/>
       <c r="BC4" s="3"/>
@@ -2086,11 +2211,12 @@
       <c r="BE4" s="3"/>
       <c r="BF4" s="3"/>
       <c r="BG4" s="3"/>
-      <c r="BH4" s="4" t="s">
+      <c r="BH4" s="3"/>
+      <c r="BI4" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:61" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>131</v>
       </c>
@@ -2181,35 +2307,38 @@
       <c r="AS5" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="AT5" s="7"/>
-      <c r="AU5" s="5" t="s">
+      <c r="AT5" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="AU5" s="7"/>
+      <c r="AV5" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="AV5" s="11" t="s">
+      <c r="AW5" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="AW5" s="11" t="s">
+      <c r="AX5" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="AX5" s="11" t="s">
+      <c r="AY5" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="AY5" s="11" t="s">
+      <c r="AZ5" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AZ5" s="6"/>
       <c r="BA5" s="6"/>
       <c r="BB5" s="6"/>
       <c r="BC5" s="6"/>
       <c r="BD5" s="6"/>
       <c r="BE5" s="6"/>
       <c r="BF5" s="6"/>
-      <c r="BG5" s="6" t="s">
+      <c r="BG5" s="6"/>
+      <c r="BH5" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="BH5" s="18"/>
+      <c r="BI5" s="18"/>
     </row>
-    <row r="6" spans="1:60" ht="102" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:61" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>131</v>
       </c>
@@ -2291,24 +2420,27 @@
       <c r="AS6" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="AT6" s="5"/>
+      <c r="AT6" s="5" t="s">
+        <v>192</v>
+      </c>
       <c r="AU6" s="5"/>
-      <c r="AV6" s="11"/>
+      <c r="AV6" s="5"/>
       <c r="AW6" s="11"/>
       <c r="AX6" s="11"/>
       <c r="AY6" s="11"/>
-      <c r="AZ6" s="6"/>
+      <c r="AZ6" s="11"/>
       <c r="BA6" s="6"/>
       <c r="BB6" s="6"/>
       <c r="BC6" s="6"/>
       <c r="BD6" s="6"/>
       <c r="BE6" s="6"/>
       <c r="BF6" s="6"/>
-      <c r="BG6" s="6" t="s">
+      <c r="BG6" s="6"/>
+      <c r="BH6" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>131</v>
       </c>
@@ -2362,24 +2494,27 @@
       <c r="AS7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="AT7" s="5"/>
+      <c r="AT7" s="5" t="s">
+        <v>192</v>
+      </c>
       <c r="AU7" s="5"/>
-      <c r="AV7" s="11"/>
+      <c r="AV7" s="5"/>
       <c r="AW7" s="11"/>
       <c r="AX7" s="11"/>
       <c r="AY7" s="11"/>
-      <c r="AZ7" s="6"/>
+      <c r="AZ7" s="11"/>
       <c r="BA7" s="6"/>
       <c r="BB7" s="6"/>
       <c r="BC7" s="6"/>
       <c r="BD7" s="6"/>
       <c r="BE7" s="6"/>
       <c r="BF7" s="6"/>
-      <c r="BG7" s="6" t="s">
+      <c r="BG7" s="6"/>
+      <c r="BH7" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>131</v>
       </c>
@@ -2440,11 +2575,11 @@
       </c>
       <c r="AT8" s="5"/>
       <c r="AU8" s="5"/>
-      <c r="AV8" s="11"/>
+      <c r="AV8" s="5"/>
       <c r="AW8" s="11"/>
       <c r="AX8" s="11"/>
       <c r="AY8" s="11"/>
-      <c r="AZ8" s="6"/>
+      <c r="AZ8" s="11"/>
       <c r="BA8" s="6"/>
       <c r="BB8" s="6"/>
       <c r="BC8" s="6"/>
@@ -2452,8 +2587,9 @@
       <c r="BE8" s="6"/>
       <c r="BF8" s="6"/>
       <c r="BG8" s="6"/>
+      <c r="BH8" s="6"/>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>131</v>
       </c>
@@ -2509,11 +2645,11 @@
       </c>
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
-      <c r="AV9" s="4"/>
+      <c r="AV9" s="2"/>
       <c r="AW9" s="4"/>
       <c r="AX9" s="4"/>
       <c r="AY9" s="4"/>
-      <c r="AZ9" s="3"/>
+      <c r="AZ9" s="4"/>
       <c r="BA9" s="3"/>
       <c r="BB9" s="3"/>
       <c r="BC9" s="3"/>
@@ -2522,8 +2658,9 @@
       <c r="BF9" s="3"/>
       <c r="BG9" s="3"/>
       <c r="BH9" s="3"/>
+      <c r="BI9" s="3"/>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>169</v>
       </c>
@@ -2589,27 +2726,28 @@
       <c r="AS10" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="AT10" s="22"/>
-      <c r="AU10" s="20" t="s">
+      <c r="AT10" s="20"/>
+      <c r="AU10" s="22"/>
+      <c r="AV10" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="AV10" s="23"/>
       <c r="AW10" s="23"/>
       <c r="AX10" s="23"/>
       <c r="AY10" s="23"/>
-      <c r="AZ10" s="21"/>
+      <c r="AZ10" s="23"/>
       <c r="BA10" s="21"/>
       <c r="BB10" s="21"/>
       <c r="BC10" s="21"/>
       <c r="BD10" s="21"/>
       <c r="BE10" s="21"/>
       <c r="BF10" s="21"/>
-      <c r="BG10" s="21" t="s">
+      <c r="BG10" s="21"/>
+      <c r="BH10" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="BH10" s="24"/>
+      <c r="BI10" s="24"/>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>179</v>
       </c>
@@ -2643,37 +2781,38 @@
       <c r="AS11" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="AT11" s="7">
+      <c r="AT11" s="5"/>
+      <c r="AU11" s="7">
         <v>42581</v>
       </c>
-      <c r="AU11" s="5" t="s">
+      <c r="AV11" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="AV11" s="25" t="s">
+      <c r="AW11" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="AW11" s="25" t="s">
+      <c r="AX11" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="AX11" s="26"/>
       <c r="AY11" s="26"/>
-      <c r="AZ11" s="6" t="s">
+      <c r="AZ11" s="26"/>
+      <c r="BA11" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="BA11" s="6" t="s">
+      <c r="BB11" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="BB11" s="6" t="s">
+      <c r="BC11" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="BC11" s="6" t="s">
+      <c r="BD11" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="BD11" s="25"/>
-      <c r="BG11" s="16" t="s">
+      <c r="BE11" s="25"/>
+      <c r="BH11" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="BH11" s="27" t="s">
+      <c r="BI11" s="27" t="s">
         <v>189</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EASY-1760: add user license to instructions.csv (#123)
* user license field in instructions + parsing + xml generation
* test checkUserLicenseOnlyWithOpenAccess validation
* documentation for DCT_LICENSE
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA0213F-6E14-D84B-8A0E-BC4F0727BBAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59921E1D-9487-9847-93A5-E1D4FEB8C616}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
     <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">Instructions!$A$1:$BF$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">Instructions!$A$1:$BG$9</definedName>
   </definedNames>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -34,7 +34,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="194">
   <si>
     <t>Use this XLS as the source, do not directly edit the resulting CSV</t>
   </si>
@@ -638,6 +638,15 @@
   </si>
   <si>
     <t>video about the hubble space telescope</t>
+  </si>
+  <si>
+    <t>http://creativecommons.org/licenses/by-nc-sa/4.0/</t>
+  </si>
+  <si>
+    <t>http://opensource.org/licenses/MIT</t>
+  </si>
+  <si>
+    <t>DCT_LICENSE</t>
   </si>
 </sst>
 </file>
@@ -1142,6 +1151,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB0F08FF-302C-6D4F-83FA-398A55808377}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12712700"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A384839C-0F16-274A-8A92-4E10DAD5AD70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12725400"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1475,13 +1592,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BH11"/>
+  <dimension ref="A1:BI11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AR2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AQ1" sqref="AQ1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AW3" sqref="AW3"/>
+      <selection pane="bottomRight" activeCell="AT1" sqref="AT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1530,24 +1647,25 @@
     <col min="43" max="43" width="14.33203125" customWidth="1"/>
     <col min="44" max="44" width="22.33203125" customWidth="1"/>
     <col min="45" max="45" width="34.33203125" customWidth="1"/>
-    <col min="46" max="46" width="15.1640625" customWidth="1"/>
-    <col min="47" max="47" width="14.6640625" customWidth="1"/>
-    <col min="48" max="48" width="33" customWidth="1"/>
-    <col min="49" max="49" width="34" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="17.1640625" customWidth="1"/>
-    <col min="52" max="52" width="11.1640625" customWidth="1"/>
-    <col min="53" max="53" width="13.5" customWidth="1"/>
-    <col min="54" max="55" width="14.1640625" customWidth="1"/>
-    <col min="56" max="56" width="20.83203125" customWidth="1"/>
-    <col min="57" max="57" width="29.1640625" customWidth="1"/>
-    <col min="58" max="58" width="23" customWidth="1"/>
-    <col min="59" max="59" width="13.1640625" customWidth="1"/>
-    <col min="60" max="60" width="35.5" customWidth="1"/>
-    <col min="61" max="1025" width="11" customWidth="1"/>
+    <col min="46" max="46" width="34.33203125" style="26" customWidth="1"/>
+    <col min="47" max="47" width="15.1640625" customWidth="1"/>
+    <col min="48" max="48" width="14.6640625" customWidth="1"/>
+    <col min="49" max="49" width="33" customWidth="1"/>
+    <col min="50" max="50" width="34" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="17.1640625" customWidth="1"/>
+    <col min="53" max="53" width="11.1640625" customWidth="1"/>
+    <col min="54" max="54" width="13.5" customWidth="1"/>
+    <col min="55" max="56" width="14.1640625" customWidth="1"/>
+    <col min="57" max="57" width="20.83203125" customWidth="1"/>
+    <col min="58" max="58" width="29.1640625" customWidth="1"/>
+    <col min="59" max="59" width="23" customWidth="1"/>
+    <col min="60" max="60" width="13.1640625" customWidth="1"/>
+    <col min="61" max="61" width="35.5" customWidth="1"/>
+    <col min="62" max="1026" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1684,52 +1802,55 @@
         <v>46</v>
       </c>
       <c r="AT1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AU1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="BF1" s="3" t="s">
+      <c r="BG1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="BG1" s="3" t="s">
+      <c r="BH1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:60" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>62</v>
       </c>
@@ -1845,51 +1966,54 @@
       <c r="AS2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="AT2" s="7">
+      <c r="AT2" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="AU2" s="7">
         <v>33815</v>
       </c>
-      <c r="AU2" s="5" t="s">
+      <c r="AV2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="AV2" s="6" t="s">
+      <c r="AW2" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="AY2" s="6"/>
-      <c r="AZ2" s="6" t="s">
+      <c r="AZ2" s="6"/>
+      <c r="BA2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="BA2" s="6" t="s">
+      <c r="BB2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="BB2" s="6" t="s">
+      <c r="BC2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="BC2" s="6" t="s">
+      <c r="BD2" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="BD2" s="6" t="s">
+      <c r="BE2" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="BE2" s="6" t="s">
+      <c r="BF2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="BF2" s="6" t="s">
+      <c r="BG2" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="BG2" s="6" t="s">
+      <c r="BH2" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="BH2" s="6" t="s">
+      <c r="BI2" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>62</v>
       </c>
@@ -1987,32 +2111,33 @@
       <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5"/>
-      <c r="AV3" s="11" t="s">
+      <c r="AV3" s="5"/>
+      <c r="AW3" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="AW3" s="11" t="s">
+      <c r="AX3" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="AX3" s="11" t="s">
+      <c r="AY3" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="AY3" s="11"/>
-      <c r="AZ3" s="6"/>
+      <c r="AZ3" s="11"/>
       <c r="BA3" s="6"/>
       <c r="BB3" s="6"/>
       <c r="BC3" s="6"/>
-      <c r="BD3" s="6" t="s">
+      <c r="BD3" s="6"/>
+      <c r="BE3" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="BE3" s="6" t="s">
+      <c r="BF3" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="BF3" s="6" t="s">
+      <c r="BG3" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="BG3" s="6"/>
+      <c r="BH3" s="6"/>
     </row>
-    <row r="4" spans="1:60" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>62</v>
       </c>
@@ -2074,11 +2199,11 @@
       <c r="AS4" s="2"/>
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
-      <c r="AV4" s="4"/>
+      <c r="AV4" s="2"/>
       <c r="AW4" s="4"/>
       <c r="AX4" s="4"/>
       <c r="AY4" s="4"/>
-      <c r="AZ4" s="3"/>
+      <c r="AZ4" s="4"/>
       <c r="BA4" s="3"/>
       <c r="BB4" s="3"/>
       <c r="BC4" s="3"/>
@@ -2086,11 +2211,12 @@
       <c r="BE4" s="3"/>
       <c r="BF4" s="3"/>
       <c r="BG4" s="3"/>
-      <c r="BH4" s="4" t="s">
+      <c r="BH4" s="3"/>
+      <c r="BI4" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:61" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>131</v>
       </c>
@@ -2181,35 +2307,38 @@
       <c r="AS5" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="AT5" s="7"/>
-      <c r="AU5" s="5" t="s">
+      <c r="AT5" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="AU5" s="7"/>
+      <c r="AV5" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="AV5" s="11" t="s">
+      <c r="AW5" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="AW5" s="11" t="s">
+      <c r="AX5" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="AX5" s="11" t="s">
+      <c r="AY5" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="AY5" s="11" t="s">
+      <c r="AZ5" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AZ5" s="6"/>
       <c r="BA5" s="6"/>
       <c r="BB5" s="6"/>
       <c r="BC5" s="6"/>
       <c r="BD5" s="6"/>
       <c r="BE5" s="6"/>
       <c r="BF5" s="6"/>
-      <c r="BG5" s="6" t="s">
+      <c r="BG5" s="6"/>
+      <c r="BH5" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="BH5" s="18"/>
+      <c r="BI5" s="18"/>
     </row>
-    <row r="6" spans="1:60" ht="102" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:61" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>131</v>
       </c>
@@ -2291,24 +2420,27 @@
       <c r="AS6" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="AT6" s="5"/>
+      <c r="AT6" s="5" t="s">
+        <v>192</v>
+      </c>
       <c r="AU6" s="5"/>
-      <c r="AV6" s="11"/>
+      <c r="AV6" s="5"/>
       <c r="AW6" s="11"/>
       <c r="AX6" s="11"/>
       <c r="AY6" s="11"/>
-      <c r="AZ6" s="6"/>
+      <c r="AZ6" s="11"/>
       <c r="BA6" s="6"/>
       <c r="BB6" s="6"/>
       <c r="BC6" s="6"/>
       <c r="BD6" s="6"/>
       <c r="BE6" s="6"/>
       <c r="BF6" s="6"/>
-      <c r="BG6" s="6" t="s">
+      <c r="BG6" s="6"/>
+      <c r="BH6" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>131</v>
       </c>
@@ -2362,24 +2494,27 @@
       <c r="AS7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="AT7" s="5"/>
+      <c r="AT7" s="5" t="s">
+        <v>192</v>
+      </c>
       <c r="AU7" s="5"/>
-      <c r="AV7" s="11"/>
+      <c r="AV7" s="5"/>
       <c r="AW7" s="11"/>
       <c r="AX7" s="11"/>
       <c r="AY7" s="11"/>
-      <c r="AZ7" s="6"/>
+      <c r="AZ7" s="11"/>
       <c r="BA7" s="6"/>
       <c r="BB7" s="6"/>
       <c r="BC7" s="6"/>
       <c r="BD7" s="6"/>
       <c r="BE7" s="6"/>
       <c r="BF7" s="6"/>
-      <c r="BG7" s="6" t="s">
+      <c r="BG7" s="6"/>
+      <c r="BH7" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>131</v>
       </c>
@@ -2440,11 +2575,11 @@
       </c>
       <c r="AT8" s="5"/>
       <c r="AU8" s="5"/>
-      <c r="AV8" s="11"/>
+      <c r="AV8" s="5"/>
       <c r="AW8" s="11"/>
       <c r="AX8" s="11"/>
       <c r="AY8" s="11"/>
-      <c r="AZ8" s="6"/>
+      <c r="AZ8" s="11"/>
       <c r="BA8" s="6"/>
       <c r="BB8" s="6"/>
       <c r="BC8" s="6"/>
@@ -2452,8 +2587,9 @@
       <c r="BE8" s="6"/>
       <c r="BF8" s="6"/>
       <c r="BG8" s="6"/>
+      <c r="BH8" s="6"/>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>131</v>
       </c>
@@ -2509,11 +2645,11 @@
       </c>
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
-      <c r="AV9" s="4"/>
+      <c r="AV9" s="2"/>
       <c r="AW9" s="4"/>
       <c r="AX9" s="4"/>
       <c r="AY9" s="4"/>
-      <c r="AZ9" s="3"/>
+      <c r="AZ9" s="4"/>
       <c r="BA9" s="3"/>
       <c r="BB9" s="3"/>
       <c r="BC9" s="3"/>
@@ -2522,8 +2658,9 @@
       <c r="BF9" s="3"/>
       <c r="BG9" s="3"/>
       <c r="BH9" s="3"/>
+      <c r="BI9" s="3"/>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>169</v>
       </c>
@@ -2589,27 +2726,28 @@
       <c r="AS10" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="AT10" s="22"/>
-      <c r="AU10" s="20" t="s">
+      <c r="AT10" s="20"/>
+      <c r="AU10" s="22"/>
+      <c r="AV10" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="AV10" s="23"/>
       <c r="AW10" s="23"/>
       <c r="AX10" s="23"/>
       <c r="AY10" s="23"/>
-      <c r="AZ10" s="21"/>
+      <c r="AZ10" s="23"/>
       <c r="BA10" s="21"/>
       <c r="BB10" s="21"/>
       <c r="BC10" s="21"/>
       <c r="BD10" s="21"/>
       <c r="BE10" s="21"/>
       <c r="BF10" s="21"/>
-      <c r="BG10" s="21" t="s">
+      <c r="BG10" s="21"/>
+      <c r="BH10" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="BH10" s="24"/>
+      <c r="BI10" s="24"/>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>179</v>
       </c>
@@ -2643,37 +2781,38 @@
       <c r="AS11" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="AT11" s="7">
+      <c r="AT11" s="5"/>
+      <c r="AU11" s="7">
         <v>42581</v>
       </c>
-      <c r="AU11" s="5" t="s">
+      <c r="AV11" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="AV11" s="25" t="s">
+      <c r="AW11" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="AW11" s="25" t="s">
+      <c r="AX11" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="AX11" s="26"/>
       <c r="AY11" s="26"/>
-      <c r="AZ11" s="6" t="s">
+      <c r="AZ11" s="26"/>
+      <c r="BA11" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="BA11" s="6" t="s">
+      <c r="BB11" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="BB11" s="6" t="s">
+      <c r="BC11" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="BC11" s="6" t="s">
+      <c r="BD11" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="BD11" s="25"/>
-      <c r="BG11" s="16" t="s">
+      <c r="BE11" s="25"/>
+      <c r="BH11" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="BH11" s="27" t="s">
+      <c r="BI11" s="27" t="s">
         <v>189</v>
       </c>
     </row>

</xml_diff>

<commit_message>
make DCT_RIGHTSHOLDER column mandatory
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59921E1D-9487-9847-93A5-E1D4FEB8C616}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E5257B-1031-6241-B9AF-53B8853D3906}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">Instructions!$A$1:$BG$9</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="195">
   <si>
     <t>Use this XLS as the source, do not directly edit the resulting CSV</t>
   </si>
@@ -647,6 +647,9 @@
   </si>
   <si>
     <t>DCT_LICENSE</t>
+  </si>
+  <si>
+    <t>stephan</t>
   </si>
 </sst>
 </file>
@@ -765,7 +768,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -798,6 +801,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1259,6 +1263,60 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95F3886E-C7BF-7B43-9923-83E1010F0D6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12725400"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1595,10 +1653,10 @@
   <dimension ref="A1:BI11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AQ1" sqref="AQ1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AT1" sqref="AT1"/>
+      <selection pane="bottomRight" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2770,6 +2828,9 @@
       <c r="R11" s="7">
         <v>42582</v>
       </c>
+      <c r="S11" s="28" t="s">
+        <v>194</v>
+      </c>
       <c r="U11" s="5" t="s">
         <v>183</v>
       </c>

</xml_diff>

<commit_message>
EASY-1978: Make DCT_RIGHTSHOLDER column mandatory (#133)
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59921E1D-9487-9847-93A5-E1D4FEB8C616}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E5257B-1031-6241-B9AF-53B8853D3906}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">Instructions!$A$1:$BG$9</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="195">
   <si>
     <t>Use this XLS as the source, do not directly edit the resulting CSV</t>
   </si>
@@ -647,6 +647,9 @@
   </si>
   <si>
     <t>DCT_LICENSE</t>
+  </si>
+  <si>
+    <t>stephan</t>
   </si>
 </sst>
 </file>
@@ -765,7 +768,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -798,6 +801,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1259,6 +1263,60 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95F3886E-C7BF-7B43-9923-83E1010F0D6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12725400"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1595,10 +1653,10 @@
   <dimension ref="A1:BI11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AQ1" sqref="AQ1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AT1" sqref="AT1"/>
+      <selection pane="bottomRight" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2770,6 +2828,9 @@
       <c r="R11" s="7">
         <v>42582</v>
       </c>
+      <c r="S11" s="28" t="s">
+        <v>194</v>
+      </c>
       <c r="U11" s="5" t="s">
         <v>183</v>
       </c>

</xml_diff>

<commit_message>
use URL validation in parsing instructions.csv
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E5257B-1031-6241-B9AF-53B8853D3906}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE54E10-8A5A-B64A-A6B9-FDAF058ED6E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,12 @@
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -325,9 +331,6 @@
     <t>dummy</t>
   </si>
   <si>
-    <t>foobar</t>
-  </si>
-  <si>
     <t>Valid</t>
   </si>
   <si>
@@ -499,9 +502,6 @@
     <t>context</t>
   </si>
   <si>
-    <t>barbapappa</t>
-  </si>
-  <si>
     <t>Date Accepted</t>
   </si>
   <si>
@@ -650,6 +650,12 @@
   </si>
   <si>
     <t>stephan</t>
+  </si>
+  <si>
+    <t>http://y</t>
+  </si>
+  <si>
+    <t>http://barbapappa</t>
   </si>
 </sst>
 </file>
@@ -780,7 +786,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -802,6 +807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1317,6 +1323,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AE77436-DCB5-8346-B8A0-90D14D5BE88E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12725400"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C42AA4FF-97AE-3B41-8224-EC46EDC6B7F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12725400"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1653,10 +1767,10 @@
   <dimension ref="A1:BI11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AQ1" sqref="AQ1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S11" sqref="S11"/>
+      <selection pane="bottomRight" activeCell="AL5" sqref="AL5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1705,7 +1819,7 @@
     <col min="43" max="43" width="14.33203125" customWidth="1"/>
     <col min="44" max="44" width="22.33203125" customWidth="1"/>
     <col min="45" max="45" width="34.33203125" customWidth="1"/>
-    <col min="46" max="46" width="34.33203125" style="26" customWidth="1"/>
+    <col min="46" max="46" width="34.33203125" style="25" customWidth="1"/>
     <col min="47" max="47" width="15.1640625" customWidth="1"/>
     <col min="48" max="48" width="14.6640625" customWidth="1"/>
     <col min="49" max="49" width="33" customWidth="1"/>
@@ -1860,7 +1974,7 @@
         <v>46</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="AU1" s="2" t="s">
         <v>47</v>
@@ -2000,75 +2114,75 @@
       <c r="AK2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AL2" s="9" t="s">
+      <c r="AL2" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="AM2" s="9">
+        <v>42946</v>
+      </c>
+      <c r="AN2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="AM2" s="10">
-        <v>42946</v>
-      </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AP2" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="AQ2" s="6" t="s">
+      <c r="AR2" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="AR2" s="6" t="s">
+      <c r="AS2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AS2" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="AT2" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AU2" s="7">
         <v>33815</v>
       </c>
       <c r="AV2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AW2" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="AY2" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="AZ2" s="6"/>
       <c r="BA2" s="6" t="s">
         <v>76</v>
       </c>
       <c r="BB2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="BC2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="BC2" s="6" t="s">
+      <c r="BD2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="BD2" s="6" t="s">
+      <c r="BE2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="BF2" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="BE2" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="BF2" s="6" t="s">
+      <c r="BG2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="BG2" s="6" t="s">
+      <c r="BH2" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="BH2" s="6" t="s">
+      <c r="BI2" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="BI2" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:61" x14ac:dyDescent="0.2">
@@ -2076,7 +2190,7 @@
         <v>62</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
@@ -2088,42 +2202,42 @@
       <c r="J3" s="5"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R3" s="7"/>
       <c r="S3" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="T3" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="V3" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="W3" s="6"/>
       <c r="X3" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y3" s="6"/>
       <c r="Z3" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA3" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>115</v>
       </c>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
@@ -2143,55 +2257,55 @@
         <v>6663</v>
       </c>
       <c r="AI3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ3" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="AJ3" s="6" t="s">
+      <c r="AK3" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AK3" s="6" t="s">
+      <c r="AL3" s="6"/>
+      <c r="AM3" s="9">
+        <v>42947</v>
+      </c>
+      <c r="AN3" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="AL3" s="6"/>
-      <c r="AM3" s="10">
-        <v>42947</v>
-      </c>
-      <c r="AN3" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="AO3" s="6"/>
       <c r="AP3" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="AQ3" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="AQ3" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="AR3" s="6"/>
       <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5"/>
       <c r="AV3" s="5"/>
-      <c r="AW3" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="AX3" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="AY3" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="AZ3" s="11"/>
+      <c r="AW3" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="AX3" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="AY3" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AZ3" s="10"/>
       <c r="BA3" s="6"/>
       <c r="BB3" s="6"/>
       <c r="BC3" s="6"/>
       <c r="BD3" s="6"/>
       <c r="BE3" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BF3" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="BG3" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="BG3" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="BH3" s="6"/>
     </row>
@@ -2215,17 +2329,17 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
-      <c r="R4" s="12"/>
+      <c r="R4" s="11"/>
       <c r="S4" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="T4" s="3"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="T4" s="3"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
@@ -2241,16 +2355,16 @@
       <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
       <c r="AK4" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL4" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="AL4" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="AM4" s="15"/>
-      <c r="AN4" s="15"/>
+      <c r="AM4" s="14"/>
+      <c r="AN4" s="14"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AQ4" s="3"/>
       <c r="AR4" s="3"/>
@@ -2271,33 +2385,33 @@
       <c r="BG4" s="3"/>
       <c r="BH4" s="3"/>
       <c r="BI4" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:61" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
@@ -2310,18 +2424,18 @@
         <v>42137</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="T5" s="6"/>
       <c r="U5" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="V5" s="6" t="s">
         <v>78</v>
       </c>
       <c r="W5" s="6"/>
       <c r="X5" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
@@ -2333,56 +2447,56 @@
       <c r="AF5" s="6"/>
       <c r="AG5" s="6"/>
       <c r="AH5" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AI5" s="6"/>
       <c r="AJ5" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="AK5" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="AK5" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="AL5" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="AM5" s="10">
+      <c r="AL5" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="AM5" s="9">
         <f>AM3+DAY(1)</f>
         <v>42948</v>
       </c>
       <c r="AN5" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="AO5" s="6"/>
       <c r="AP5" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AQ5" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="AR5" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="AQ5" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="AR5" s="17" t="s">
-        <v>148</v>
-      </c>
       <c r="AS5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AT5" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AU5" s="7"/>
       <c r="AV5" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW5" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="AW5" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX5" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AY5" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="AX5" s="11" t="s">
+      <c r="AZ5" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="AY5" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="AZ5" s="11" t="s">
-        <v>152</v>
       </c>
       <c r="BA5" s="6"/>
       <c r="BB5" s="6"/>
@@ -2392,36 +2506,36 @@
       <c r="BF5" s="6"/>
       <c r="BG5" s="6"/>
       <c r="BH5" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="BI5" s="18"/>
+        <v>101</v>
+      </c>
+      <c r="BI5" s="17"/>
     </row>
     <row r="6" spans="1:61" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H6" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="J6" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>158</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
@@ -2434,14 +2548,14 @@
         <v>42137</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="T6" s="6"/>
       <c r="U6" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
@@ -2455,38 +2569,38 @@
       <c r="AF6" s="6"/>
       <c r="AG6" s="6"/>
       <c r="AH6" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AI6" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AJ6" s="6"/>
       <c r="AK6" s="6"/>
       <c r="AL6" s="6"/>
-      <c r="AM6" s="10" t="s">
-        <v>113</v>
+      <c r="AM6" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="AN6" s="6"/>
       <c r="AO6" s="6"/>
       <c r="AP6" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AQ6" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AR6" s="6"/>
       <c r="AS6" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AT6" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AU6" s="5"/>
       <c r="AV6" s="5"/>
-      <c r="AW6" s="11"/>
-      <c r="AX6" s="11"/>
-      <c r="AY6" s="11"/>
-      <c r="AZ6" s="11"/>
+      <c r="AW6" s="10"/>
+      <c r="AX6" s="10"/>
+      <c r="AY6" s="10"/>
+      <c r="AZ6" s="10"/>
       <c r="BA6" s="6"/>
       <c r="BB6" s="6"/>
       <c r="BC6" s="6"/>
@@ -2495,12 +2609,12 @@
       <c r="BF6" s="6"/>
       <c r="BG6" s="6"/>
       <c r="BH6" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
@@ -2522,7 +2636,7 @@
         <v>42137</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="T7" s="6"/>
       <c r="U7" s="5"/>
@@ -2550,17 +2664,17 @@
       <c r="AQ7" s="6"/>
       <c r="AR7" s="6"/>
       <c r="AS7" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AT7" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AU7" s="5"/>
       <c r="AV7" s="5"/>
-      <c r="AW7" s="11"/>
-      <c r="AX7" s="11"/>
-      <c r="AY7" s="11"/>
-      <c r="AZ7" s="11"/>
+      <c r="AW7" s="10"/>
+      <c r="AX7" s="10"/>
+      <c r="AY7" s="10"/>
+      <c r="AZ7" s="10"/>
       <c r="BA7" s="6"/>
       <c r="BB7" s="6"/>
       <c r="BC7" s="6"/>
@@ -2569,12 +2683,12 @@
       <c r="BF7" s="6"/>
       <c r="BG7" s="6"/>
       <c r="BH7" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
@@ -2596,7 +2710,7 @@
         <v>42137</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="T8" s="6"/>
       <c r="U8" s="5"/>
@@ -2617,27 +2731,27 @@
       <c r="AJ8" s="6"/>
       <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="10">
+      <c r="AM8" s="9">
         <f>AM5+DAY(1)</f>
         <v>42949</v>
       </c>
       <c r="AN8" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AO8" s="6"/>
       <c r="AP8" s="6"/>
       <c r="AQ8" s="6"/>
       <c r="AR8" s="6"/>
       <c r="AS8" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AT8" s="5"/>
       <c r="AU8" s="5"/>
       <c r="AV8" s="5"/>
-      <c r="AW8" s="11"/>
-      <c r="AX8" s="11"/>
-      <c r="AY8" s="11"/>
-      <c r="AZ8" s="11"/>
+      <c r="AW8" s="10"/>
+      <c r="AX8" s="10"/>
+      <c r="AY8" s="10"/>
+      <c r="AZ8" s="10"/>
       <c r="BA8" s="6"/>
       <c r="BB8" s="6"/>
       <c r="BC8" s="6"/>
@@ -2649,7 +2763,7 @@
     </row>
     <row r="9" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
@@ -2667,11 +2781,11 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="12">
+      <c r="R9" s="11">
         <v>42137</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T9" s="3"/>
       <c r="U9" s="2"/>
@@ -2699,7 +2813,7 @@
       <c r="AQ9" s="3"/>
       <c r="AR9" s="3"/>
       <c r="AS9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
@@ -2719,172 +2833,174 @@
       <c r="BI9" s="3"/>
     </row>
     <row r="10" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="F10" s="19"/>
+      <c r="G10" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20" t="s">
+      <c r="H10" s="19"/>
+      <c r="I10" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20" t="s">
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="21">
+        <v>42581</v>
+      </c>
+      <c r="S10" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20" t="s">
+      <c r="T10" s="20"/>
+      <c r="U10" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="22">
-        <v>42581</v>
-      </c>
-      <c r="S10" s="21" t="s">
+      <c r="V10" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="T10" s="21"/>
-      <c r="U10" s="20" t="s">
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="20"/>
+      <c r="AI10" s="20"/>
+      <c r="AJ10" s="20"/>
+      <c r="AK10" s="20"/>
+      <c r="AL10" s="20"/>
+      <c r="AM10" s="20"/>
+      <c r="AN10" s="20"/>
+      <c r="AO10" s="20"/>
+      <c r="AP10" s="20"/>
+      <c r="AQ10" s="20"/>
+      <c r="AR10" s="20"/>
+      <c r="AS10" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="V10" s="21" t="s">
+      <c r="AT10" s="19"/>
+      <c r="AU10" s="21"/>
+      <c r="AV10" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
-      <c r="AC10" s="21"/>
-      <c r="AD10" s="21"/>
-      <c r="AE10" s="21"/>
-      <c r="AF10" s="21"/>
-      <c r="AG10" s="21"/>
-      <c r="AH10" s="21"/>
-      <c r="AI10" s="21"/>
-      <c r="AJ10" s="21"/>
-      <c r="AK10" s="21"/>
-      <c r="AL10" s="21"/>
-      <c r="AM10" s="21"/>
-      <c r="AN10" s="21"/>
-      <c r="AO10" s="21"/>
-      <c r="AP10" s="21"/>
-      <c r="AQ10" s="21"/>
-      <c r="AR10" s="21"/>
-      <c r="AS10" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AT10" s="20"/>
-      <c r="AU10" s="22"/>
-      <c r="AV10" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="AW10" s="23"/>
-      <c r="AX10" s="23"/>
-      <c r="AY10" s="23"/>
-      <c r="AZ10" s="23"/>
-      <c r="BA10" s="21"/>
-      <c r="BB10" s="21"/>
-      <c r="BC10" s="21"/>
-      <c r="BD10" s="21"/>
-      <c r="BE10" s="21"/>
-      <c r="BF10" s="21"/>
-      <c r="BG10" s="21"/>
-      <c r="BH10" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="BI10" s="24"/>
+      <c r="AW10" s="22"/>
+      <c r="AX10" s="22"/>
+      <c r="AY10" s="22"/>
+      <c r="AZ10" s="22"/>
+      <c r="BA10" s="20"/>
+      <c r="BB10" s="20"/>
+      <c r="BC10" s="20"/>
+      <c r="BD10" s="20"/>
+      <c r="BE10" s="20"/>
+      <c r="BF10" s="20"/>
+      <c r="BG10" s="20"/>
+      <c r="BH10" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="BI10" s="23"/>
     </row>
     <row r="11" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J11" s="5"/>
       <c r="R11" s="7">
         <v>42582</v>
       </c>
-      <c r="S11" s="28" t="s">
-        <v>194</v>
+      <c r="S11" s="27" t="s">
+        <v>192</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AM11" s="6"/>
       <c r="AN11" s="6"/>
       <c r="AP11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AS11" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AT11" s="5"/>
       <c r="AU11" s="7">
         <v>42581</v>
       </c>
       <c r="AV11" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW11" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="AX11" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="AY11" s="26"/>
-      <c r="AZ11" s="26"/>
+        <v>92</v>
+      </c>
+      <c r="AW11" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="AX11" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="AY11" s="25"/>
+      <c r="AZ11" s="25"/>
       <c r="BA11" s="6" t="s">
         <v>76</v>
       </c>
       <c r="BB11" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="BC11" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="BC11" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="BD11" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="BE11" s="25"/>
-      <c r="BH11" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="BI11" s="27" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+      <c r="BE11" s="24"/>
+      <c r="BH11" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="BI11" s="26" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AL4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="AR5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="AL2" r:id="rId3" xr:uid="{462BC0B8-EB92-2841-A55E-814BC5E3B2A0}"/>
+    <hyperlink ref="AL5" r:id="rId4" xr:uid="{4599B7FD-CDD1-B046-9E1D-1331ED609B8F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EASY-2662: URL validation in DCX_RELATION_LINK column (#147)
</commit_message>
<xml_diff>
--- a/src/test/resources/allfields/input/instructions.xlsx
+++ b/src/test/resources/allfields/input/instructions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/allfields/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E5257B-1031-6241-B9AF-53B8853D3906}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE54E10-8A5A-B64A-A6B9-FDAF058ED6E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,12 @@
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -325,9 +331,6 @@
     <t>dummy</t>
   </si>
   <si>
-    <t>foobar</t>
-  </si>
-  <si>
     <t>Valid</t>
   </si>
   <si>
@@ -499,9 +502,6 @@
     <t>context</t>
   </si>
   <si>
-    <t>barbapappa</t>
-  </si>
-  <si>
     <t>Date Accepted</t>
   </si>
   <si>
@@ -650,6 +650,12 @@
   </si>
   <si>
     <t>stephan</t>
+  </si>
+  <si>
+    <t>http://y</t>
+  </si>
+  <si>
+    <t>http://barbapappa</t>
   </si>
 </sst>
 </file>
@@ -780,7 +786,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -802,6 +807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1317,6 +1323,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AE77436-DCB5-8346-B8A0-90D14D5BE88E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12725400"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C42AA4FF-97AE-3B41-8224-EC46EDC6B7F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12725400"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1653,10 +1767,10 @@
   <dimension ref="A1:BI11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AQ1" sqref="AQ1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S11" sqref="S11"/>
+      <selection pane="bottomRight" activeCell="AL5" sqref="AL5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1705,7 +1819,7 @@
     <col min="43" max="43" width="14.33203125" customWidth="1"/>
     <col min="44" max="44" width="22.33203125" customWidth="1"/>
     <col min="45" max="45" width="34.33203125" customWidth="1"/>
-    <col min="46" max="46" width="34.33203125" style="26" customWidth="1"/>
+    <col min="46" max="46" width="34.33203125" style="25" customWidth="1"/>
     <col min="47" max="47" width="15.1640625" customWidth="1"/>
     <col min="48" max="48" width="14.6640625" customWidth="1"/>
     <col min="49" max="49" width="33" customWidth="1"/>
@@ -1860,7 +1974,7 @@
         <v>46</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="AU1" s="2" t="s">
         <v>47</v>
@@ -2000,75 +2114,75 @@
       <c r="AK2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AL2" s="9" t="s">
+      <c r="AL2" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="AM2" s="9">
+        <v>42946</v>
+      </c>
+      <c r="AN2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="AM2" s="10">
-        <v>42946</v>
-      </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AP2" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="AQ2" s="6" t="s">
+      <c r="AR2" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="AR2" s="6" t="s">
+      <c r="AS2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AS2" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="AT2" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AU2" s="7">
         <v>33815</v>
       </c>
       <c r="AV2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AW2" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="AY2" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="AZ2" s="6"/>
       <c r="BA2" s="6" t="s">
         <v>76</v>
       </c>
       <c r="BB2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="BC2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="BC2" s="6" t="s">
+      <c r="BD2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="BD2" s="6" t="s">
+      <c r="BE2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="BF2" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="BE2" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="BF2" s="6" t="s">
+      <c r="BG2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="BG2" s="6" t="s">
+      <c r="BH2" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="BH2" s="6" t="s">
+      <c r="BI2" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="BI2" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:61" x14ac:dyDescent="0.2">
@@ -2076,7 +2190,7 @@
         <v>62</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
@@ -2088,42 +2202,42 @@
       <c r="J3" s="5"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R3" s="7"/>
       <c r="S3" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="T3" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="V3" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="W3" s="6"/>
       <c r="X3" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y3" s="6"/>
       <c r="Z3" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA3" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>115</v>
       </c>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
@@ -2143,55 +2257,55 @@
         <v>6663</v>
       </c>
       <c r="AI3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ3" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="AJ3" s="6" t="s">
+      <c r="AK3" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AK3" s="6" t="s">
+      <c r="AL3" s="6"/>
+      <c r="AM3" s="9">
+        <v>42947</v>
+      </c>
+      <c r="AN3" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="AL3" s="6"/>
-      <c r="AM3" s="10">
-        <v>42947</v>
-      </c>
-      <c r="AN3" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="AO3" s="6"/>
       <c r="AP3" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="AQ3" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="AQ3" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="AR3" s="6"/>
       <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5"/>
       <c r="AV3" s="5"/>
-      <c r="AW3" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="AX3" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="AY3" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="AZ3" s="11"/>
+      <c r="AW3" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="AX3" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="AY3" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AZ3" s="10"/>
       <c r="BA3" s="6"/>
       <c r="BB3" s="6"/>
       <c r="BC3" s="6"/>
       <c r="BD3" s="6"/>
       <c r="BE3" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BF3" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="BG3" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="BG3" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="BH3" s="6"/>
     </row>
@@ -2215,17 +2329,17 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
-      <c r="R4" s="12"/>
+      <c r="R4" s="11"/>
       <c r="S4" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="T4" s="3"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="T4" s="3"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
@@ -2241,16 +2355,16 @@
       <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
       <c r="AK4" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL4" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="AL4" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="AM4" s="15"/>
-      <c r="AN4" s="15"/>
+      <c r="AM4" s="14"/>
+      <c r="AN4" s="14"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AQ4" s="3"/>
       <c r="AR4" s="3"/>
@@ -2271,33 +2385,33 @@
       <c r="BG4" s="3"/>
       <c r="BH4" s="3"/>
       <c r="BI4" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:61" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
@@ -2310,18 +2424,18 @@
         <v>42137</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="T5" s="6"/>
       <c r="U5" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="V5" s="6" t="s">
         <v>78</v>
       </c>
       <c r="W5" s="6"/>
       <c r="X5" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
@@ -2333,56 +2447,56 @@
       <c r="AF5" s="6"/>
       <c r="AG5" s="6"/>
       <c r="AH5" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AI5" s="6"/>
       <c r="AJ5" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="AK5" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="AK5" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="AL5" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="AM5" s="10">
+      <c r="AL5" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="AM5" s="9">
         <f>AM3+DAY(1)</f>
         <v>42948</v>
       </c>
       <c r="AN5" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="AO5" s="6"/>
       <c r="AP5" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AQ5" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="AR5" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="AQ5" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="AR5" s="17" t="s">
-        <v>148</v>
-      </c>
       <c r="AS5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AT5" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AU5" s="7"/>
       <c r="AV5" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW5" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="AW5" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX5" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AY5" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="AX5" s="11" t="s">
+      <c r="AZ5" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="AY5" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="AZ5" s="11" t="s">
-        <v>152</v>
       </c>
       <c r="BA5" s="6"/>
       <c r="BB5" s="6"/>
@@ -2392,36 +2506,36 @@
       <c r="BF5" s="6"/>
       <c r="BG5" s="6"/>
       <c r="BH5" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="BI5" s="18"/>
+        <v>101</v>
+      </c>
+      <c r="BI5" s="17"/>
     </row>
     <row r="6" spans="1:61" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H6" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="J6" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>158</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
@@ -2434,14 +2548,14 @@
         <v>42137</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="T6" s="6"/>
       <c r="U6" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
@@ -2455,38 +2569,38 @@
       <c r="AF6" s="6"/>
       <c r="AG6" s="6"/>
       <c r="AH6" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AI6" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AJ6" s="6"/>
       <c r="AK6" s="6"/>
       <c r="AL6" s="6"/>
-      <c r="AM6" s="10" t="s">
-        <v>113</v>
+      <c r="AM6" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="AN6" s="6"/>
       <c r="AO6" s="6"/>
       <c r="AP6" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AQ6" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AR6" s="6"/>
       <c r="AS6" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AT6" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AU6" s="5"/>
       <c r="AV6" s="5"/>
-      <c r="AW6" s="11"/>
-      <c r="AX6" s="11"/>
-      <c r="AY6" s="11"/>
-      <c r="AZ6" s="11"/>
+      <c r="AW6" s="10"/>
+      <c r="AX6" s="10"/>
+      <c r="AY6" s="10"/>
+      <c r="AZ6" s="10"/>
       <c r="BA6" s="6"/>
       <c r="BB6" s="6"/>
       <c r="BC6" s="6"/>
@@ -2495,12 +2609,12 @@
       <c r="BF6" s="6"/>
       <c r="BG6" s="6"/>
       <c r="BH6" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
@@ -2522,7 +2636,7 @@
         <v>42137</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="T7" s="6"/>
       <c r="U7" s="5"/>
@@ -2550,17 +2664,17 @@
       <c r="AQ7" s="6"/>
       <c r="AR7" s="6"/>
       <c r="AS7" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AT7" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AU7" s="5"/>
       <c r="AV7" s="5"/>
-      <c r="AW7" s="11"/>
-      <c r="AX7" s="11"/>
-      <c r="AY7" s="11"/>
-      <c r="AZ7" s="11"/>
+      <c r="AW7" s="10"/>
+      <c r="AX7" s="10"/>
+      <c r="AY7" s="10"/>
+      <c r="AZ7" s="10"/>
       <c r="BA7" s="6"/>
       <c r="BB7" s="6"/>
       <c r="BC7" s="6"/>
@@ -2569,12 +2683,12 @@
       <c r="BF7" s="6"/>
       <c r="BG7" s="6"/>
       <c r="BH7" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
@@ -2596,7 +2710,7 @@
         <v>42137</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="T8" s="6"/>
       <c r="U8" s="5"/>
@@ -2617,27 +2731,27 @@
       <c r="AJ8" s="6"/>
       <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="10">
+      <c r="AM8" s="9">
         <f>AM5+DAY(1)</f>
         <v>42949</v>
       </c>
       <c r="AN8" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AO8" s="6"/>
       <c r="AP8" s="6"/>
       <c r="AQ8" s="6"/>
       <c r="AR8" s="6"/>
       <c r="AS8" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AT8" s="5"/>
       <c r="AU8" s="5"/>
       <c r="AV8" s="5"/>
-      <c r="AW8" s="11"/>
-      <c r="AX8" s="11"/>
-      <c r="AY8" s="11"/>
-      <c r="AZ8" s="11"/>
+      <c r="AW8" s="10"/>
+      <c r="AX8" s="10"/>
+      <c r="AY8" s="10"/>
+      <c r="AZ8" s="10"/>
       <c r="BA8" s="6"/>
       <c r="BB8" s="6"/>
       <c r="BC8" s="6"/>
@@ -2649,7 +2763,7 @@
     </row>
     <row r="9" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
@@ -2667,11 +2781,11 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="12">
+      <c r="R9" s="11">
         <v>42137</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T9" s="3"/>
       <c r="U9" s="2"/>
@@ -2699,7 +2813,7 @@
       <c r="AQ9" s="3"/>
       <c r="AR9" s="3"/>
       <c r="AS9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
@@ -2719,172 +2833,174 @@
       <c r="BI9" s="3"/>
     </row>
     <row r="10" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="F10" s="19"/>
+      <c r="G10" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20" t="s">
+      <c r="H10" s="19"/>
+      <c r="I10" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20" t="s">
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="21">
+        <v>42581</v>
+      </c>
+      <c r="S10" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20" t="s">
+      <c r="T10" s="20"/>
+      <c r="U10" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="22">
-        <v>42581</v>
-      </c>
-      <c r="S10" s="21" t="s">
+      <c r="V10" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="T10" s="21"/>
-      <c r="U10" s="20" t="s">
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="20"/>
+      <c r="AI10" s="20"/>
+      <c r="AJ10" s="20"/>
+      <c r="AK10" s="20"/>
+      <c r="AL10" s="20"/>
+      <c r="AM10" s="20"/>
+      <c r="AN10" s="20"/>
+      <c r="AO10" s="20"/>
+      <c r="AP10" s="20"/>
+      <c r="AQ10" s="20"/>
+      <c r="AR10" s="20"/>
+      <c r="AS10" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="V10" s="21" t="s">
+      <c r="AT10" s="19"/>
+      <c r="AU10" s="21"/>
+      <c r="AV10" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
-      <c r="AC10" s="21"/>
-      <c r="AD10" s="21"/>
-      <c r="AE10" s="21"/>
-      <c r="AF10" s="21"/>
-      <c r="AG10" s="21"/>
-      <c r="AH10" s="21"/>
-      <c r="AI10" s="21"/>
-      <c r="AJ10" s="21"/>
-      <c r="AK10" s="21"/>
-      <c r="AL10" s="21"/>
-      <c r="AM10" s="21"/>
-      <c r="AN10" s="21"/>
-      <c r="AO10" s="21"/>
-      <c r="AP10" s="21"/>
-      <c r="AQ10" s="21"/>
-      <c r="AR10" s="21"/>
-      <c r="AS10" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AT10" s="20"/>
-      <c r="AU10" s="22"/>
-      <c r="AV10" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="AW10" s="23"/>
-      <c r="AX10" s="23"/>
-      <c r="AY10" s="23"/>
-      <c r="AZ10" s="23"/>
-      <c r="BA10" s="21"/>
-      <c r="BB10" s="21"/>
-      <c r="BC10" s="21"/>
-      <c r="BD10" s="21"/>
-      <c r="BE10" s="21"/>
-      <c r="BF10" s="21"/>
-      <c r="BG10" s="21"/>
-      <c r="BH10" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="BI10" s="24"/>
+      <c r="AW10" s="22"/>
+      <c r="AX10" s="22"/>
+      <c r="AY10" s="22"/>
+      <c r="AZ10" s="22"/>
+      <c r="BA10" s="20"/>
+      <c r="BB10" s="20"/>
+      <c r="BC10" s="20"/>
+      <c r="BD10" s="20"/>
+      <c r="BE10" s="20"/>
+      <c r="BF10" s="20"/>
+      <c r="BG10" s="20"/>
+      <c r="BH10" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="BI10" s="23"/>
     </row>
     <row r="11" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J11" s="5"/>
       <c r="R11" s="7">
         <v>42582</v>
       </c>
-      <c r="S11" s="28" t="s">
-        <v>194</v>
+      <c r="S11" s="27" t="s">
+        <v>192</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AM11" s="6"/>
       <c r="AN11" s="6"/>
       <c r="AP11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AS11" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AT11" s="5"/>
       <c r="AU11" s="7">
         <v>42581</v>
       </c>
       <c r="AV11" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW11" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="AX11" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="AY11" s="26"/>
-      <c r="AZ11" s="26"/>
+        <v>92</v>
+      </c>
+      <c r="AW11" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="AX11" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="AY11" s="25"/>
+      <c r="AZ11" s="25"/>
       <c r="BA11" s="6" t="s">
         <v>76</v>
       </c>
       <c r="BB11" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="BC11" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="BC11" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="BD11" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="BE11" s="25"/>
-      <c r="BH11" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="BI11" s="27" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+      <c r="BE11" s="24"/>
+      <c r="BH11" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="BI11" s="26" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AL4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="AR5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="AL2" r:id="rId3" xr:uid="{462BC0B8-EB92-2841-A55E-814BC5E3B2A0}"/>
+    <hyperlink ref="AL5" r:id="rId4" xr:uid="{4599B7FD-CDD1-B046-9E1D-1331ED609B8F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>